<commit_message>
added desmopressin action item
</commit_message>
<xml_diff>
--- a/Working QA Team Folders/Pre- Release QA/Action Items (Master).xlsx
+++ b/Working QA Team Folders/Pre- Release QA/Action Items (Master).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="17268" windowHeight="5376"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="17268" windowHeight="5316" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Action Items, Open" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="F121" authorId="0">
+    <comment ref="F122" authorId="0">
       <text>
         <r>
           <rPr>
@@ -34,7 +34,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F135" authorId="0">
+    <comment ref="F136" authorId="0">
       <text>
         <r>
           <rPr>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1691" uniqueCount="1007">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1696" uniqueCount="1011">
   <si>
     <t>TM</t>
   </si>
@@ -4341,6 +4341,18 @@
       </rPr>
       <t xml:space="preserve"> methylprednisolone (methylprednisolone sodium succinate) 125 mg powder for solution for injection with diluent solution per vial</t>
     </r>
+  </si>
+  <si>
+    <t>QA Release 20180704 Relationship file for QA.xlsx</t>
+  </si>
+  <si>
+    <t>00873993</t>
+  </si>
+  <si>
+    <t>desmopressin acetate 4 mcg per mL solution for injection</t>
+  </si>
+  <si>
+    <t>UoP: 13867, ampoule, 1, mL, Y, N</t>
   </si>
 </sst>
 </file>
@@ -4962,7 +4974,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="246">
+  <cellXfs count="247">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -5630,6 +5642,39 @@
     <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="53" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="40" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -5650,38 +5695,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="53" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="40" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5996,7 +6011,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6007,11 +6022,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J145"/>
+  <dimension ref="A1:J146"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H110" sqref="H110"/>
+    <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.8"/>
@@ -7335,32 +7350,30 @@
       <c r="H54" s="178"/>
       <c r="I54" s="179"/>
     </row>
-    <row r="55" spans="1:10" ht="27.6">
-      <c r="A55" s="173" t="s">
+    <row r="55" spans="1:10" ht="41.4">
+      <c r="A55" s="212" t="s">
         <v>372</v>
       </c>
-      <c r="B55" s="174" t="s">
-        <v>373</v>
-      </c>
-      <c r="C55" s="174"/>
-      <c r="D55" s="174" t="s">
-        <v>374</v>
+      <c r="B55" s="178" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C55" s="178"/>
+      <c r="D55" s="175" t="s">
+        <v>1008</v>
       </c>
       <c r="E55" s="182" t="s">
-        <v>375</v>
-      </c>
-      <c r="F55" s="211" t="s">
-        <v>377</v>
-      </c>
-      <c r="G55" s="178" t="s">
-        <v>378</v>
-      </c>
+        <v>1009</v>
+      </c>
+      <c r="F55" s="246" t="s">
+        <v>1010</v>
+      </c>
+      <c r="G55" s="199"/>
       <c r="H55" s="178"/>
       <c r="I55" s="179">
-        <v>43252</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" ht="179.4">
+        <v>43298</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="27.6">
       <c r="A56" s="173" t="s">
         <v>372</v>
       </c>
@@ -7369,49 +7382,47 @@
       </c>
       <c r="C56" s="174"/>
       <c r="D56" s="174" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="E56" s="182" t="s">
-        <v>380</v>
-      </c>
-      <c r="F56" s="213" t="s">
-        <v>381</v>
-      </c>
-      <c r="G56" s="178"/>
+        <v>375</v>
+      </c>
+      <c r="F56" s="211" t="s">
+        <v>377</v>
+      </c>
+      <c r="G56" s="178" t="s">
+        <v>378</v>
+      </c>
       <c r="H56" s="178"/>
       <c r="I56" s="179">
-        <v>43290</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="41.4">
+        <v>43252</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="179.4">
       <c r="A57" s="173" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="B57" s="174" t="s">
-        <v>383</v>
-      </c>
-      <c r="C57" s="174" t="s">
-        <v>22</v>
-      </c>
+        <v>373</v>
+      </c>
+      <c r="C57" s="174"/>
       <c r="D57" s="174" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="E57" s="182" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="F57" s="213" t="s">
-        <v>386</v>
-      </c>
-      <c r="G57" s="178" t="s">
-        <v>387</v>
-      </c>
+        <v>381</v>
+      </c>
+      <c r="G57" s="178"/>
       <c r="H57" s="178"/>
       <c r="I57" s="179">
-        <v>43277</v>
+        <v>43290</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="41.4">
-      <c r="A58" s="196" t="s">
+      <c r="A58" s="173" t="s">
         <v>382</v>
       </c>
       <c r="B58" s="174" t="s">
@@ -7421,16 +7432,20 @@
         <v>22</v>
       </c>
       <c r="D58" s="174" t="s">
-        <v>388</v>
-      </c>
-      <c r="E58" s="182"/>
-      <c r="F58" s="211" t="s">
-        <v>389</v>
-      </c>
-      <c r="G58" s="178"/>
+        <v>384</v>
+      </c>
+      <c r="E58" s="182" t="s">
+        <v>385</v>
+      </c>
+      <c r="F58" s="213" t="s">
+        <v>386</v>
+      </c>
+      <c r="G58" s="178" t="s">
+        <v>387</v>
+      </c>
       <c r="H58" s="178"/>
       <c r="I58" s="179">
-        <v>43278</v>
+        <v>43277</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="41.4">
@@ -7444,7 +7459,7 @@
         <v>22</v>
       </c>
       <c r="D59" s="174" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E59" s="182"/>
       <c r="F59" s="211" t="s">
@@ -7467,7 +7482,7 @@
         <v>22</v>
       </c>
       <c r="D60" s="174" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E60" s="182"/>
       <c r="F60" s="211" t="s">
@@ -7479,42 +7494,44 @@
         <v>43278</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="55.2">
+    <row r="61" spans="1:10" ht="41.4">
       <c r="A61" s="196" t="s">
         <v>382</v>
       </c>
       <c r="B61" s="174" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
       <c r="C61" s="174" t="s">
         <v>22</v>
       </c>
       <c r="D61" s="174" t="s">
-        <v>394</v>
-      </c>
-      <c r="E61" s="182" t="s">
-        <v>954</v>
-      </c>
-      <c r="F61" s="213" t="s">
-        <v>395</v>
+        <v>391</v>
+      </c>
+      <c r="E61" s="182"/>
+      <c r="F61" s="211" t="s">
+        <v>389</v>
       </c>
       <c r="G61" s="178"/>
       <c r="H61" s="178"/>
-      <c r="I61" s="179"/>
-    </row>
-    <row r="62" spans="1:10" ht="41.4">
-      <c r="A62" s="173" t="s">
-        <v>396</v>
+      <c r="I61" s="179">
+        <v>43278</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="55.2">
+      <c r="A62" s="196" t="s">
+        <v>382</v>
       </c>
       <c r="B62" s="174" t="s">
-        <v>397</v>
-      </c>
-      <c r="C62" s="174"/>
+        <v>393</v>
+      </c>
+      <c r="C62" s="174" t="s">
+        <v>22</v>
+      </c>
       <c r="D62" s="174" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="E62" s="182" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="F62" s="213" t="s">
         <v>395</v>
@@ -7523,55 +7540,49 @@
       <c r="H62" s="178"/>
       <c r="I62" s="179"/>
     </row>
-    <row r="63" spans="1:10" ht="27.6">
+    <row r="63" spans="1:10" ht="41.4">
       <c r="A63" s="173" t="s">
+        <v>396</v>
+      </c>
+      <c r="B63" s="174" t="s">
+        <v>397</v>
+      </c>
+      <c r="C63" s="174"/>
+      <c r="D63" s="174" t="s">
+        <v>398</v>
+      </c>
+      <c r="E63" s="182" t="s">
+        <v>955</v>
+      </c>
+      <c r="F63" s="213" t="s">
+        <v>395</v>
+      </c>
+      <c r="G63" s="178"/>
+      <c r="H63" s="178"/>
+      <c r="I63" s="179"/>
+    </row>
+    <row r="64" spans="1:10" ht="27.6">
+      <c r="A64" s="173" t="s">
         <v>76</v>
       </c>
-      <c r="B63" s="178" t="s">
+      <c r="B64" s="178" t="s">
         <v>401</v>
       </c>
-      <c r="C63" s="178" t="s">
+      <c r="C64" s="178" t="s">
         <v>22</v>
       </c>
-      <c r="D63" s="178" t="s">
+      <c r="D64" s="178" t="s">
         <v>402</v>
       </c>
-      <c r="E63" s="176" t="s">
+      <c r="E64" s="176" t="s">
         <v>403</v>
       </c>
-      <c r="F63" s="199" t="s">
+      <c r="F64" s="199" t="s">
         <v>404</v>
-      </c>
-      <c r="H63" s="178"/>
-      <c r="I63" s="179">
-        <v>43283</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" ht="41.4">
-      <c r="A64" s="196" t="s">
-        <v>76</v>
-      </c>
-      <c r="B64" s="174" t="s">
-        <v>77</v>
-      </c>
-      <c r="C64" s="174" t="s">
-        <v>22</v>
-      </c>
-      <c r="D64" s="214">
-        <v>2320789</v>
-      </c>
-      <c r="E64" s="182" t="s">
-        <v>406</v>
-      </c>
-      <c r="F64" s="213" t="s">
-        <v>408</v>
-      </c>
-      <c r="G64" s="178" t="s">
-        <v>409</v>
       </c>
       <c r="H64" s="178"/>
       <c r="I64" s="179">
-        <v>43284</v>
+        <v>43283</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="41.4">
@@ -7584,8 +7595,8 @@
       <c r="C65" s="174" t="s">
         <v>22</v>
       </c>
-      <c r="D65" s="214" t="s">
-        <v>410</v>
+      <c r="D65" s="214">
+        <v>2320789</v>
       </c>
       <c r="E65" s="182" t="s">
         <v>406</v>
@@ -7594,11 +7605,11 @@
         <v>408</v>
       </c>
       <c r="G65" s="178" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="H65" s="178"/>
       <c r="I65" s="179">
-        <v>43285</v>
+        <v>43284</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="41.4">
@@ -7612,20 +7623,20 @@
         <v>22</v>
       </c>
       <c r="D66" s="214" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E66" s="182" t="s">
-        <v>102</v>
+        <v>406</v>
       </c>
       <c r="F66" s="213" t="s">
         <v>408</v>
       </c>
       <c r="G66" s="178" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H66" s="178"/>
       <c r="I66" s="179">
-        <v>43287</v>
+        <v>43285</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="41.4">
@@ -7639,7 +7650,7 @@
         <v>22</v>
       </c>
       <c r="D67" s="214" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="E67" s="182" t="s">
         <v>102</v>
@@ -7647,12 +7658,12 @@
       <c r="F67" s="213" t="s">
         <v>408</v>
       </c>
-      <c r="G67" s="214" t="s">
-        <v>417</v>
+      <c r="G67" s="178" t="s">
+        <v>413</v>
       </c>
       <c r="H67" s="178"/>
       <c r="I67" s="179">
-        <v>43288</v>
+        <v>43287</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="41.4">
@@ -7666,19 +7677,21 @@
         <v>22</v>
       </c>
       <c r="D68" s="214" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="E68" s="182" t="s">
         <v>102</v>
       </c>
       <c r="F68" s="213" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
       <c r="G68" s="214" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="H68" s="178"/>
-      <c r="I68" s="179"/>
+      <c r="I68" s="179">
+        <v>43288</v>
+      </c>
     </row>
     <row r="69" spans="1:9" ht="41.4">
       <c r="A69" s="196" t="s">
@@ -7691,7 +7704,7 @@
         <v>22</v>
       </c>
       <c r="D69" s="214" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="E69" s="182" t="s">
         <v>102</v>
@@ -7700,7 +7713,7 @@
         <v>422</v>
       </c>
       <c r="G69" s="214" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="H69" s="178"/>
       <c r="I69" s="179"/>
@@ -7715,17 +7728,17 @@
       <c r="C70" s="174" t="s">
         <v>22</v>
       </c>
-      <c r="D70" s="200" t="s">
-        <v>432</v>
+      <c r="D70" s="214" t="s">
+        <v>424</v>
       </c>
       <c r="E70" s="182" t="s">
         <v>102</v>
       </c>
       <c r="F70" s="213" t="s">
-        <v>408</v>
+        <v>422</v>
       </c>
       <c r="G70" s="214" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="H70" s="178"/>
       <c r="I70" s="179"/>
@@ -7741,16 +7754,16 @@
         <v>22</v>
       </c>
       <c r="D71" s="200" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="E71" s="182" t="s">
         <v>102</v>
       </c>
       <c r="F71" s="213" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
       <c r="G71" s="214" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H71" s="178"/>
       <c r="I71" s="179"/>
@@ -7766,23 +7779,23 @@
         <v>22</v>
       </c>
       <c r="D72" s="200" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="E72" s="182" t="s">
         <v>102</v>
       </c>
       <c r="F72" s="213" t="s">
-        <v>408</v>
+        <v>422</v>
       </c>
       <c r="G72" s="214" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="H72" s="178"/>
       <c r="I72" s="179"/>
     </row>
-    <row r="73" spans="1:9" ht="262.2">
-      <c r="A73" s="173" t="s">
-        <v>443</v>
+    <row r="73" spans="1:9" ht="41.4">
+      <c r="A73" s="196" t="s">
+        <v>76</v>
       </c>
       <c r="B73" s="174" t="s">
         <v>77</v>
@@ -7790,24 +7803,24 @@
       <c r="C73" s="174" t="s">
         <v>22</v>
       </c>
-      <c r="D73" s="215">
-        <v>2368196</v>
+      <c r="D73" s="200" t="s">
+        <v>437</v>
       </c>
       <c r="E73" s="182" t="s">
-        <v>445</v>
+        <v>102</v>
       </c>
       <c r="F73" s="213" t="s">
-        <v>446</v>
+        <v>408</v>
       </c>
       <c r="G73" s="214" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="H73" s="178"/>
       <c r="I73" s="179"/>
     </row>
-    <row r="74" spans="1:9" ht="41.4">
-      <c r="A74" s="196" t="s">
-        <v>448</v>
+    <row r="74" spans="1:9" ht="262.2">
+      <c r="A74" s="173" t="s">
+        <v>443</v>
       </c>
       <c r="B74" s="174" t="s">
         <v>77</v>
@@ -7815,26 +7828,24 @@
       <c r="C74" s="174" t="s">
         <v>22</v>
       </c>
-      <c r="D74" s="216">
-        <v>2356457</v>
+      <c r="D74" s="215">
+        <v>2368196</v>
       </c>
       <c r="E74" s="182" t="s">
-        <v>102</v>
+        <v>445</v>
       </c>
       <c r="F74" s="213" t="s">
-        <v>408</v>
+        <v>446</v>
       </c>
       <c r="G74" s="214" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="H74" s="178"/>
-      <c r="I74" s="179">
-        <v>43289</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" ht="55.2">
-      <c r="A75" s="173" t="s">
-        <v>451</v>
+      <c r="I74" s="179"/>
+    </row>
+    <row r="75" spans="1:9" ht="41.4">
+      <c r="A75" s="196" t="s">
+        <v>448</v>
       </c>
       <c r="B75" s="174" t="s">
         <v>77</v>
@@ -7843,7 +7854,7 @@
         <v>22</v>
       </c>
       <c r="D75" s="216">
-        <v>535230</v>
+        <v>2356457</v>
       </c>
       <c r="E75" s="182" t="s">
         <v>102</v>
@@ -7852,192 +7863,192 @@
         <v>408</v>
       </c>
       <c r="G75" s="214" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="H75" s="178"/>
       <c r="I75" s="179">
-        <v>43290</v>
+        <v>43289</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="55.2">
-      <c r="A76" s="217" t="s">
-        <v>453</v>
+      <c r="A76" s="173" t="s">
+        <v>451</v>
       </c>
       <c r="B76" s="174" t="s">
-        <v>454</v>
-      </c>
-      <c r="C76" s="174"/>
-      <c r="D76" s="214" t="s">
-        <v>365</v>
+        <v>77</v>
+      </c>
+      <c r="C76" s="174" t="s">
+        <v>22</v>
+      </c>
+      <c r="D76" s="216">
+        <v>535230</v>
       </c>
       <c r="E76" s="182" t="s">
         <v>102</v>
       </c>
       <c r="F76" s="213" t="s">
-        <v>455</v>
-      </c>
-      <c r="G76" s="214"/>
+        <v>408</v>
+      </c>
+      <c r="G76" s="214" t="s">
+        <v>452</v>
+      </c>
       <c r="H76" s="178"/>
       <c r="I76" s="179">
-        <v>43288</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" ht="193.2">
-      <c r="A77" s="173" t="s">
-        <v>456</v>
+        <v>43290</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="55.2">
+      <c r="A77" s="217" t="s">
+        <v>453</v>
       </c>
       <c r="B77" s="174" t="s">
-        <v>77</v>
-      </c>
-      <c r="C77" s="174" t="s">
-        <v>22</v>
-      </c>
-      <c r="D77" s="216">
-        <v>2410583</v>
+        <v>454</v>
+      </c>
+      <c r="C77" s="174"/>
+      <c r="D77" s="214" t="s">
+        <v>365</v>
       </c>
       <c r="E77" s="182" t="s">
-        <v>457</v>
+        <v>102</v>
       </c>
       <c r="F77" s="213" t="s">
         <v>455</v>
       </c>
-      <c r="G77" s="214" t="s">
-        <v>458</v>
-      </c>
+      <c r="G77" s="214"/>
       <c r="H77" s="178"/>
       <c r="I77" s="179">
-        <v>43291</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" ht="55.2">
+        <v>43288</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="193.2">
       <c r="A78" s="173" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="B78" s="174" t="s">
-        <v>461</v>
+        <v>77</v>
       </c>
       <c r="C78" s="174" t="s">
-        <v>462</v>
-      </c>
-      <c r="D78" s="178" t="s">
-        <v>208</v>
-      </c>
-      <c r="E78" s="218"/>
+        <v>22</v>
+      </c>
+      <c r="D78" s="216">
+        <v>2410583</v>
+      </c>
+      <c r="E78" s="182" t="s">
+        <v>457</v>
+      </c>
       <c r="F78" s="213" t="s">
-        <v>463</v>
-      </c>
-      <c r="G78" s="178" t="s">
-        <v>464</v>
+        <v>455</v>
+      </c>
+      <c r="G78" s="214" t="s">
+        <v>458</v>
       </c>
       <c r="H78" s="178"/>
       <c r="I78" s="179">
-        <v>43196</v>
+        <v>43291</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="55.2">
-      <c r="A79" s="196" t="s">
+      <c r="A79" s="173" t="s">
         <v>460</v>
       </c>
-      <c r="B79" s="174"/>
-      <c r="C79" s="174"/>
-      <c r="D79" s="174" t="s">
-        <v>465</v>
-      </c>
-      <c r="E79" s="182" t="s">
-        <v>466</v>
-      </c>
-      <c r="F79" s="211" t="s">
-        <v>467</v>
+      <c r="B79" s="174" t="s">
+        <v>461</v>
+      </c>
+      <c r="C79" s="174" t="s">
+        <v>462</v>
+      </c>
+      <c r="D79" s="178" t="s">
+        <v>208</v>
+      </c>
+      <c r="E79" s="218"/>
+      <c r="F79" s="213" t="s">
+        <v>463</v>
       </c>
       <c r="G79" s="178" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="H79" s="178"/>
       <c r="I79" s="179">
         <v>43196</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="151.80000000000001">
-      <c r="A80" s="173" t="s">
-        <v>469</v>
-      </c>
-      <c r="B80" s="174" t="s">
-        <v>461</v>
-      </c>
-      <c r="C80" s="174" t="s">
-        <v>470</v>
-      </c>
-      <c r="D80" s="178" t="s">
-        <v>13</v>
-      </c>
-      <c r="E80" s="218"/>
+    <row r="80" spans="1:9" ht="55.2">
+      <c r="A80" s="196" t="s">
+        <v>460</v>
+      </c>
+      <c r="B80" s="174"/>
+      <c r="C80" s="174"/>
+      <c r="D80" s="174" t="s">
+        <v>465</v>
+      </c>
+      <c r="E80" s="182" t="s">
+        <v>466</v>
+      </c>
       <c r="F80" s="211" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="G80" s="178" t="s">
-        <v>473</v>
-      </c>
-      <c r="H80" s="178" t="s">
-        <v>473</v>
-      </c>
+        <v>468</v>
+      </c>
+      <c r="H80" s="178"/>
       <c r="I80" s="179">
         <v>43196</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="124.2">
+    <row r="81" spans="1:10" ht="151.80000000000001">
       <c r="A81" s="173" t="s">
+        <v>469</v>
+      </c>
+      <c r="B81" s="174" t="s">
+        <v>461</v>
+      </c>
+      <c r="C81" s="174" t="s">
+        <v>470</v>
+      </c>
+      <c r="D81" s="178" t="s">
+        <v>13</v>
+      </c>
+      <c r="E81" s="218"/>
+      <c r="F81" s="211" t="s">
+        <v>472</v>
+      </c>
+      <c r="G81" s="178" t="s">
+        <v>473</v>
+      </c>
+      <c r="H81" s="178" t="s">
+        <v>473</v>
+      </c>
+      <c r="I81" s="179">
+        <v>43196</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="124.2">
+      <c r="A82" s="173" t="s">
         <v>474</v>
       </c>
-      <c r="B81" s="174" t="s">
+      <c r="B82" s="174" t="s">
         <v>475</v>
       </c>
-      <c r="C81" s="174"/>
-      <c r="D81" s="175" t="s">
+      <c r="C82" s="174"/>
+      <c r="D82" s="175" t="s">
         <v>476</v>
       </c>
-      <c r="E81" s="182" t="s">
+      <c r="E82" s="182" t="s">
         <v>477</v>
       </c>
-      <c r="F81" s="213" t="s">
+      <c r="F82" s="213" t="s">
         <v>478</v>
       </c>
-      <c r="G81" s="178" t="s">
+      <c r="G82" s="178" t="s">
         <v>479</v>
-      </c>
-      <c r="H81" s="178"/>
-      <c r="I81" s="179">
-        <v>43264</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="409.6">
-      <c r="A82" s="173" t="s">
-        <v>481</v>
-      </c>
-      <c r="B82" s="178" t="s">
-        <v>45</v>
-      </c>
-      <c r="C82" s="194">
-        <v>8001266</v>
-      </c>
-      <c r="D82" s="200" t="s">
-        <v>488</v>
-      </c>
-      <c r="E82" s="192" t="s">
-        <v>489</v>
-      </c>
-      <c r="F82" s="199" t="s">
-        <v>490</v>
-      </c>
-      <c r="G82" s="178" t="s">
-        <v>491</v>
       </c>
       <c r="H82" s="178"/>
       <c r="I82" s="179">
-        <v>43240</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" ht="41.4">
-      <c r="A83" s="196" t="s">
+        <v>43264</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="409.6">
+      <c r="A83" s="173" t="s">
         <v>481</v>
       </c>
       <c r="B83" s="178" t="s">
@@ -8047,23 +8058,23 @@
         <v>8001266</v>
       </c>
       <c r="D83" s="200" t="s">
-        <v>492</v>
-      </c>
-      <c r="E83" s="182" t="s">
+        <v>488</v>
+      </c>
+      <c r="E83" s="192" t="s">
         <v>489</v>
       </c>
       <c r="F83" s="199" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="G83" s="178" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="H83" s="178"/>
       <c r="I83" s="179">
         <v>43240</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="69">
+    <row r="84" spans="1:10" ht="41.4">
       <c r="A84" s="196" t="s">
         <v>481</v>
       </c>
@@ -8074,23 +8085,23 @@
         <v>8001266</v>
       </c>
       <c r="D84" s="200" t="s">
-        <v>498</v>
-      </c>
-      <c r="E84" s="219" t="s">
-        <v>499</v>
+        <v>492</v>
+      </c>
+      <c r="E84" s="182" t="s">
+        <v>489</v>
       </c>
       <c r="F84" s="199" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="G84" s="178" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="H84" s="178"/>
       <c r="I84" s="179">
         <v>43240</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="55.2">
+    <row r="85" spans="1:10" ht="69">
       <c r="A85" s="196" t="s">
         <v>481</v>
       </c>
@@ -8101,23 +8112,23 @@
         <v>8001266</v>
       </c>
       <c r="D85" s="200" t="s">
-        <v>502</v>
-      </c>
-      <c r="E85" s="182" t="s">
-        <v>489</v>
+        <v>498</v>
+      </c>
+      <c r="E85" s="219" t="s">
+        <v>499</v>
       </c>
       <c r="F85" s="199" t="s">
-        <v>503</v>
-      </c>
-      <c r="G85" s="180" t="s">
-        <v>491</v>
-      </c>
-      <c r="H85" s="174"/>
+        <v>500</v>
+      </c>
+      <c r="G85" s="178" t="s">
+        <v>501</v>
+      </c>
+      <c r="H85" s="178"/>
       <c r="I85" s="179">
         <v>43240</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="138">
+    <row r="86" spans="1:10" ht="55.2">
       <c r="A86" s="196" t="s">
         <v>481</v>
       </c>
@@ -8128,23 +8139,23 @@
         <v>8001266</v>
       </c>
       <c r="D86" s="200" t="s">
-        <v>504</v>
-      </c>
-      <c r="E86" s="176" t="s">
+        <v>502</v>
+      </c>
+      <c r="E86" s="182" t="s">
         <v>489</v>
       </c>
       <c r="F86" s="199" t="s">
-        <v>505</v>
-      </c>
-      <c r="G86" s="199" t="s">
-        <v>507</v>
-      </c>
-      <c r="H86" s="194"/>
+        <v>503</v>
+      </c>
+      <c r="G86" s="180" t="s">
+        <v>491</v>
+      </c>
+      <c r="H86" s="174"/>
       <c r="I86" s="179">
         <v>43240</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="69">
+    <row r="87" spans="1:10" ht="138">
       <c r="A87" s="196" t="s">
         <v>481</v>
       </c>
@@ -8155,18 +8166,18 @@
         <v>8001266</v>
       </c>
       <c r="D87" s="200" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="E87" s="176" t="s">
         <v>489</v>
       </c>
       <c r="F87" s="199" t="s">
-        <v>509</v>
-      </c>
-      <c r="G87" s="178" t="s">
-        <v>510</v>
-      </c>
-      <c r="H87" s="178"/>
+        <v>505</v>
+      </c>
+      <c r="G87" s="199" t="s">
+        <v>507</v>
+      </c>
+      <c r="H87" s="194"/>
       <c r="I87" s="179">
         <v>43240</v>
       </c>
@@ -8182,16 +8193,16 @@
         <v>8001266</v>
       </c>
       <c r="D88" s="200" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="E88" s="176" t="s">
-        <v>512</v>
+        <v>489</v>
       </c>
       <c r="F88" s="199" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="G88" s="178" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="H88" s="178"/>
       <c r="I88" s="179">
@@ -8199,55 +8210,59 @@
       </c>
     </row>
     <row r="89" spans="1:10" ht="69">
-      <c r="A89" s="173" t="s">
-        <v>515</v>
+      <c r="A89" s="196" t="s">
+        <v>481</v>
       </c>
       <c r="B89" s="178" t="s">
-        <v>151</v>
-      </c>
-      <c r="C89" s="174" t="s">
-        <v>516</v>
-      </c>
-      <c r="D89" s="174" t="s">
-        <v>517</v>
-      </c>
-      <c r="E89" s="182" t="s">
-        <v>956</v>
-      </c>
-      <c r="F89" s="211" t="s">
-        <v>519</v>
-      </c>
-      <c r="G89" s="178"/>
+        <v>45</v>
+      </c>
+      <c r="C89" s="194">
+        <v>8001266</v>
+      </c>
+      <c r="D89" s="200" t="s">
+        <v>511</v>
+      </c>
+      <c r="E89" s="176" t="s">
+        <v>512</v>
+      </c>
+      <c r="F89" s="199" t="s">
+        <v>513</v>
+      </c>
+      <c r="G89" s="178" t="s">
+        <v>514</v>
+      </c>
       <c r="H89" s="178"/>
       <c r="I89" s="179">
+        <v>43240</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="69">
+      <c r="A90" s="173" t="s">
+        <v>515</v>
+      </c>
+      <c r="B90" s="178" t="s">
+        <v>151</v>
+      </c>
+      <c r="C90" s="174" t="s">
+        <v>516</v>
+      </c>
+      <c r="D90" s="174" t="s">
+        <v>517</v>
+      </c>
+      <c r="E90" s="182" t="s">
+        <v>956</v>
+      </c>
+      <c r="F90" s="211" t="s">
+        <v>519</v>
+      </c>
+      <c r="G90" s="178"/>
+      <c r="H90" s="178"/>
+      <c r="I90" s="179">
         <v>43196</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="96.6">
-      <c r="A90" s="173" t="s">
-        <v>520</v>
-      </c>
-      <c r="B90" s="178" t="s">
-        <v>521</v>
-      </c>
-      <c r="C90" s="174"/>
-      <c r="D90" s="174" t="s">
-        <v>522</v>
-      </c>
-      <c r="E90" s="182" t="s">
-        <v>523</v>
-      </c>
-      <c r="F90" s="213" t="s">
-        <v>967</v>
-      </c>
-      <c r="G90" s="178" t="s">
-        <v>525</v>
-      </c>
-      <c r="H90" s="178"/>
-      <c r="I90" s="179"/>
-    </row>
-    <row r="91" spans="1:10" ht="138">
-      <c r="A91" s="196" t="s">
+    <row r="91" spans="1:10" ht="96.6">
+      <c r="A91" s="173" t="s">
         <v>520</v>
       </c>
       <c r="B91" s="178" t="s">
@@ -8255,113 +8270,110 @@
       </c>
       <c r="C91" s="174"/>
       <c r="D91" s="174" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="E91" s="182" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="F91" s="213" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="G91" s="178" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="H91" s="178"/>
       <c r="I91" s="179"/>
     </row>
-    <row r="92" spans="1:10" ht="234.6">
+    <row r="92" spans="1:10" ht="138">
       <c r="A92" s="196" t="s">
         <v>520</v>
       </c>
-      <c r="B92" s="178"/>
+      <c r="B92" s="178" t="s">
+        <v>521</v>
+      </c>
       <c r="C92" s="174"/>
       <c r="D92" s="174" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="E92" s="182" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="F92" s="213" t="s">
-        <v>969</v>
-      </c>
-      <c r="G92" s="194" t="s">
-        <v>533</v>
+        <v>968</v>
+      </c>
+      <c r="G92" s="178" t="s">
+        <v>529</v>
       </c>
       <c r="H92" s="178"/>
       <c r="I92" s="179"/>
     </row>
-    <row r="93" spans="1:10" ht="82.8">
-      <c r="A93" s="173" t="s">
+    <row r="93" spans="1:10" ht="234.6">
+      <c r="A93" s="196" t="s">
+        <v>520</v>
+      </c>
+      <c r="B93" s="178"/>
+      <c r="C93" s="174"/>
+      <c r="D93" s="174" t="s">
+        <v>530</v>
+      </c>
+      <c r="E93" s="182" t="s">
+        <v>531</v>
+      </c>
+      <c r="F93" s="213" t="s">
+        <v>969</v>
+      </c>
+      <c r="G93" s="194" t="s">
+        <v>533</v>
+      </c>
+      <c r="H93" s="178"/>
+      <c r="I93" s="179"/>
+    </row>
+    <row r="94" spans="1:10" ht="82.8">
+      <c r="A94" s="173" t="s">
         <v>534</v>
       </c>
-      <c r="B93" s="178" t="s">
+      <c r="B94" s="178" t="s">
         <v>151</v>
       </c>
-      <c r="C93" s="174" t="s">
+      <c r="C94" s="174" t="s">
         <v>535</v>
       </c>
-      <c r="D93" s="174" t="s">
+      <c r="D94" s="174" t="s">
         <v>536</v>
       </c>
-      <c r="E93" s="182" t="s">
+      <c r="E94" s="182" t="s">
         <v>957</v>
       </c>
-      <c r="F93" s="199" t="s">
+      <c r="F94" s="199" t="s">
         <v>538</v>
       </c>
-      <c r="G93" s="174" t="s">
+      <c r="G94" s="174" t="s">
         <v>539</v>
-      </c>
-      <c r="H93" s="178"/>
-      <c r="I93" s="179">
-        <v>43196</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" ht="55.2">
-      <c r="A94" s="181" t="s">
-        <v>540</v>
-      </c>
-      <c r="B94" s="178" t="s">
-        <v>547</v>
-      </c>
-      <c r="C94" s="178"/>
-      <c r="D94" s="175" t="s">
-        <v>553</v>
-      </c>
-      <c r="E94" s="182" t="s">
-        <v>554</v>
-      </c>
-      <c r="F94" s="201" t="s">
-        <v>555</v>
-      </c>
-      <c r="G94" s="178" t="s">
-        <v>559</v>
       </c>
       <c r="H94" s="178"/>
       <c r="I94" s="179">
-        <v>76138</v>
-      </c>
-      <c r="J94" s="178"/>
-    </row>
-    <row r="95" spans="1:10" ht="96.6">
-      <c r="A95" s="173" t="s">
-        <v>565</v>
+        <v>43196</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" ht="55.2">
+      <c r="A95" s="181" t="s">
+        <v>540</v>
       </c>
       <c r="B95" s="178" t="s">
         <v>547</v>
       </c>
       <c r="C95" s="178"/>
       <c r="D95" s="175" t="s">
-        <v>570</v>
+        <v>553</v>
       </c>
       <c r="E95" s="182" t="s">
-        <v>958</v>
-      </c>
-      <c r="F95" s="199" t="s">
-        <v>579</v>
+        <v>554</v>
+      </c>
+      <c r="F95" s="201" t="s">
+        <v>555</v>
       </c>
       <c r="G95" s="178" t="s">
-        <v>583</v>
+        <v>559</v>
       </c>
       <c r="H95" s="178"/>
       <c r="I95" s="179">
@@ -8369,137 +8381,134 @@
       </c>
       <c r="J95" s="178"/>
     </row>
-    <row r="96" spans="1:10" ht="41.4">
+    <row r="96" spans="1:10" ht="96.6">
       <c r="A96" s="173" t="s">
+        <v>565</v>
+      </c>
+      <c r="B96" s="178" t="s">
+        <v>547</v>
+      </c>
+      <c r="C96" s="178"/>
+      <c r="D96" s="175" t="s">
+        <v>570</v>
+      </c>
+      <c r="E96" s="182" t="s">
+        <v>958</v>
+      </c>
+      <c r="F96" s="199" t="s">
+        <v>579</v>
+      </c>
+      <c r="G96" s="178" t="s">
+        <v>583</v>
+      </c>
+      <c r="H96" s="178"/>
+      <c r="I96" s="179">
+        <v>76138</v>
+      </c>
+      <c r="J96" s="178"/>
+    </row>
+    <row r="97" spans="1:10" ht="41.4">
+      <c r="A97" s="173" t="s">
         <v>588</v>
       </c>
-      <c r="B96" s="178" t="s">
+      <c r="B97" s="178" t="s">
         <v>592</v>
       </c>
-      <c r="C96" s="178"/>
-      <c r="D96" s="174" t="s">
+      <c r="C97" s="178"/>
+      <c r="D97" s="174" t="s">
         <v>593</v>
       </c>
-      <c r="E96" s="182" t="s">
+      <c r="E97" s="182" t="s">
         <v>594</v>
       </c>
-      <c r="F96" s="201" t="s">
+      <c r="F97" s="201" t="s">
         <v>595</v>
       </c>
-      <c r="G96" s="178" t="s">
+      <c r="G97" s="178" t="s">
         <v>598</v>
       </c>
-      <c r="H96" s="178"/>
-      <c r="I96" s="179"/>
-      <c r="J96" s="178"/>
-    </row>
-    <row r="97" spans="1:9" ht="55.2">
-      <c r="A97" s="173" t="s">
+      <c r="H97" s="178"/>
+      <c r="I97" s="179"/>
+      <c r="J97" s="178"/>
+    </row>
+    <row r="98" spans="1:10" ht="55.2">
+      <c r="A98" s="173" t="s">
         <v>599</v>
       </c>
-      <c r="B97" s="178" t="s">
+      <c r="B98" s="178" t="s">
         <v>45</v>
       </c>
-      <c r="C97" s="178" t="s">
+      <c r="C98" s="178" t="s">
         <v>22</v>
       </c>
-      <c r="D97" s="197" t="s">
+      <c r="D98" s="197" t="s">
         <v>600</v>
       </c>
-      <c r="E97" s="176"/>
-      <c r="F97" s="220" t="s">
+      <c r="E98" s="176"/>
+      <c r="F98" s="220" t="s">
         <v>970</v>
       </c>
-      <c r="G97" s="178"/>
-      <c r="H97" s="178" t="s">
+      <c r="G98" s="178"/>
+      <c r="H98" s="178" t="s">
         <v>606</v>
       </c>
-      <c r="I97" s="179">
+      <c r="I98" s="179">
         <v>43240</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="55.2">
-      <c r="A98" s="173" t="s">
-        <v>607</v>
-      </c>
-      <c r="B98" s="178" t="s">
-        <v>222</v>
-      </c>
-      <c r="C98" s="178"/>
-      <c r="D98" s="175" t="s">
-        <v>608</v>
-      </c>
-      <c r="E98" s="176" t="s">
-        <v>609</v>
-      </c>
-      <c r="F98" s="221" t="s">
-        <v>610</v>
-      </c>
-      <c r="G98" s="178"/>
-      <c r="H98" s="178"/>
-      <c r="I98" s="179"/>
-    </row>
-    <row r="99" spans="1:9" ht="27.6">
-      <c r="A99" s="196" t="s">
+    <row r="99" spans="1:10" ht="55.2">
+      <c r="A99" s="173" t="s">
         <v>607</v>
       </c>
       <c r="B99" s="178" t="s">
         <v>222</v>
       </c>
       <c r="C99" s="178"/>
-      <c r="D99" s="175"/>
-      <c r="E99" s="176"/>
-      <c r="F99" s="220"/>
+      <c r="D99" s="175" t="s">
+        <v>608</v>
+      </c>
+      <c r="E99" s="176" t="s">
+        <v>609</v>
+      </c>
+      <c r="F99" s="221" t="s">
+        <v>610</v>
+      </c>
       <c r="G99" s="178"/>
       <c r="H99" s="178"/>
       <c r="I99" s="179"/>
     </row>
-    <row r="100" spans="1:9">
-      <c r="A100" s="173" t="s">
+    <row r="100" spans="1:10" ht="27.6">
+      <c r="A100" s="196" t="s">
+        <v>607</v>
+      </c>
+      <c r="B100" s="178" t="s">
+        <v>222</v>
+      </c>
+      <c r="C100" s="178"/>
+      <c r="D100" s="175"/>
+      <c r="E100" s="176"/>
+      <c r="F100" s="220"/>
+      <c r="G100" s="178"/>
+      <c r="H100" s="178"/>
+      <c r="I100" s="179"/>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="A101" s="173" t="s">
         <v>615</v>
       </c>
-      <c r="B100" s="178" t="s">
+      <c r="B101" s="178" t="s">
         <v>616</v>
       </c>
-      <c r="C100" s="178">
+      <c r="C101" s="178">
         <v>8001119</v>
       </c>
-      <c r="D100" s="194"/>
-      <c r="E100" s="176"/>
-      <c r="F100" s="199" t="s">
+      <c r="D101" s="194"/>
+      <c r="E101" s="176"/>
+      <c r="F101" s="199" t="s">
         <v>619</v>
       </c>
-      <c r="G100" s="178" t="s">
+      <c r="G101" s="178" t="s">
         <v>620</v>
-      </c>
-      <c r="H100" s="178" t="s">
-        <v>621</v>
-      </c>
-      <c r="I100" s="179">
-        <v>43196</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" ht="82.8">
-      <c r="A101" s="173" t="s">
-        <v>622</v>
-      </c>
-      <c r="B101" s="174" t="s">
-        <v>484</v>
-      </c>
-      <c r="C101" s="178">
-        <v>8001130</v>
-      </c>
-      <c r="D101" s="174" t="s">
-        <v>624</v>
-      </c>
-      <c r="E101" s="182" t="s">
-        <v>625</v>
-      </c>
-      <c r="F101" s="199" t="s">
-        <v>626</v>
-      </c>
-      <c r="G101" s="178" t="s">
-        <v>627</v>
       </c>
       <c r="H101" s="178" t="s">
         <v>621</v>
@@ -8508,313 +8517,319 @@
         <v>43196</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="27.6">
+    <row r="102" spans="1:10" ht="82.8">
       <c r="A102" s="173" t="s">
+        <v>622</v>
+      </c>
+      <c r="B102" s="174" t="s">
+        <v>484</v>
+      </c>
+      <c r="C102" s="178">
+        <v>8001130</v>
+      </c>
+      <c r="D102" s="174" t="s">
+        <v>624</v>
+      </c>
+      <c r="E102" s="182" t="s">
+        <v>625</v>
+      </c>
+      <c r="F102" s="199" t="s">
+        <v>626</v>
+      </c>
+      <c r="G102" s="178" t="s">
+        <v>627</v>
+      </c>
+      <c r="H102" s="178" t="s">
+        <v>621</v>
+      </c>
+      <c r="I102" s="179">
+        <v>43196</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" ht="27.6">
+      <c r="A103" s="173" t="s">
         <v>628</v>
       </c>
-      <c r="B102" s="174" t="s">
+      <c r="B103" s="174" t="s">
         <v>629</v>
       </c>
-      <c r="C102" s="174" t="s">
+      <c r="C103" s="174" t="s">
         <v>630</v>
       </c>
-      <c r="D102" s="174" t="s">
+      <c r="D103" s="174" t="s">
         <v>631</v>
       </c>
-      <c r="E102" s="182" t="s">
+      <c r="E103" s="182" t="s">
         <v>632</v>
       </c>
-      <c r="F102" s="201" t="s">
+      <c r="F103" s="201" t="s">
         <v>633</v>
       </c>
-      <c r="G102" s="178" t="s">
+      <c r="G103" s="178" t="s">
         <v>634</v>
       </c>
-      <c r="H102" s="178"/>
-      <c r="I102" s="179">
+      <c r="H103" s="178"/>
+      <c r="I103" s="179">
         <v>43266</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="41.4">
-      <c r="A103" s="173" t="s">
+    <row r="104" spans="1:10" ht="41.4">
+      <c r="A104" s="173" t="s">
         <v>635</v>
       </c>
-      <c r="B103" s="174" t="s">
+      <c r="B104" s="174" t="s">
         <v>637</v>
       </c>
-      <c r="C103" s="178"/>
-      <c r="D103" s="175" t="s">
+      <c r="C104" s="178"/>
+      <c r="D104" s="175" t="s">
         <v>638</v>
       </c>
-      <c r="E103" s="182" t="s">
+      <c r="E104" s="182" t="s">
         <v>102</v>
       </c>
-      <c r="F103" s="201" t="s">
+      <c r="F104" s="201" t="s">
         <v>640</v>
       </c>
-      <c r="G103" s="178" t="s">
+      <c r="G104" s="178" t="s">
         <v>641</v>
       </c>
-      <c r="H103" s="178"/>
-      <c r="I103" s="179"/>
-    </row>
-    <row r="104" spans="1:9" ht="69">
-      <c r="A104" s="173" t="s">
+      <c r="H104" s="178"/>
+      <c r="I104" s="179"/>
+    </row>
+    <row r="105" spans="1:10" ht="69">
+      <c r="A105" s="173" t="s">
         <v>644</v>
       </c>
-      <c r="B104" s="178" t="s">
+      <c r="B105" s="178" t="s">
         <v>45</v>
       </c>
-      <c r="C104" s="178" t="s">
+      <c r="C105" s="178" t="s">
         <v>22</v>
       </c>
-      <c r="D104" s="243" t="s">
+      <c r="D105" s="235" t="s">
         <v>989</v>
       </c>
-      <c r="E104" s="245" t="s">
+      <c r="E105" s="237" t="s">
         <v>995</v>
       </c>
-      <c r="F104" s="199" t="s">
+      <c r="F105" s="199" t="s">
         <v>996</v>
       </c>
-      <c r="G104" s="178" t="s">
+      <c r="G105" s="178" t="s">
         <v>1005</v>
-      </c>
-      <c r="H104" s="178"/>
-      <c r="I104" s="179">
-        <v>43240</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" ht="69">
-      <c r="A105" s="196" t="s">
-        <v>644</v>
-      </c>
-      <c r="B105" s="178"/>
-      <c r="C105" s="178"/>
-      <c r="D105" s="244" t="s">
-        <v>990</v>
-      </c>
-      <c r="E105" s="245" t="s">
-        <v>995</v>
-      </c>
-      <c r="F105" s="199" t="s">
-        <v>997</v>
-      </c>
-      <c r="G105" s="178" t="s">
-        <v>1004</v>
       </c>
       <c r="H105" s="178"/>
       <c r="I105" s="179">
-        <v>43298</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" ht="69">
+        <v>43240</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" ht="69">
       <c r="A106" s="196" t="s">
         <v>644</v>
       </c>
       <c r="B106" s="178"/>
       <c r="C106" s="178"/>
-      <c r="D106" s="244" t="s">
-        <v>991</v>
-      </c>
-      <c r="E106" s="245" t="s">
-        <v>998</v>
+      <c r="D106" s="236" t="s">
+        <v>990</v>
+      </c>
+      <c r="E106" s="237" t="s">
+        <v>995</v>
       </c>
       <c r="F106" s="199" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G106" s="178" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="H106" s="178"/>
       <c r="I106" s="179">
         <v>43298</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="55.2">
+    <row r="107" spans="1:10" ht="69">
       <c r="A107" s="196" t="s">
         <v>644</v>
       </c>
       <c r="B107" s="178"/>
       <c r="C107" s="178"/>
-      <c r="D107" s="244" t="s">
-        <v>992</v>
-      </c>
-      <c r="E107" s="245" t="s">
+      <c r="D107" s="236" t="s">
+        <v>991</v>
+      </c>
+      <c r="E107" s="237" t="s">
         <v>998</v>
       </c>
       <c r="F107" s="199" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="G107" s="178" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="H107" s="178"/>
       <c r="I107" s="179">
         <v>43298</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="69">
+    <row r="108" spans="1:10" ht="55.2">
       <c r="A108" s="196" t="s">
         <v>644</v>
       </c>
       <c r="B108" s="178"/>
       <c r="C108" s="178"/>
-      <c r="D108" s="244" t="s">
-        <v>993</v>
-      </c>
-      <c r="E108" s="245" t="s">
-        <v>999</v>
+      <c r="D108" s="236" t="s">
+        <v>992</v>
+      </c>
+      <c r="E108" s="237" t="s">
+        <v>998</v>
       </c>
       <c r="F108" s="199" t="s">
         <v>997</v>
       </c>
       <c r="G108" s="178" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="H108" s="178"/>
       <c r="I108" s="179">
         <v>43298</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="69">
+    <row r="109" spans="1:10" ht="69">
       <c r="A109" s="196" t="s">
         <v>644</v>
       </c>
       <c r="B109" s="178"/>
       <c r="C109" s="178"/>
-      <c r="D109" s="244" t="s">
-        <v>994</v>
-      </c>
-      <c r="E109" s="245" t="s">
-        <v>1000</v>
+      <c r="D109" s="236" t="s">
+        <v>993</v>
+      </c>
+      <c r="E109" s="237" t="s">
+        <v>999</v>
       </c>
       <c r="F109" s="199" t="s">
         <v>997</v>
       </c>
       <c r="G109" s="178" t="s">
-        <v>1006</v>
+        <v>1001</v>
       </c>
       <c r="H109" s="178"/>
       <c r="I109" s="179">
         <v>43298</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="124.2">
-      <c r="A110" s="173" t="s">
+    <row r="110" spans="1:10" ht="69">
+      <c r="A110" s="196" t="s">
+        <v>644</v>
+      </c>
+      <c r="B110" s="178"/>
+      <c r="C110" s="178"/>
+      <c r="D110" s="236" t="s">
+        <v>994</v>
+      </c>
+      <c r="E110" s="237" t="s">
+        <v>1000</v>
+      </c>
+      <c r="F110" s="199" t="s">
+        <v>997</v>
+      </c>
+      <c r="G110" s="178" t="s">
+        <v>1006</v>
+      </c>
+      <c r="H110" s="178"/>
+      <c r="I110" s="179">
+        <v>43298</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" ht="124.2">
+      <c r="A111" s="173" t="s">
         <v>658</v>
       </c>
-      <c r="B110" s="178" t="s">
+      <c r="B111" s="178" t="s">
         <v>592</v>
-      </c>
-      <c r="C110" s="178"/>
-      <c r="D110" s="174" t="s">
-        <v>659</v>
-      </c>
-      <c r="E110" s="182" t="s">
-        <v>660</v>
-      </c>
-      <c r="F110" s="199" t="s">
-        <v>661</v>
-      </c>
-      <c r="G110" s="178" t="s">
-        <v>663</v>
-      </c>
-      <c r="H110" s="178"/>
-      <c r="I110" s="179"/>
-    </row>
-    <row r="111" spans="1:9" ht="138">
-      <c r="A111" s="196" t="s">
-        <v>658</v>
-      </c>
-      <c r="B111" s="178" t="s">
-        <v>664</v>
       </c>
       <c r="C111" s="178"/>
       <c r="D111" s="174" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
       <c r="E111" s="182" t="s">
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="F111" s="199" t="s">
         <v>661</v>
       </c>
       <c r="G111" s="178" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="H111" s="178"/>
       <c r="I111" s="179"/>
     </row>
-    <row r="112" spans="1:9" ht="124.2">
+    <row r="112" spans="1:10" ht="138">
       <c r="A112" s="196" t="s">
         <v>658</v>
       </c>
       <c r="B112" s="178" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="C112" s="178"/>
       <c r="D112" s="174" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="E112" s="182" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="F112" s="199" t="s">
         <v>661</v>
       </c>
-      <c r="G112" s="194" t="s">
-        <v>671</v>
+      <c r="G112" s="178" t="s">
+        <v>667</v>
       </c>
       <c r="H112" s="178"/>
       <c r="I112" s="179"/>
     </row>
-    <row r="113" spans="1:9" ht="82.8">
-      <c r="A113" s="173" t="s">
+    <row r="113" spans="1:9" ht="124.2">
+      <c r="A113" s="196" t="s">
+        <v>658</v>
+      </c>
+      <c r="B113" s="178" t="s">
+        <v>668</v>
+      </c>
+      <c r="C113" s="178"/>
+      <c r="D113" s="174" t="s">
+        <v>669</v>
+      </c>
+      <c r="E113" s="182" t="s">
+        <v>670</v>
+      </c>
+      <c r="F113" s="199" t="s">
+        <v>661</v>
+      </c>
+      <c r="G113" s="194" t="s">
+        <v>671</v>
+      </c>
+      <c r="H113" s="178"/>
+      <c r="I113" s="179"/>
+    </row>
+    <row r="114" spans="1:9" ht="82.8">
+      <c r="A114" s="173" t="s">
         <v>672</v>
       </c>
-      <c r="B113" s="178" t="s">
+      <c r="B114" s="178" t="s">
         <v>151</v>
       </c>
-      <c r="C113" s="174" t="s">
+      <c r="C114" s="174" t="s">
         <v>673</v>
       </c>
-      <c r="D113" s="174" t="s">
+      <c r="D114" s="174" t="s">
         <v>675</v>
       </c>
-      <c r="E113" s="176"/>
-      <c r="F113" s="204" t="s">
+      <c r="E114" s="176"/>
+      <c r="F114" s="204" t="s">
         <v>677</v>
       </c>
-      <c r="G113" s="178" t="s">
+      <c r="G114" s="178" t="s">
         <v>686</v>
       </c>
-      <c r="H113" s="178"/>
-      <c r="I113" s="179">
-        <v>43196</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" ht="41.4">
-      <c r="A114" s="173" t="s">
-        <v>687</v>
-      </c>
-      <c r="B114" s="174" t="s">
-        <v>77</v>
-      </c>
-      <c r="C114" s="174" t="s">
-        <v>22</v>
-      </c>
-      <c r="D114" s="175" t="s">
-        <v>689</v>
-      </c>
-      <c r="E114" s="182"/>
-      <c r="F114" s="211" t="s">
-        <v>971</v>
-      </c>
-      <c r="G114" s="178"/>
       <c r="H114" s="178"/>
       <c r="I114" s="179">
-        <v>43276</v>
+        <v>43196</v>
       </c>
     </row>
     <row r="115" spans="1:9" ht="41.4">
@@ -8828,11 +8843,11 @@
         <v>22</v>
       </c>
       <c r="D115" s="175" t="s">
-        <v>699</v>
+        <v>689</v>
       </c>
       <c r="E115" s="182"/>
-      <c r="F115" s="193" t="s">
-        <v>972</v>
+      <c r="F115" s="211" t="s">
+        <v>971</v>
       </c>
       <c r="G115" s="178"/>
       <c r="H115" s="178"/>
@@ -8840,112 +8855,110 @@
         <v>43276</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="55.2">
+    <row r="116" spans="1:9" ht="41.4">
       <c r="A116" s="173" t="s">
-        <v>706</v>
+        <v>687</v>
       </c>
       <c r="B116" s="174" t="s">
         <v>77</v>
       </c>
-      <c r="C116" s="174"/>
-      <c r="D116" s="174" t="s">
-        <v>707</v>
-      </c>
-      <c r="E116" s="176" t="s">
-        <v>708</v>
-      </c>
+      <c r="C116" s="174" t="s">
+        <v>22</v>
+      </c>
+      <c r="D116" s="175" t="s">
+        <v>699</v>
+      </c>
+      <c r="E116" s="182"/>
       <c r="F116" s="193" t="s">
-        <v>710</v>
-      </c>
-      <c r="G116" s="178" t="s">
-        <v>713</v>
-      </c>
+        <v>972</v>
+      </c>
+      <c r="G116" s="178"/>
       <c r="H116" s="178"/>
       <c r="I116" s="179">
-        <v>43293</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" ht="207">
+        <v>43276</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" ht="55.2">
       <c r="A117" s="173" t="s">
-        <v>714</v>
-      </c>
-      <c r="B117" s="178" t="s">
-        <v>45</v>
-      </c>
-      <c r="C117" s="178" t="s">
-        <v>22</v>
-      </c>
-      <c r="D117" s="200" t="s">
-        <v>717</v>
-      </c>
-      <c r="E117" s="176"/>
-      <c r="F117" s="199" t="s">
-        <v>720</v>
+        <v>706</v>
+      </c>
+      <c r="B117" s="174" t="s">
+        <v>77</v>
+      </c>
+      <c r="C117" s="174"/>
+      <c r="D117" s="174" t="s">
+        <v>707</v>
+      </c>
+      <c r="E117" s="176" t="s">
+        <v>708</v>
+      </c>
+      <c r="F117" s="193" t="s">
+        <v>710</v>
       </c>
       <c r="G117" s="178" t="s">
-        <v>721</v>
+        <v>713</v>
       </c>
       <c r="H117" s="178"/>
       <c r="I117" s="179">
+        <v>43293</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" ht="207">
+      <c r="A118" s="173" t="s">
+        <v>714</v>
+      </c>
+      <c r="B118" s="178" t="s">
+        <v>45</v>
+      </c>
+      <c r="C118" s="178" t="s">
+        <v>22</v>
+      </c>
+      <c r="D118" s="200" t="s">
+        <v>717</v>
+      </c>
+      <c r="E118" s="176"/>
+      <c r="F118" s="199" t="s">
+        <v>720</v>
+      </c>
+      <c r="G118" s="178" t="s">
+        <v>721</v>
+      </c>
+      <c r="H118" s="178"/>
+      <c r="I118" s="179">
         <v>43240</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="69">
-      <c r="A118" s="173" t="s">
-        <v>722</v>
-      </c>
-      <c r="B118" s="194" t="s">
-        <v>151</v>
-      </c>
-      <c r="C118" s="194">
-        <v>8000823</v>
-      </c>
-      <c r="D118" s="174" t="s">
-        <v>729</v>
-      </c>
-      <c r="E118" s="182" t="s">
-        <v>733</v>
-      </c>
-      <c r="F118" s="220" t="s">
-        <v>735</v>
-      </c>
-      <c r="G118" s="194" t="s">
-        <v>736</v>
-      </c>
-      <c r="H118" s="178" t="s">
-        <v>737</v>
-      </c>
-      <c r="I118" s="179">
-        <v>43196</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" ht="82.8">
+    <row r="119" spans="1:9" ht="69">
       <c r="A119" s="173" t="s">
         <v>722</v>
       </c>
       <c r="B119" s="194" t="s">
         <v>151</v>
       </c>
-      <c r="C119" s="194"/>
+      <c r="C119" s="194">
+        <v>8000823</v>
+      </c>
       <c r="D119" s="174" t="s">
-        <v>738</v>
+        <v>729</v>
       </c>
       <c r="E119" s="182" t="s">
-        <v>739</v>
-      </c>
-      <c r="F119" s="177" t="s">
-        <v>741</v>
-      </c>
-      <c r="G119" s="199" t="s">
-        <v>743</v>
-      </c>
-      <c r="H119" s="178"/>
+        <v>733</v>
+      </c>
+      <c r="F119" s="220" t="s">
+        <v>735</v>
+      </c>
+      <c r="G119" s="194" t="s">
+        <v>736</v>
+      </c>
+      <c r="H119" s="178" t="s">
+        <v>737</v>
+      </c>
       <c r="I119" s="179">
         <v>43196</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="41.4">
-      <c r="A120" s="196" t="s">
+    <row r="120" spans="1:9" ht="82.8">
+      <c r="A120" s="173" t="s">
         <v>722</v>
       </c>
       <c r="B120" s="194" t="s">
@@ -8953,101 +8966,103 @@
       </c>
       <c r="C120" s="194"/>
       <c r="D120" s="174" t="s">
-        <v>745</v>
+        <v>738</v>
       </c>
       <c r="E120" s="182" t="s">
-        <v>746</v>
-      </c>
-      <c r="F120" s="178" t="s">
-        <v>747</v>
-      </c>
-      <c r="G120" s="177" t="s">
-        <v>748</v>
+        <v>739</v>
+      </c>
+      <c r="F120" s="177" t="s">
+        <v>741</v>
+      </c>
+      <c r="G120" s="199" t="s">
+        <v>743</v>
       </c>
       <c r="H120" s="178"/>
       <c r="I120" s="179">
         <v>43196</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="27.6">
-      <c r="A121" s="173" t="s">
-        <v>749</v>
-      </c>
-      <c r="B121" s="178" t="s">
-        <v>144</v>
-      </c>
-      <c r="C121" s="178" t="s">
-        <v>22</v>
-      </c>
-      <c r="D121" s="197" t="s">
-        <v>750</v>
-      </c>
-      <c r="E121" s="222" t="s">
-        <v>762</v>
-      </c>
-      <c r="F121" s="201" t="s">
-        <v>772</v>
-      </c>
-      <c r="G121" s="178" t="s">
-        <v>773</v>
+    <row r="121" spans="1:9" ht="41.4">
+      <c r="A121" s="196" t="s">
+        <v>722</v>
+      </c>
+      <c r="B121" s="194" t="s">
+        <v>151</v>
+      </c>
+      <c r="C121" s="194"/>
+      <c r="D121" s="174" t="s">
+        <v>745</v>
+      </c>
+      <c r="E121" s="182" t="s">
+        <v>746</v>
+      </c>
+      <c r="F121" s="178" t="s">
+        <v>747</v>
+      </c>
+      <c r="G121" s="177" t="s">
+        <v>748</v>
       </c>
       <c r="H121" s="178"/>
       <c r="I121" s="179">
-        <v>43250</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" ht="82.8">
+        <v>43196</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" ht="27.6">
       <c r="A122" s="173" t="s">
-        <v>774</v>
+        <v>749</v>
       </c>
       <c r="B122" s="178" t="s">
-        <v>775</v>
+        <v>144</v>
       </c>
       <c r="C122" s="178" t="s">
         <v>22</v>
       </c>
-      <c r="D122" s="200" t="s">
+      <c r="D122" s="197" t="s">
+        <v>750</v>
+      </c>
+      <c r="E122" s="222" t="s">
+        <v>762</v>
+      </c>
+      <c r="F122" s="201" t="s">
+        <v>772</v>
+      </c>
+      <c r="G122" s="178" t="s">
+        <v>773</v>
+      </c>
+      <c r="H122" s="178"/>
+      <c r="I122" s="179">
+        <v>43250</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" ht="82.8">
+      <c r="A123" s="173" t="s">
+        <v>774</v>
+      </c>
+      <c r="B123" s="178" t="s">
+        <v>775</v>
+      </c>
+      <c r="C123" s="178" t="s">
+        <v>22</v>
+      </c>
+      <c r="D123" s="200" t="s">
         <v>776</v>
       </c>
-      <c r="E122" s="222" t="s">
+      <c r="E123" s="222" t="s">
         <v>609</v>
       </c>
-      <c r="F122" s="199" t="s">
+      <c r="F123" s="199" t="s">
         <v>777</v>
       </c>
-      <c r="G122" s="178" t="s">
+      <c r="G123" s="178" t="s">
         <v>778</v>
       </c>
-      <c r="H122" s="223"/>
-      <c r="I122" s="179">
+      <c r="H123" s="223"/>
+      <c r="I123" s="179">
         <v>43264</v>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="27.6">
-      <c r="A123" s="173" t="s">
-        <v>780</v>
-      </c>
-      <c r="B123" s="178" t="s">
-        <v>781</v>
-      </c>
-      <c r="C123" s="178"/>
-      <c r="D123" s="191" t="s">
-        <v>782</v>
-      </c>
-      <c r="E123" s="192" t="s">
-        <v>786</v>
-      </c>
-      <c r="F123" s="201" t="s">
-        <v>787</v>
-      </c>
-      <c r="G123" s="178"/>
-      <c r="H123" s="224" t="s">
-        <v>978</v>
-      </c>
-      <c r="I123" s="179"/>
-    </row>
     <row r="124" spans="1:9" ht="27.6">
-      <c r="A124" s="196" t="s">
+      <c r="A124" s="173" t="s">
         <v>780</v>
       </c>
       <c r="B124" s="178" t="s">
@@ -9055,7 +9070,7 @@
       </c>
       <c r="C124" s="178"/>
       <c r="D124" s="191" t="s">
-        <v>788</v>
+        <v>782</v>
       </c>
       <c r="E124" s="192" t="s">
         <v>786</v>
@@ -9078,7 +9093,7 @@
       </c>
       <c r="C125" s="178"/>
       <c r="D125" s="191" t="s">
-        <v>797</v>
+        <v>788</v>
       </c>
       <c r="E125" s="192" t="s">
         <v>786</v>
@@ -9094,153 +9109,149 @@
     </row>
     <row r="126" spans="1:9" ht="27.6">
       <c r="A126" s="196" t="s">
+        <v>780</v>
+      </c>
+      <c r="B126" s="178" t="s">
+        <v>781</v>
+      </c>
+      <c r="C126" s="178"/>
+      <c r="D126" s="191" t="s">
+        <v>797</v>
+      </c>
+      <c r="E126" s="192" t="s">
+        <v>786</v>
+      </c>
+      <c r="F126" s="201" t="s">
+        <v>787</v>
+      </c>
+      <c r="G126" s="178"/>
+      <c r="H126" s="224" t="s">
+        <v>978</v>
+      </c>
+      <c r="I126" s="179"/>
+    </row>
+    <row r="127" spans="1:9" ht="27.6">
+      <c r="A127" s="196" t="s">
         <v>810</v>
       </c>
-      <c r="B126" s="178" t="s">
+      <c r="B127" s="178" t="s">
         <v>811</v>
       </c>
-      <c r="C126" s="174" t="s">
+      <c r="C127" s="174" t="s">
         <v>812</v>
       </c>
-      <c r="D126" s="174" t="s">
+      <c r="D127" s="174" t="s">
         <v>814</v>
       </c>
-      <c r="E126" s="182" t="s">
+      <c r="E127" s="182" t="s">
         <v>819</v>
       </c>
-      <c r="F126" s="199" t="s">
+      <c r="F127" s="199" t="s">
         <v>820</v>
       </c>
-      <c r="G126" s="178" t="s">
+      <c r="G127" s="178" t="s">
         <v>821</v>
       </c>
-      <c r="H126" s="223"/>
-      <c r="I126" s="179"/>
-    </row>
-    <row r="127" spans="1:9">
-      <c r="A127" s="173" t="s">
+      <c r="H127" s="223"/>
+      <c r="I127" s="179"/>
+    </row>
+    <row r="128" spans="1:9">
+      <c r="A128" s="173" t="s">
         <v>822</v>
-      </c>
-      <c r="B127" s="178" t="s">
-        <v>45</v>
-      </c>
-      <c r="C127" s="174" t="s">
-        <v>823</v>
-      </c>
-      <c r="D127" s="200" t="s">
-        <v>824</v>
-      </c>
-      <c r="E127" s="176" t="s">
-        <v>609</v>
-      </c>
-      <c r="F127" s="201" t="s">
-        <v>836</v>
-      </c>
-      <c r="G127" s="178"/>
-      <c r="H127" s="178"/>
-      <c r="I127" s="179">
-        <v>43240</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9" ht="96.6">
-      <c r="A128" s="173" t="s">
-        <v>842</v>
       </c>
       <c r="B128" s="178" t="s">
         <v>45</v>
       </c>
-      <c r="C128" s="178" t="s">
-        <v>22</v>
-      </c>
-      <c r="D128" s="178" t="s">
-        <v>843</v>
+      <c r="C128" s="174" t="s">
+        <v>823</v>
+      </c>
+      <c r="D128" s="200" t="s">
+        <v>824</v>
       </c>
       <c r="E128" s="176" t="s">
-        <v>842</v>
+        <v>609</v>
       </c>
       <c r="F128" s="201" t="s">
-        <v>849</v>
-      </c>
-      <c r="G128" s="180" t="s">
-        <v>973</v>
-      </c>
+        <v>836</v>
+      </c>
+      <c r="G128" s="178"/>
       <c r="H128" s="178"/>
       <c r="I128" s="179">
         <v>43240</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="41.4">
+    <row r="129" spans="1:9" ht="96.6">
       <c r="A129" s="173" t="s">
-        <v>850</v>
+        <v>842</v>
       </c>
       <c r="B129" s="178" t="s">
-        <v>851</v>
-      </c>
-      <c r="C129" s="178"/>
-      <c r="D129" s="178"/>
-      <c r="E129" s="176"/>
-      <c r="F129" s="199" t="s">
-        <v>856</v>
-      </c>
-      <c r="G129" s="178"/>
+        <v>45</v>
+      </c>
+      <c r="C129" s="178" t="s">
+        <v>22</v>
+      </c>
+      <c r="D129" s="178" t="s">
+        <v>843</v>
+      </c>
+      <c r="E129" s="176" t="s">
+        <v>842</v>
+      </c>
+      <c r="F129" s="201" t="s">
+        <v>849</v>
+      </c>
+      <c r="G129" s="180" t="s">
+        <v>973</v>
+      </c>
       <c r="H129" s="178"/>
       <c r="I129" s="179">
-        <v>43196</v>
+        <v>43240</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="41.4">
       <c r="A130" s="173" t="s">
-        <v>857</v>
-      </c>
-      <c r="B130" s="174" t="s">
-        <v>295</v>
-      </c>
-      <c r="C130" s="174"/>
-      <c r="D130" s="209" t="s">
-        <v>859</v>
-      </c>
-      <c r="E130" s="182" t="s">
-        <v>860</v>
-      </c>
-      <c r="F130" s="177" t="s">
-        <v>861</v>
-      </c>
-      <c r="G130" s="178" t="s">
-        <v>869</v>
-      </c>
+        <v>850</v>
+      </c>
+      <c r="B130" s="178" t="s">
+        <v>851</v>
+      </c>
+      <c r="C130" s="178"/>
+      <c r="D130" s="178"/>
+      <c r="E130" s="176"/>
+      <c r="F130" s="199" t="s">
+        <v>856</v>
+      </c>
+      <c r="G130" s="178"/>
       <c r="H130" s="178"/>
       <c r="I130" s="179">
+        <v>43196</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" ht="41.4">
+      <c r="A131" s="173" t="s">
+        <v>857</v>
+      </c>
+      <c r="B131" s="174" t="s">
+        <v>295</v>
+      </c>
+      <c r="C131" s="174"/>
+      <c r="D131" s="209" t="s">
+        <v>859</v>
+      </c>
+      <c r="E131" s="182" t="s">
+        <v>860</v>
+      </c>
+      <c r="F131" s="177" t="s">
+        <v>861</v>
+      </c>
+      <c r="G131" s="178" t="s">
+        <v>869</v>
+      </c>
+      <c r="H131" s="178"/>
+      <c r="I131" s="179">
         <v>43288</v>
       </c>
     </row>
-    <row r="131" spans="1:9" ht="138">
-      <c r="A131" s="173" t="s">
-        <v>871</v>
-      </c>
-      <c r="B131" s="174" t="s">
-        <v>77</v>
-      </c>
-      <c r="C131" s="174" t="s">
-        <v>22</v>
-      </c>
-      <c r="D131" s="175" t="s">
-        <v>872</v>
-      </c>
-      <c r="E131" s="182"/>
-      <c r="F131" s="193" t="s">
-        <v>873</v>
-      </c>
-      <c r="G131" s="178" t="s">
-        <v>874</v>
-      </c>
-      <c r="H131" s="224" t="s">
-        <v>978</v>
-      </c>
-      <c r="I131" s="179">
-        <v>43270</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9" ht="41.4">
+    <row r="132" spans="1:9" ht="138">
       <c r="A132" s="173" t="s">
         <v>871</v>
       </c>
@@ -9251,17 +9262,17 @@
         <v>22</v>
       </c>
       <c r="D132" s="175" t="s">
-        <v>875</v>
+        <v>872</v>
       </c>
       <c r="E132" s="182"/>
       <c r="F132" s="193" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
       <c r="G132" s="178" t="s">
-        <v>877</v>
-      </c>
-      <c r="H132" s="195" t="s">
-        <v>979</v>
+        <v>874</v>
+      </c>
+      <c r="H132" s="224" t="s">
+        <v>978</v>
       </c>
       <c r="I132" s="179">
         <v>43270</v>
@@ -9278,11 +9289,11 @@
         <v>22</v>
       </c>
       <c r="D133" s="175" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
       <c r="E133" s="182"/>
       <c r="F133" s="193" t="s">
-        <v>879</v>
+        <v>876</v>
       </c>
       <c r="G133" s="178" t="s">
         <v>877</v>
@@ -9305,15 +9316,17 @@
         <v>22</v>
       </c>
       <c r="D134" s="175" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="E134" s="182"/>
-      <c r="F134" s="211" t="s">
-        <v>881</v>
-      </c>
-      <c r="G134" s="178"/>
-      <c r="H134" s="224" t="s">
-        <v>978</v>
+      <c r="F134" s="193" t="s">
+        <v>879</v>
+      </c>
+      <c r="G134" s="178" t="s">
+        <v>877</v>
+      </c>
+      <c r="H134" s="195" t="s">
+        <v>979</v>
       </c>
       <c r="I134" s="179">
         <v>43270</v>
@@ -9321,69 +9334,83 @@
     </row>
     <row r="135" spans="1:9" ht="41.4">
       <c r="A135" s="173" t="s">
+        <v>871</v>
+      </c>
+      <c r="B135" s="174" t="s">
+        <v>77</v>
+      </c>
+      <c r="C135" s="174" t="s">
+        <v>22</v>
+      </c>
+      <c r="D135" s="175" t="s">
+        <v>880</v>
+      </c>
+      <c r="E135" s="182"/>
+      <c r="F135" s="211" t="s">
+        <v>881</v>
+      </c>
+      <c r="G135" s="178"/>
+      <c r="H135" s="224" t="s">
+        <v>978</v>
+      </c>
+      <c r="I135" s="179">
+        <v>43270</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" ht="41.4">
+      <c r="A136" s="173" t="s">
         <v>882</v>
       </c>
-      <c r="B135" s="178" t="s">
+      <c r="B136" s="178" t="s">
         <v>144</v>
-      </c>
-      <c r="C135" s="178" t="s">
-        <v>22</v>
-      </c>
-      <c r="D135" s="197" t="s">
-        <v>883</v>
-      </c>
-      <c r="E135" s="225" t="s">
-        <v>884</v>
-      </c>
-      <c r="F135" s="201" t="s">
-        <v>772</v>
-      </c>
-      <c r="G135" s="178" t="s">
-        <v>891</v>
-      </c>
-      <c r="H135" s="224" t="s">
-        <v>980</v>
-      </c>
-      <c r="I135" s="179">
-        <v>43250</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9" ht="27.6">
-      <c r="A136" s="173" t="s">
-        <v>892</v>
-      </c>
-      <c r="B136" s="178" t="s">
-        <v>775</v>
       </c>
       <c r="C136" s="178" t="s">
         <v>22</v>
       </c>
-      <c r="D136" s="200" t="s">
+      <c r="D136" s="197" t="s">
+        <v>883</v>
+      </c>
+      <c r="E136" s="225" t="s">
+        <v>884</v>
+      </c>
+      <c r="F136" s="201" t="s">
+        <v>772</v>
+      </c>
+      <c r="G136" s="178" t="s">
+        <v>891</v>
+      </c>
+      <c r="H136" s="224" t="s">
+        <v>980</v>
+      </c>
+      <c r="I136" s="179">
+        <v>43250</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" ht="27.6">
+      <c r="A137" s="173" t="s">
+        <v>892</v>
+      </c>
+      <c r="B137" s="178" t="s">
+        <v>775</v>
+      </c>
+      <c r="C137" s="178" t="s">
+        <v>22</v>
+      </c>
+      <c r="D137" s="200" t="s">
         <v>898</v>
       </c>
-      <c r="F136" s="201" t="s">
+      <c r="F137" s="201" t="s">
         <v>909</v>
       </c>
-      <c r="H136" s="224" t="s">
+      <c r="H137" s="224" t="s">
         <v>978</v>
       </c>
-      <c r="I136" s="226">
+      <c r="I137" s="226">
         <v>43288</v>
       </c>
     </row>
-    <row r="137" spans="1:9">
-      <c r="D137" s="178"/>
-    </row>
     <row r="138" spans="1:9">
-      <c r="A138" s="173"/>
-      <c r="B138" s="174"/>
-      <c r="C138" s="174"/>
-      <c r="D138" s="174"/>
-      <c r="E138" s="182"/>
-      <c r="F138" s="213"/>
-      <c r="G138" s="178"/>
-      <c r="H138" s="178"/>
-      <c r="I138" s="179"/>
+      <c r="D138" s="178"/>
     </row>
     <row r="139" spans="1:9">
       <c r="A139" s="173"/>
@@ -9462,9 +9489,20 @@
       <c r="H145" s="178"/>
       <c r="I145" s="179"/>
     </row>
+    <row r="146" spans="1:9">
+      <c r="A146" s="173"/>
+      <c r="B146" s="174"/>
+      <c r="C146" s="174"/>
+      <c r="D146" s="174"/>
+      <c r="E146" s="182"/>
+      <c r="F146" s="213"/>
+      <c r="G146" s="178"/>
+      <c r="H146" s="178"/>
+      <c r="I146" s="179"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F113" r:id="rId1" location="gid=314589613&amp;range=309:309"/>
+    <hyperlink ref="F114" r:id="rId1" location="gid=314589613&amp;range=309:309"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -9480,8 +9518,8 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21:XFD25"/>
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2"/>
@@ -9514,10 +9552,10 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="227" t="s">
+      <c r="I1" s="238" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="228"/>
+      <c r="J1" s="239"/>
     </row>
     <row r="2" spans="1:10" ht="26.4">
       <c r="A2" s="1"/>
@@ -10004,10 +10042,10 @@
       <c r="C19" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="235" t="s">
+      <c r="D19" s="227" t="s">
         <v>110</v>
       </c>
-      <c r="E19" s="236" t="s">
+      <c r="E19" s="228" t="s">
         <v>108</v>
       </c>
       <c r="F19" s="40" t="s">
@@ -10020,28 +10058,28 @@
       <c r="I19" s="12"/>
       <c r="J19" s="36"/>
     </row>
-    <row r="20" spans="1:10" s="242" customFormat="1" ht="66">
-      <c r="A20" s="237" t="s">
+    <row r="20" spans="1:10" s="234" customFormat="1" ht="66">
+      <c r="A20" s="229" t="s">
         <v>644</v>
       </c>
-      <c r="B20" s="237" t="s">
+      <c r="B20" s="229" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="237" t="s">
+      <c r="C20" s="229" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="238" t="s">
+      <c r="D20" s="230" t="s">
         <v>988</v>
       </c>
-      <c r="E20" s="239"/>
-      <c r="F20" s="240" t="s">
+      <c r="E20" s="231"/>
+      <c r="F20" s="232" t="s">
         <v>987</v>
       </c>
-      <c r="G20" s="237" t="s">
+      <c r="G20" s="229" t="s">
         <v>986</v>
       </c>
-      <c r="H20" s="237"/>
-      <c r="I20" s="241">
+      <c r="H20" s="229"/>
+      <c r="I20" s="233">
         <v>43240</v>
       </c>
     </row>
@@ -10121,8 +10159,8 @@
   </sheetPr>
   <dimension ref="A1:J128"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B79" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B106" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="H55" sqref="H55"/>
@@ -10166,10 +10204,10 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="227" t="s">
+      <c r="I1" s="238" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="228"/>
+      <c r="J1" s="239"/>
     </row>
     <row r="2" spans="1:10" ht="26.4">
       <c r="A2" s="1"/>
@@ -10240,13 +10278,13 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="86.4">
-      <c r="A5" s="232" t="s">
+      <c r="A5" s="243" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="229" t="s">
+      <c r="B5" s="240" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="229" t="s">
+      <c r="C5" s="240" t="s">
         <v>42</v>
       </c>
       <c r="D5" s="13" t="s">
@@ -10268,9 +10306,9 @@
       <c r="J5" s="32"/>
     </row>
     <row r="6" spans="1:10" ht="86.4">
-      <c r="A6" s="228"/>
-      <c r="B6" s="228"/>
-      <c r="C6" s="228"/>
+      <c r="A6" s="239"/>
+      <c r="B6" s="239"/>
+      <c r="C6" s="239"/>
       <c r="D6" s="13" t="s">
         <v>68</v>
       </c>
@@ -10288,7 +10326,7 @@
       <c r="J6" s="36"/>
     </row>
     <row r="7" spans="1:10" ht="39.6">
-      <c r="A7" s="232" t="s">
+      <c r="A7" s="243" t="s">
         <v>79</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -10318,7 +10356,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="39.6">
-      <c r="A8" s="228"/>
+      <c r="A8" s="239"/>
       <c r="B8" s="8" t="s">
         <v>21</v>
       </c>
@@ -10345,7 +10383,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="39.6">
-      <c r="A9" s="231"/>
+      <c r="A9" s="242"/>
       <c r="B9" s="47" t="s">
         <v>21</v>
       </c>
@@ -10397,7 +10435,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="39.6">
-      <c r="A11" s="233" t="s">
+      <c r="A11" s="244" t="s">
         <v>119</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -10426,7 +10464,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="39.6">
-      <c r="A12" s="228"/>
+      <c r="A12" s="239"/>
       <c r="B12" s="8" t="s">
         <v>21</v>
       </c>
@@ -10453,7 +10491,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="39.6">
-      <c r="A13" s="228"/>
+      <c r="A13" s="239"/>
       <c r="B13" s="8" t="s">
         <v>21</v>
       </c>
@@ -10480,7 +10518,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="39.6">
-      <c r="A14" s="228"/>
+      <c r="A14" s="239"/>
       <c r="B14" s="47" t="s">
         <v>21</v>
       </c>
@@ -10874,7 +10912,7 @@
       </c>
     </row>
     <row r="36" spans="1:10" ht="39.6">
-      <c r="A36" s="230" t="s">
+      <c r="A36" s="241" t="s">
         <v>376</v>
       </c>
       <c r="B36" s="90" t="s">
@@ -10904,7 +10942,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" ht="39.6">
-      <c r="A37" s="228"/>
+      <c r="A37" s="239"/>
       <c r="B37" s="8" t="s">
         <v>21</v>
       </c>
@@ -10932,7 +10970,7 @@
       </c>
     </row>
     <row r="38" spans="1:10" ht="66">
-      <c r="A38" s="228"/>
+      <c r="A38" s="239"/>
       <c r="B38" s="8" t="s">
         <v>21</v>
       </c>
@@ -10960,7 +10998,7 @@
       </c>
     </row>
     <row r="39" spans="1:10" ht="39.6">
-      <c r="A39" s="228"/>
+      <c r="A39" s="239"/>
       <c r="B39" s="8" t="s">
         <v>21</v>
       </c>
@@ -10988,7 +11026,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" ht="39.6">
-      <c r="A40" s="228"/>
+      <c r="A40" s="239"/>
       <c r="B40" s="8" t="s">
         <v>21</v>
       </c>
@@ -11016,7 +11054,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="39.6">
-      <c r="A41" s="228"/>
+      <c r="A41" s="239"/>
       <c r="B41" s="8" t="s">
         <v>21</v>
       </c>
@@ -11044,7 +11082,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="39.6">
-      <c r="A42" s="228"/>
+      <c r="A42" s="239"/>
       <c r="B42" s="8" t="s">
         <v>21</v>
       </c>
@@ -11072,7 +11110,7 @@
       </c>
     </row>
     <row r="43" spans="1:10" ht="39.6">
-      <c r="A43" s="228"/>
+      <c r="A43" s="239"/>
       <c r="B43" s="8" t="s">
         <v>21</v>
       </c>
@@ -11100,7 +11138,7 @@
       </c>
     </row>
     <row r="44" spans="1:10" ht="39.6">
-      <c r="A44" s="228"/>
+      <c r="A44" s="239"/>
       <c r="B44" s="8" t="s">
         <v>21</v>
       </c>
@@ -11128,7 +11166,7 @@
       </c>
     </row>
     <row r="45" spans="1:10" ht="39.6">
-      <c r="A45" s="231"/>
+      <c r="A45" s="242"/>
       <c r="B45" s="47" t="s">
         <v>21</v>
       </c>
@@ -11216,7 +11254,7 @@
       </c>
     </row>
     <row r="48" spans="1:10" ht="66">
-      <c r="A48" s="230" t="s">
+      <c r="A48" s="241" t="s">
         <v>496</v>
       </c>
       <c r="B48" s="90" t="s">
@@ -11246,7 +11284,7 @@
       </c>
     </row>
     <row r="49" spans="1:10" ht="39.6">
-      <c r="A49" s="231"/>
+      <c r="A49" s="242"/>
       <c r="B49" s="47" t="s">
         <v>21</v>
       </c>
@@ -12376,7 +12414,7 @@
       </c>
     </row>
     <row r="88" spans="1:10" ht="39.6">
-      <c r="A88" s="232" t="s">
+      <c r="A88" s="243" t="s">
         <v>784</v>
       </c>
       <c r="B88" s="8" t="s">
@@ -12406,7 +12444,7 @@
       </c>
     </row>
     <row r="89" spans="1:10" ht="39.6">
-      <c r="A89" s="228"/>
+      <c r="A89" s="239"/>
       <c r="B89" s="8" t="s">
         <v>45</v>
       </c>
@@ -12434,7 +12472,7 @@
       </c>
     </row>
     <row r="90" spans="1:10" ht="39.6">
-      <c r="A90" s="228"/>
+      <c r="A90" s="239"/>
       <c r="B90" s="8" t="s">
         <v>45</v>
       </c>
@@ -12462,7 +12500,7 @@
       </c>
     </row>
     <row r="91" spans="1:10" ht="39.6">
-      <c r="A91" s="228"/>
+      <c r="A91" s="239"/>
       <c r="B91" s="8" t="s">
         <v>45</v>
       </c>
@@ -12490,7 +12528,7 @@
       </c>
     </row>
     <row r="92" spans="1:10" ht="39.6">
-      <c r="A92" s="228"/>
+      <c r="A92" s="239"/>
       <c r="B92" s="8" t="s">
         <v>45</v>
       </c>
@@ -12518,7 +12556,7 @@
       </c>
     </row>
     <row r="93" spans="1:10" ht="39.6">
-      <c r="A93" s="228"/>
+      <c r="A93" s="239"/>
       <c r="B93" s="8" t="s">
         <v>45</v>
       </c>
@@ -12546,7 +12584,7 @@
       </c>
     </row>
     <row r="94" spans="1:10" ht="39.6">
-      <c r="A94" s="228"/>
+      <c r="A94" s="239"/>
       <c r="B94" s="8" t="s">
         <v>45</v>
       </c>
@@ -12574,7 +12612,7 @@
       </c>
     </row>
     <row r="95" spans="1:10" ht="39.6">
-      <c r="A95" s="228"/>
+      <c r="A95" s="239"/>
       <c r="B95" s="8" t="s">
         <v>45</v>
       </c>
@@ -13463,10 +13501,10 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="234" t="s">
+      <c r="I1" s="245" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="228"/>
+      <c r="J1" s="239"/>
     </row>
     <row r="2" spans="1:10" ht="26.4">
       <c r="A2" s="3"/>

</xml_diff>

<commit_message>
Restored lost changes to Action Items
</commit_message>
<xml_diff>
--- a/Working QA Team Folders/Pre- Release QA/Action Items (Master).xlsx
+++ b/Working QA Team Folders/Pre- Release QA/Action Items (Master).xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barbj\Documents\Infoway-Health Canada CCDD\formulary\Working QA Team Folders\Pre- Release QA\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D0A31C1B-A009-4E14-95F9-9DC6FBBE9C11}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="180" windowWidth="17268" windowHeight="5256"/>
+    <workbookView xWindow="0" yWindow="180" windowWidth="17268" windowHeight="5256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Action Items, Open" sheetId="1" r:id="rId1"/>
@@ -12,17 +18,17 @@
     <sheet name="Completed AIs Released" sheetId="3" r:id="rId3"/>
     <sheet name="AIs no longer relevant" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="F130" authorId="0">
+    <comment ref="F131" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -34,7 +40,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F142" authorId="0">
+    <comment ref="F143" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -51,12 +57,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="G21" authorId="0">
+    <comment ref="G21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -68,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="0">
+    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -88,12 +94,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="E93" authorId="0">
+    <comment ref="E93" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -105,7 +111,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G101" authorId="0">
+    <comment ref="G101" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -119,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H122" authorId="0">
+    <comment ref="H122" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -136,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1795" uniqueCount="1086">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1804" uniqueCount="1094">
   <si>
     <t>TM</t>
   </si>
@@ -4631,18 +4637,105 @@
   <si>
     <t>fluorometholone acetate 0.1 % ophthalmic drops</t>
   </si>
+  <si>
+    <t>pilocarpine</t>
+  </si>
+  <si>
+    <t>August Release QA</t>
+  </si>
+  <si>
+    <t>0000868
+0000841
+0000844</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. pilocarpine hydrochloride 20 mg per mL ophthalmic drops </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF521BED"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(2 %)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2. pilocarpine hydrochloride 40 mg per mL ophthalmic drops </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF521BED"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(4 %)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+3. pilocarpine hydrochloride 10 mg per mL ophthalmic drops </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF521BED"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(1 %)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Louise: Change strength to percentage. </t>
+  </si>
+  <si>
+    <t>Aug 3 2018</t>
+  </si>
+  <si>
+    <t>Done - one remaining action item for TM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outstanding </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="mmmm\ d\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="166" formatCode="#0"/>
     <numFmt numFmtId="167" formatCode="mmmm\ yyyy"/>
   </numFmts>
-  <fonts count="63">
+  <fonts count="64">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -4991,6 +5084,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF521BED"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -5288,7 +5388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="314">
+  <cellXfs count="315">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -6170,6 +6270,15 @@
     <xf numFmtId="0" fontId="53" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6194,14 +6303,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6516,22 +6619,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J152"/>
+  <dimension ref="A1:J153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G95" sqref="G95"/>
+      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J128" sqref="J128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.8"/>
@@ -6549,7 +6652,7 @@
     <col min="11" max="16384" width="14.44140625" style="166"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="158" customFormat="1" ht="27.6">
+    <row r="1" spans="1:10" s="158" customFormat="1" ht="28.2">
       <c r="A1" s="154" t="s">
         <v>0</v>
       </c>
@@ -6602,7 +6705,7 @@
         <v>43281</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="96.6">
+    <row r="3" spans="1:10" ht="98.7">
       <c r="A3" s="159" t="s">
         <v>1001</v>
       </c>
@@ -6723,7 +6826,7 @@
         <v>43255</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="317.39999999999998">
+    <row r="8" spans="1:10" ht="345">
       <c r="A8" s="170" t="s">
         <v>435</v>
       </c>
@@ -6744,7 +6847,7 @@
       <c r="H8" s="164"/>
       <c r="I8" s="165"/>
     </row>
-    <row r="9" spans="1:10" ht="331.2">
+    <row r="9" spans="1:10" ht="358.8">
       <c r="A9" s="173" t="s">
         <v>934</v>
       </c>
@@ -6765,7 +6868,7 @@
       <c r="H9" s="164"/>
       <c r="I9" s="165"/>
     </row>
-    <row r="10" spans="1:10" ht="409.6">
+    <row r="10" spans="1:10" ht="409.5">
       <c r="A10" s="170" t="s">
         <v>958</v>
       </c>
@@ -6951,7 +7054,7 @@
       </c>
       <c r="I17" s="165"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" ht="14.1">
       <c r="A18" s="159" t="s">
         <v>121</v>
       </c>
@@ -6999,7 +7102,7 @@
         <v>43240</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="41.4">
+    <row r="20" spans="1:9" ht="42.3">
       <c r="A20" s="159" t="s">
         <v>135</v>
       </c>
@@ -7166,7 +7269,7 @@
         <v>43196</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="27.6">
+    <row r="27" spans="1:9" ht="28.2">
       <c r="A27" s="159" t="s">
         <v>209</v>
       </c>
@@ -7212,7 +7315,7 @@
       <c r="H28" s="181"/>
       <c r="I28" s="165"/>
     </row>
-    <row r="29" spans="1:9" ht="41.4">
+    <row r="29" spans="1:9" ht="55.2">
       <c r="A29" s="159" t="s">
         <v>221</v>
       </c>
@@ -7237,7 +7340,7 @@
         <v>43196</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="41.4">
+    <row r="30" spans="1:9" ht="55.2">
       <c r="A30" s="182" t="s">
         <v>221</v>
       </c>
@@ -7258,7 +7361,7 @@
         <v>43196</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="41.4">
+    <row r="31" spans="1:9" ht="55.2">
       <c r="A31" s="182" t="s">
         <v>221</v>
       </c>
@@ -7279,7 +7382,7 @@
         <v>43196</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="41.4">
+    <row r="32" spans="1:9" ht="55.2">
       <c r="A32" s="182" t="s">
         <v>221</v>
       </c>
@@ -7485,7 +7588,7 @@
       <c r="I40" s="191"/>
       <c r="J40" s="192"/>
     </row>
-    <row r="41" spans="1:10" ht="124.2">
+    <row r="41" spans="1:10" ht="151.80000000000001">
       <c r="A41" s="159" t="s">
         <v>266</v>
       </c>
@@ -7708,7 +7811,7 @@
         <v>43250</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="69.599999999999994">
+    <row r="49" spans="1:9" ht="69.3">
       <c r="A49" s="159" t="s">
         <v>336</v>
       </c>
@@ -8043,7 +8146,7 @@
         <v>43283</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="41.4">
+    <row r="63" spans="1:9" ht="55.2">
       <c r="A63" s="182" t="s">
         <v>76</v>
       </c>
@@ -8070,7 +8173,7 @@
         <v>43284</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="41.4">
+    <row r="64" spans="1:9" ht="55.2">
       <c r="A64" s="182" t="s">
         <v>76</v>
       </c>
@@ -8097,7 +8200,7 @@
         <v>43285</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="41.4">
+    <row r="65" spans="1:9" ht="55.2">
       <c r="A65" s="182" t="s">
         <v>76</v>
       </c>
@@ -8124,7 +8227,7 @@
         <v>43287</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="41.4">
+    <row r="66" spans="1:9" ht="55.2">
       <c r="A66" s="182" t="s">
         <v>76</v>
       </c>
@@ -8201,7 +8304,7 @@
       <c r="H68" s="164"/>
       <c r="I68" s="165"/>
     </row>
-    <row r="69" spans="1:9" ht="41.4">
+    <row r="69" spans="1:9" ht="55.2">
       <c r="A69" s="182" t="s">
         <v>76</v>
       </c>
@@ -8251,7 +8354,7 @@
       <c r="H70" s="164"/>
       <c r="I70" s="165"/>
     </row>
-    <row r="71" spans="1:9" ht="41.4">
+    <row r="71" spans="1:9" ht="55.2">
       <c r="A71" s="182" t="s">
         <v>76</v>
       </c>
@@ -8301,7 +8404,7 @@
       <c r="H72" s="164"/>
       <c r="I72" s="165"/>
     </row>
-    <row r="73" spans="1:9" ht="41.4">
+    <row r="73" spans="1:9" ht="55.2">
       <c r="A73" s="182" t="s">
         <v>440</v>
       </c>
@@ -8328,7 +8431,7 @@
         <v>43289</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="55.2">
+    <row r="74" spans="1:9" ht="56.4">
       <c r="A74" s="159" t="s">
         <v>443</v>
       </c>
@@ -8355,7 +8458,7 @@
         <v>43290</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="55.2">
+    <row r="75" spans="1:9" ht="56.4">
       <c r="A75" s="203" t="s">
         <v>445</v>
       </c>
@@ -8505,7 +8608,7 @@
         <v>43264</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="55.2">
+    <row r="81" spans="1:9" ht="41.4">
       <c r="A81" s="159" t="s">
         <v>1058</v>
       </c>
@@ -8516,7 +8619,7 @@
       <c r="D81" s="161" t="s">
         <v>1059</v>
       </c>
-      <c r="E81" s="311" t="s">
+      <c r="E81" s="301" t="s">
         <v>1061</v>
       </c>
       <c r="F81" s="197" t="s">
@@ -8531,7 +8634,7 @@
       </c>
     </row>
     <row r="82" spans="1:9" ht="55.2">
-      <c r="A82" s="312" t="s">
+      <c r="A82" s="302" t="s">
         <v>1064</v>
       </c>
       <c r="B82" s="160" t="s">
@@ -8555,7 +8658,7 @@
         <v>43315</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="55.2">
+    <row r="83" spans="1:9" ht="41.4">
       <c r="A83" s="159" t="s">
         <v>1065</v>
       </c>
@@ -8580,7 +8683,7 @@
         <v>43315</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="409.6">
+    <row r="84" spans="1:9" ht="409.5">
       <c r="A84" s="159" t="s">
         <v>472</v>
       </c>
@@ -8872,7 +8975,7 @@
       <c r="E95" s="221" t="s">
         <v>1085</v>
       </c>
-      <c r="F95" s="313" t="s">
+      <c r="F95" s="303" t="s">
         <v>1083</v>
       </c>
       <c r="G95" s="164" t="s">
@@ -9150,7 +9253,7 @@
       <c r="H106" s="164"/>
       <c r="I106" s="165"/>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" ht="14.1">
       <c r="A107" s="159" t="s">
         <v>603</v>
       </c>
@@ -9304,7 +9407,7 @@
         <v>43315</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="69">
+    <row r="113" spans="1:10" ht="69">
       <c r="A113" s="159" t="s">
         <v>632</v>
       </c>
@@ -9331,7 +9434,7 @@
         <v>43240</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="69">
+    <row r="114" spans="1:10" ht="69">
       <c r="A114" s="182" t="s">
         <v>632</v>
       </c>
@@ -9354,7 +9457,7 @@
         <v>43298</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="69">
+    <row r="115" spans="1:10" ht="69">
       <c r="A115" s="182" t="s">
         <v>632</v>
       </c>
@@ -9377,7 +9480,7 @@
         <v>43298</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="55.2">
+    <row r="116" spans="1:10" ht="55.2">
       <c r="A116" s="182" t="s">
         <v>632</v>
       </c>
@@ -9400,7 +9503,7 @@
         <v>43298</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="69">
+    <row r="117" spans="1:10" ht="69">
       <c r="A117" s="182" t="s">
         <v>632</v>
       </c>
@@ -9423,7 +9526,7 @@
         <v>43298</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="69">
+    <row r="118" spans="1:10" ht="69">
       <c r="A118" s="182" t="s">
         <v>632</v>
       </c>
@@ -9446,7 +9549,7 @@
         <v>43298</v>
       </c>
     </row>
-    <row r="119" spans="1:9" ht="124.2">
+    <row r="119" spans="1:10" ht="124.2">
       <c r="A119" s="159" t="s">
         <v>646</v>
       </c>
@@ -9469,7 +9572,7 @@
       <c r="H119" s="164"/>
       <c r="I119" s="165"/>
     </row>
-    <row r="120" spans="1:9" ht="138">
+    <row r="120" spans="1:10" ht="138">
       <c r="A120" s="182" t="s">
         <v>646</v>
       </c>
@@ -9492,7 +9595,7 @@
       <c r="H120" s="164"/>
       <c r="I120" s="165"/>
     </row>
-    <row r="121" spans="1:9" ht="124.2">
+    <row r="121" spans="1:10" ht="124.2">
       <c r="A121" s="182" t="s">
         <v>646</v>
       </c>
@@ -9515,7 +9618,7 @@
       <c r="H121" s="164"/>
       <c r="I121" s="165"/>
     </row>
-    <row r="122" spans="1:9" ht="82.8">
+    <row r="122" spans="1:10" ht="96.6">
       <c r="A122" s="159" t="s">
         <v>660</v>
       </c>
@@ -9540,7 +9643,7 @@
         <v>43196</v>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="41.4">
+    <row r="123" spans="1:10" ht="41.4">
       <c r="A123" s="159" t="s">
         <v>675</v>
       </c>
@@ -9563,7 +9666,7 @@
         <v>43276</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="41.4">
+    <row r="124" spans="1:10" ht="41.4">
       <c r="A124" s="159" t="s">
         <v>675</v>
       </c>
@@ -9586,7 +9689,7 @@
         <v>43276</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="55.2">
+    <row r="125" spans="1:10" ht="55.2">
       <c r="A125" s="159" t="s">
         <v>694</v>
       </c>
@@ -9611,7 +9714,7 @@
         <v>43293</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="207">
+    <row r="126" spans="1:10" ht="207">
       <c r="A126" s="159" t="s">
         <v>702</v>
       </c>
@@ -9636,7 +9739,7 @@
         <v>43240</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="69">
+    <row r="127" spans="1:10" ht="69">
       <c r="A127" s="159" t="s">
         <v>710</v>
       </c>
@@ -9664,8 +9767,11 @@
       <c r="I127" s="165">
         <v>43196</v>
       </c>
-    </row>
-    <row r="128" spans="1:9" ht="82.8">
+      <c r="J127" s="166" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" ht="82.8">
       <c r="A128" s="159" t="s">
         <v>710</v>
       </c>
@@ -9689,8 +9795,11 @@
       <c r="I128" s="165">
         <v>43196</v>
       </c>
-    </row>
-    <row r="129" spans="1:9" ht="41.4">
+      <c r="J128" s="181" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" ht="55.2">
       <c r="A129" s="182" t="s">
         <v>710</v>
       </c>
@@ -9714,226 +9823,225 @@
       <c r="I129" s="165">
         <v>43196</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" ht="27.6">
-      <c r="A130" s="159" t="s">
-        <v>737</v>
-      </c>
-      <c r="B130" s="164" t="s">
-        <v>142</v>
-      </c>
-      <c r="C130" s="164" t="s">
-        <v>22</v>
-      </c>
-      <c r="D130" s="183" t="s">
-        <v>738</v>
-      </c>
-      <c r="E130" s="207" t="s">
-        <v>750</v>
-      </c>
-      <c r="F130" s="187" t="s">
-        <v>760</v>
-      </c>
-      <c r="G130" s="164" t="s">
-        <v>761</v>
-      </c>
+      <c r="J129" s="166" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" ht="86.4">
+      <c r="A130" s="182" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B130" s="180" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C130" s="180"/>
+      <c r="D130" s="314" t="s">
+        <v>1088</v>
+      </c>
+      <c r="E130" s="168" t="s">
+        <v>1089</v>
+      </c>
+      <c r="F130" s="185" t="s">
+        <v>1090</v>
+      </c>
+      <c r="G130" s="163"/>
       <c r="H130" s="164"/>
-      <c r="I130" s="165">
-        <v>43250</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" ht="27.6">
-      <c r="A131" s="182" t="s">
+      <c r="I130" s="165" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" ht="41.4">
+      <c r="A131" s="159" t="s">
         <v>737</v>
       </c>
       <c r="B131" s="164" t="s">
         <v>142</v>
       </c>
-      <c r="C131" s="164"/>
-      <c r="D131" s="299" t="s">
-        <v>876</v>
-      </c>
-      <c r="E131" s="160" t="s">
-        <v>879</v>
+      <c r="C131" s="164" t="s">
+        <v>22</v>
+      </c>
+      <c r="D131" s="183" t="s">
+        <v>738</v>
+      </c>
+      <c r="E131" s="207" t="s">
+        <v>750</v>
       </c>
       <c r="F131" s="187" t="s">
-        <v>1041</v>
-      </c>
-      <c r="G131" s="164"/>
+        <v>760</v>
+      </c>
+      <c r="G131" s="164" t="s">
+        <v>761</v>
+      </c>
       <c r="H131" s="164"/>
       <c r="I131" s="165">
+        <v>43250</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" ht="27.6">
+      <c r="A132" s="182" t="s">
+        <v>737</v>
+      </c>
+      <c r="B132" s="164" t="s">
+        <v>142</v>
+      </c>
+      <c r="C132" s="164"/>
+      <c r="D132" s="299" t="s">
+        <v>876</v>
+      </c>
+      <c r="E132" s="160" t="s">
+        <v>879</v>
+      </c>
+      <c r="F132" s="187" t="s">
+        <v>1041</v>
+      </c>
+      <c r="G132" s="164"/>
+      <c r="H132" s="164"/>
+      <c r="I132" s="165">
         <v>43311</v>
       </c>
     </row>
-    <row r="132" spans="1:9" ht="96.6">
-      <c r="A132" s="159" t="s">
+    <row r="133" spans="1:10" ht="96.6">
+      <c r="A133" s="159" t="s">
         <v>762</v>
       </c>
-      <c r="B132" s="164" t="s">
+      <c r="B133" s="164" t="s">
         <v>763</v>
       </c>
-      <c r="C132" s="164" t="s">
+      <c r="C133" s="164" t="s">
         <v>22</v>
       </c>
-      <c r="D132" s="186" t="s">
+      <c r="D133" s="186" t="s">
         <v>764</v>
       </c>
-      <c r="E132" s="207" t="s">
+      <c r="E133" s="207" t="s">
         <v>598</v>
       </c>
-      <c r="F132" s="185" t="s">
+      <c r="F133" s="185" t="s">
         <v>995</v>
       </c>
-      <c r="G132" s="164" t="s">
+      <c r="G133" s="164" t="s">
         <v>996</v>
       </c>
-      <c r="H132" s="208"/>
-      <c r="I132" s="165">
+      <c r="H133" s="208"/>
+      <c r="I133" s="165">
         <v>43264</v>
       </c>
     </row>
-    <row r="133" spans="1:9" ht="27.6">
-      <c r="A133" s="182" t="s">
+    <row r="134" spans="1:10" ht="41.4">
+      <c r="A134" s="182" t="s">
         <v>796</v>
       </c>
-      <c r="B133" s="164" t="s">
+      <c r="B134" s="164" t="s">
         <v>797</v>
       </c>
-      <c r="C133" s="160" t="s">
+      <c r="C134" s="160" t="s">
         <v>798</v>
       </c>
-      <c r="D133" s="160" t="s">
+      <c r="D134" s="160" t="s">
         <v>800</v>
       </c>
-      <c r="E133" s="168" t="s">
+      <c r="E134" s="168" t="s">
         <v>805</v>
       </c>
-      <c r="F133" s="185" t="s">
+      <c r="F134" s="185" t="s">
         <v>806</v>
       </c>
-      <c r="G133" s="164" t="s">
+      <c r="G134" s="164" t="s">
         <v>807</v>
       </c>
-      <c r="H133" s="208"/>
-      <c r="I133" s="165"/>
-    </row>
-    <row r="134" spans="1:9">
-      <c r="A134" s="159" t="s">
+      <c r="H134" s="208"/>
+      <c r="I134" s="165"/>
+    </row>
+    <row r="135" spans="1:10" ht="14.1">
+      <c r="A135" s="159" t="s">
         <v>808</v>
-      </c>
-      <c r="B134" s="164" t="s">
-        <v>45</v>
-      </c>
-      <c r="C134" s="160" t="s">
-        <v>809</v>
-      </c>
-      <c r="D134" s="186" t="s">
-        <v>810</v>
-      </c>
-      <c r="E134" s="162" t="s">
-        <v>598</v>
-      </c>
-      <c r="F134" s="187" t="s">
-        <v>822</v>
-      </c>
-      <c r="G134" s="164"/>
-      <c r="H134" s="164"/>
-      <c r="I134" s="165">
-        <v>43240</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" ht="96.6">
-      <c r="A135" s="159" t="s">
-        <v>828</v>
       </c>
       <c r="B135" s="164" t="s">
         <v>45</v>
       </c>
-      <c r="C135" s="164" t="s">
-        <v>22</v>
-      </c>
-      <c r="D135" s="164" t="s">
-        <v>829</v>
-      </c>
-      <c r="E135" s="162"/>
+      <c r="C135" s="160" t="s">
+        <v>809</v>
+      </c>
+      <c r="D135" s="186" t="s">
+        <v>810</v>
+      </c>
+      <c r="E135" s="162" t="s">
+        <v>598</v>
+      </c>
       <c r="F135" s="187" t="s">
-        <v>835</v>
-      </c>
-      <c r="G135" s="166" t="s">
-        <v>957</v>
-      </c>
+        <v>822</v>
+      </c>
+      <c r="G135" s="164"/>
       <c r="H135" s="164"/>
       <c r="I135" s="165">
         <v>43240</v>
       </c>
     </row>
-    <row r="136" spans="1:9" ht="41.4">
-      <c r="A136" s="170" t="s">
+    <row r="136" spans="1:10" ht="96.6">
+      <c r="A136" s="159" t="s">
+        <v>828</v>
+      </c>
+      <c r="B136" s="164" t="s">
+        <v>45</v>
+      </c>
+      <c r="C136" s="164" t="s">
+        <v>22</v>
+      </c>
+      <c r="D136" s="164" t="s">
+        <v>829</v>
+      </c>
+      <c r="E136" s="162"/>
+      <c r="F136" s="187" t="s">
+        <v>835</v>
+      </c>
+      <c r="G136" s="166" t="s">
+        <v>957</v>
+      </c>
+      <c r="H136" s="164"/>
+      <c r="I136" s="165">
+        <v>43240</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" ht="41.4">
+      <c r="A137" s="170" t="s">
         <v>836</v>
       </c>
-      <c r="D136" s="297">
+      <c r="D137" s="297">
         <v>2420287</v>
       </c>
-      <c r="F136" s="166" t="s">
+      <c r="F137" s="166" t="s">
         <v>1040</v>
       </c>
-      <c r="I136" s="298">
+      <c r="I137" s="298">
         <v>372000</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="41.4">
-      <c r="A137" s="159" t="s">
+    <row r="138" spans="1:10" ht="41.4">
+      <c r="A138" s="159" t="s">
         <v>843</v>
       </c>
-      <c r="B137" s="160" t="s">
+      <c r="B138" s="160" t="s">
         <v>289</v>
       </c>
-      <c r="C137" s="160"/>
-      <c r="D137" s="195" t="s">
+      <c r="C138" s="160"/>
+      <c r="D138" s="195" t="s">
         <v>845</v>
       </c>
-      <c r="E137" s="168" t="s">
+      <c r="E138" s="168" t="s">
         <v>846</v>
       </c>
-      <c r="F137" s="163" t="s">
+      <c r="F138" s="163" t="s">
         <v>847</v>
       </c>
-      <c r="G137" s="164" t="s">
+      <c r="G138" s="164" t="s">
         <v>855</v>
       </c>
-      <c r="H137" s="164"/>
-      <c r="I137" s="165">
+      <c r="H138" s="164"/>
+      <c r="I138" s="165">
         <v>43288</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="138">
-      <c r="A138" s="159" t="s">
-        <v>857</v>
-      </c>
-      <c r="B138" s="160" t="s">
-        <v>77</v>
-      </c>
-      <c r="C138" s="160" t="s">
-        <v>22</v>
-      </c>
-      <c r="D138" s="161" t="s">
-        <v>858</v>
-      </c>
-      <c r="E138" s="168"/>
-      <c r="F138" s="179" t="s">
-        <v>859</v>
-      </c>
-      <c r="G138" s="164" t="s">
-        <v>860</v>
-      </c>
-      <c r="H138" s="209" t="s">
-        <v>962</v>
-      </c>
-      <c r="I138" s="165">
-        <v>43270</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9" ht="41.4">
+    <row r="139" spans="1:10" ht="138">
       <c r="A139" s="159" t="s">
         <v>857</v>
       </c>
@@ -9944,23 +10052,23 @@
         <v>22</v>
       </c>
       <c r="D139" s="161" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="E139" s="168"/>
       <c r="F139" s="179" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="G139" s="164" t="s">
-        <v>863</v>
-      </c>
-      <c r="H139" s="181" t="s">
-        <v>963</v>
+        <v>860</v>
+      </c>
+      <c r="H139" s="209" t="s">
+        <v>962</v>
       </c>
       <c r="I139" s="165">
         <v>43270</v>
       </c>
     </row>
-    <row r="140" spans="1:9" ht="41.4">
+    <row r="140" spans="1:10" ht="41.4">
       <c r="A140" s="159" t="s">
         <v>857</v>
       </c>
@@ -9971,11 +10079,11 @@
         <v>22</v>
       </c>
       <c r="D140" s="161" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="E140" s="168"/>
       <c r="F140" s="179" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
       <c r="G140" s="164" t="s">
         <v>863</v>
@@ -9987,7 +10095,7 @@
         <v>43270</v>
       </c>
     </row>
-    <row r="141" spans="1:9" ht="41.4">
+    <row r="141" spans="1:10" ht="41.4">
       <c r="A141" s="159" t="s">
         <v>857</v>
       </c>
@@ -9998,87 +10106,103 @@
         <v>22</v>
       </c>
       <c r="D141" s="161" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="E141" s="168"/>
-      <c r="F141" s="197" t="s">
-        <v>867</v>
-      </c>
-      <c r="G141" s="164"/>
-      <c r="H141" s="209" t="s">
-        <v>962</v>
+      <c r="F141" s="179" t="s">
+        <v>865</v>
+      </c>
+      <c r="G141" s="164" t="s">
+        <v>863</v>
+      </c>
+      <c r="H141" s="181" t="s">
+        <v>963</v>
       </c>
       <c r="I141" s="165">
         <v>43270</v>
       </c>
     </row>
-    <row r="142" spans="1:9" ht="41.4">
+    <row r="142" spans="1:10" ht="55.2">
       <c r="A142" s="159" t="s">
+        <v>857</v>
+      </c>
+      <c r="B142" s="160" t="s">
+        <v>77</v>
+      </c>
+      <c r="C142" s="160" t="s">
+        <v>22</v>
+      </c>
+      <c r="D142" s="161" t="s">
+        <v>866</v>
+      </c>
+      <c r="E142" s="168"/>
+      <c r="F142" s="197" t="s">
+        <v>867</v>
+      </c>
+      <c r="G142" s="164"/>
+      <c r="H142" s="209" t="s">
+        <v>962</v>
+      </c>
+      <c r="I142" s="165">
+        <v>43270</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" ht="41.4">
+      <c r="A143" s="159" t="s">
         <v>868</v>
       </c>
-      <c r="B142" s="164" t="s">
+      <c r="B143" s="164" t="s">
         <v>142</v>
-      </c>
-      <c r="C142" s="164" t="s">
-        <v>22</v>
-      </c>
-      <c r="D142" s="183" t="s">
-        <v>869</v>
-      </c>
-      <c r="E142" s="210" t="s">
-        <v>870</v>
-      </c>
-      <c r="F142" s="187" t="s">
-        <v>760</v>
-      </c>
-      <c r="G142" s="164" t="s">
-        <v>877</v>
-      </c>
-      <c r="H142" s="209" t="s">
-        <v>964</v>
-      </c>
-      <c r="I142" s="165">
-        <v>43250</v>
-      </c>
-    </row>
-    <row r="143" spans="1:9" ht="27.6">
-      <c r="A143" s="159" t="s">
-        <v>878</v>
-      </c>
-      <c r="B143" s="164" t="s">
-        <v>763</v>
       </c>
       <c r="C143" s="164" t="s">
         <v>22</v>
       </c>
-      <c r="D143" s="186" t="s">
+      <c r="D143" s="183" t="s">
+        <v>869</v>
+      </c>
+      <c r="E143" s="210" t="s">
+        <v>870</v>
+      </c>
+      <c r="F143" s="187" t="s">
+        <v>760</v>
+      </c>
+      <c r="G143" s="164" t="s">
+        <v>877</v>
+      </c>
+      <c r="H143" s="209" t="s">
+        <v>964</v>
+      </c>
+      <c r="I143" s="165">
+        <v>43250</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" ht="27.6">
+      <c r="A144" s="159" t="s">
+        <v>878</v>
+      </c>
+      <c r="B144" s="164" t="s">
+        <v>763</v>
+      </c>
+      <c r="C144" s="164" t="s">
+        <v>22</v>
+      </c>
+      <c r="D144" s="186" t="s">
         <v>883</v>
       </c>
-      <c r="F143" s="187" t="s">
+      <c r="F144" s="187" t="s">
         <v>894</v>
       </c>
-      <c r="H143" s="209" t="s">
+      <c r="H144" s="209" t="s">
         <v>962</v>
       </c>
-      <c r="I143" s="211">
+      <c r="I144" s="211">
         <v>43288</v>
       </c>
     </row>
-    <row r="144" spans="1:9">
-      <c r="D144" s="164"/>
-    </row>
     <row r="145" spans="1:9">
-      <c r="A145" s="159"/>
-      <c r="B145" s="160"/>
-      <c r="C145" s="160"/>
-      <c r="D145" s="160"/>
-      <c r="E145" s="168"/>
-      <c r="F145" s="199"/>
-      <c r="G145" s="164"/>
-      <c r="H145" s="164"/>
-      <c r="I145" s="165"/>
-    </row>
-    <row r="146" spans="1:9">
+      <c r="D145" s="164"/>
+    </row>
+    <row r="146" spans="1:9" ht="14.1">
       <c r="A146" s="159"/>
       <c r="B146" s="160"/>
       <c r="C146" s="160"/>
@@ -10089,7 +10213,7 @@
       <c r="H146" s="164"/>
       <c r="I146" s="165"/>
     </row>
-    <row r="147" spans="1:9">
+    <row r="147" spans="1:9" ht="14.1">
       <c r="A147" s="159"/>
       <c r="B147" s="160"/>
       <c r="C147" s="160"/>
@@ -10100,7 +10224,7 @@
       <c r="H147" s="164"/>
       <c r="I147" s="165"/>
     </row>
-    <row r="148" spans="1:9">
+    <row r="148" spans="1:9" ht="14.1">
       <c r="A148" s="159"/>
       <c r="B148" s="160"/>
       <c r="C148" s="160"/>
@@ -10111,7 +10235,7 @@
       <c r="H148" s="164"/>
       <c r="I148" s="165"/>
     </row>
-    <row r="149" spans="1:9">
+    <row r="149" spans="1:9" ht="14.1">
       <c r="A149" s="159"/>
       <c r="B149" s="160"/>
       <c r="C149" s="160"/>
@@ -10122,7 +10246,7 @@
       <c r="H149" s="164"/>
       <c r="I149" s="165"/>
     </row>
-    <row r="150" spans="1:9">
+    <row r="150" spans="1:9" ht="14.1">
       <c r="A150" s="159"/>
       <c r="B150" s="160"/>
       <c r="C150" s="160"/>
@@ -10133,7 +10257,7 @@
       <c r="H150" s="164"/>
       <c r="I150" s="165"/>
     </row>
-    <row r="151" spans="1:9">
+    <row r="151" spans="1:9" ht="14.1">
       <c r="A151" s="159"/>
       <c r="B151" s="160"/>
       <c r="C151" s="160"/>
@@ -10144,7 +10268,7 @@
       <c r="H151" s="164"/>
       <c r="I151" s="165"/>
     </row>
-    <row r="152" spans="1:9">
+    <row r="152" spans="1:9" ht="14.1">
       <c r="A152" s="159"/>
       <c r="B152" s="160"/>
       <c r="C152" s="160"/>
@@ -10155,9 +10279,20 @@
       <c r="H152" s="164"/>
       <c r="I152" s="165"/>
     </row>
+    <row r="153" spans="1:9" ht="14.1">
+      <c r="A153" s="159"/>
+      <c r="B153" s="160"/>
+      <c r="C153" s="160"/>
+      <c r="D153" s="160"/>
+      <c r="E153" s="168"/>
+      <c r="F153" s="199"/>
+      <c r="G153" s="164"/>
+      <c r="H153" s="164"/>
+      <c r="I153" s="165"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F122" r:id="rId1" location="gid=314589613&amp;range=309:309"/>
+    <hyperlink ref="F122" r:id="rId1" location="gid=314589613&amp;range=309:309" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -10166,7 +10301,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -10177,7 +10312,7 @@
       <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="12.3"/>
   <cols>
     <col min="1" max="1" width="18.109375" style="232" customWidth="1"/>
     <col min="2" max="5" width="14.44140625" style="232"/>
@@ -10189,7 +10324,7 @@
     <col min="11" max="16384" width="14.44140625" style="232"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="272" customFormat="1" ht="26.4">
+    <row r="1" spans="1:10" s="272" customFormat="1" ht="24.6">
       <c r="A1" s="270" t="s">
         <v>0</v>
       </c>
@@ -10214,12 +10349,12 @@
       <c r="H1" s="270" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="301" t="s">
+      <c r="I1" s="304" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="302"/>
-    </row>
-    <row r="2" spans="1:10" s="276" customFormat="1" ht="26.4">
+      <c r="J1" s="305"/>
+    </row>
+    <row r="2" spans="1:10" s="276" customFormat="1" ht="24.6">
       <c r="A2" s="273"/>
       <c r="B2" s="274"/>
       <c r="C2" s="274"/>
@@ -10235,7 +10370,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="286" customFormat="1" ht="66">
+    <row r="3" spans="1:10" s="286" customFormat="1" ht="61.5">
       <c r="A3" s="277" t="s">
         <v>60</v>
       </c>
@@ -10265,7 +10400,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="92.4">
+    <row r="4" spans="1:10" ht="86.1">
       <c r="A4" s="233" t="s">
         <v>19</v>
       </c>
@@ -10295,7 +10430,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="105.6">
+    <row r="5" spans="1:10" ht="98.4">
       <c r="A5" s="233" t="s">
         <v>19</v>
       </c>
@@ -10325,7 +10460,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="105.6">
+    <row r="6" spans="1:10" ht="98.4">
       <c r="A6" s="233" t="s">
         <v>19</v>
       </c>
@@ -10355,7 +10490,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="105.6">
+    <row r="7" spans="1:10" ht="98.4">
       <c r="A7" s="233" t="s">
         <v>19</v>
       </c>
@@ -10415,7 +10550,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="92.4">
+    <row r="9" spans="1:10" ht="73.8">
       <c r="A9" s="229" t="s">
         <v>44</v>
       </c>
@@ -10443,7 +10578,7 @@
       </c>
       <c r="J9" s="231"/>
     </row>
-    <row r="10" spans="1:10" ht="92.4">
+    <row r="10" spans="1:10" ht="73.8">
       <c r="A10" s="226" t="s">
         <v>44</v>
       </c>
@@ -10471,7 +10606,7 @@
       </c>
       <c r="J10" s="231"/>
     </row>
-    <row r="11" spans="1:10" ht="92.4">
+    <row r="11" spans="1:10" ht="73.8">
       <c r="A11" s="226" t="s">
         <v>44</v>
       </c>
@@ -10499,7 +10634,7 @@
       </c>
       <c r="J11" s="231"/>
     </row>
-    <row r="12" spans="1:10" ht="118.8">
+    <row r="12" spans="1:10" ht="98.4">
       <c r="A12" s="226" t="s">
         <v>193</v>
       </c>
@@ -10525,7 +10660,7 @@
       </c>
       <c r="J12" s="231"/>
     </row>
-    <row r="13" spans="1:10" ht="250.8">
+    <row r="13" spans="1:10" ht="233.7">
       <c r="A13" s="229" t="s">
         <v>217</v>
       </c>
@@ -10556,7 +10691,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="165.6">
+    <row r="14" spans="1:10" ht="160.19999999999999">
       <c r="A14" s="162" t="s">
         <v>282</v>
       </c>
@@ -10584,7 +10719,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="79.2">
+    <row r="15" spans="1:10" ht="73.8">
       <c r="A15" s="226" t="s">
         <v>76</v>
       </c>
@@ -10636,7 +10771,7 @@
       </c>
       <c r="J16" s="231"/>
     </row>
-    <row r="17" spans="1:10" ht="55.2">
+    <row r="17" spans="1:10" ht="51.6">
       <c r="A17" s="226" t="s">
         <v>76</v>
       </c>
@@ -10662,7 +10797,7 @@
       <c r="I17" s="230"/>
       <c r="J17" s="231"/>
     </row>
-    <row r="18" spans="1:10" ht="55.2">
+    <row r="18" spans="1:10" ht="51.6">
       <c r="A18" s="226" t="s">
         <v>76</v>
       </c>
@@ -10688,7 +10823,7 @@
       <c r="I18" s="230"/>
       <c r="J18" s="231"/>
     </row>
-    <row r="19" spans="1:10" s="267" customFormat="1" ht="39.6">
+    <row r="19" spans="1:10" s="267" customFormat="1" ht="36.9">
       <c r="A19" s="295" t="s">
         <v>589</v>
       </c>
@@ -10713,7 +10848,7 @@
         <v>43240</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="267" customFormat="1" ht="66">
+    <row r="20" spans="1:10" s="267" customFormat="1" ht="61.5">
       <c r="A20" s="263" t="s">
         <v>632</v>
       </c>
@@ -10768,7 +10903,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="79.2">
+    <row r="22" spans="1:10" ht="73.8">
       <c r="A22" s="263" t="s">
         <v>737</v>
       </c>
@@ -10800,7 +10935,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="267" customFormat="1" ht="79.2">
+    <row r="23" spans="1:10" s="267" customFormat="1" ht="61.5">
       <c r="A23" s="295" t="s">
         <v>766</v>
       </c>
@@ -10826,7 +10961,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="267" customFormat="1" ht="79.2">
+    <row r="24" spans="1:10" s="267" customFormat="1" ht="61.5">
       <c r="A24" s="295" t="s">
         <v>766</v>
       </c>
@@ -10852,7 +10987,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="267" customFormat="1" ht="79.2">
+    <row r="25" spans="1:10" s="267" customFormat="1" ht="61.5">
       <c r="A25" s="295" t="s">
         <v>766</v>
       </c>
@@ -10910,7 +11045,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -10923,7 +11058,7 @@
       <selection pane="bottomRight" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="12.3"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
@@ -10936,7 +11071,7 @@
     <col min="10" max="10" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="26.4">
+    <row r="1" spans="1:10" ht="24.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10961,12 +11096,12 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="305" t="s">
+      <c r="I1" s="308" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="304"/>
-    </row>
-    <row r="2" spans="1:10" ht="26.4">
+      <c r="J1" s="307"/>
+    </row>
+    <row r="2" spans="1:10" ht="24.6">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -10982,7 +11117,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="52.8">
+    <row r="3" spans="1:10" ht="49.2">
       <c r="A3" s="6" t="s">
         <v>11</v>
       </c>
@@ -11008,7 +11143,7 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="26.4">
+    <row r="4" spans="1:10" ht="24.6">
       <c r="A4" s="17" t="s">
         <v>24</v>
       </c>
@@ -11035,13 +11170,13 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="86.4">
-      <c r="A5" s="308" t="s">
+      <c r="A5" s="311" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="303" t="s">
+      <c r="B5" s="306" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="303" t="s">
+      <c r="C5" s="306" t="s">
         <v>42</v>
       </c>
       <c r="D5" s="13" t="s">
@@ -11063,9 +11198,9 @@
       <c r="J5" s="32"/>
     </row>
     <row r="6" spans="1:10" ht="86.4">
-      <c r="A6" s="304"/>
-      <c r="B6" s="304"/>
-      <c r="C6" s="304"/>
+      <c r="A6" s="307"/>
+      <c r="B6" s="307"/>
+      <c r="C6" s="307"/>
       <c r="D6" s="13" t="s">
         <v>68</v>
       </c>
@@ -11082,8 +11217,8 @@
       </c>
       <c r="J6" s="35"/>
     </row>
-    <row r="7" spans="1:10" ht="39.6">
-      <c r="A7" s="308" t="s">
+    <row r="7" spans="1:10" ht="36.9">
+      <c r="A7" s="311" t="s">
         <v>79</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -11112,8 +11247,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="39.6">
-      <c r="A8" s="304"/>
+    <row r="8" spans="1:10" ht="36.9">
+      <c r="A8" s="307"/>
       <c r="B8" s="8" t="s">
         <v>21</v>
       </c>
@@ -11139,8 +11274,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="39.6">
-      <c r="A9" s="307"/>
+    <row r="9" spans="1:10" ht="36.9">
+      <c r="A9" s="310"/>
       <c r="B9" s="41" t="s">
         <v>21</v>
       </c>
@@ -11191,8 +11326,8 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="39.6">
-      <c r="A11" s="309" t="s">
+    <row r="11" spans="1:10" ht="36.9">
+      <c r="A11" s="312" t="s">
         <v>117</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -11220,8 +11355,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="39.6">
-      <c r="A12" s="304"/>
+    <row r="12" spans="1:10" ht="36.9">
+      <c r="A12" s="307"/>
       <c r="B12" s="8" t="s">
         <v>21</v>
       </c>
@@ -11247,8 +11382,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="39.6">
-      <c r="A13" s="304"/>
+    <row r="13" spans="1:10" ht="24.6">
+      <c r="A13" s="307"/>
       <c r="B13" s="8" t="s">
         <v>21</v>
       </c>
@@ -11274,8 +11409,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="39.6">
-      <c r="A14" s="304"/>
+    <row r="14" spans="1:10" ht="36.9">
+      <c r="A14" s="307"/>
       <c r="B14" s="41" t="s">
         <v>21</v>
       </c>
@@ -11302,7 +11437,7 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="232" customFormat="1" ht="118.8">
+    <row r="15" spans="1:10" s="232" customFormat="1" ht="98.4">
       <c r="A15" s="225" t="s">
         <v>148</v>
       </c>
@@ -11334,7 +11469,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="26.4">
+    <row r="16" spans="1:10" ht="24.6">
       <c r="A16" s="6" t="s">
         <v>155</v>
       </c>
@@ -11360,7 +11495,7 @@
       </c>
       <c r="J16" s="35"/>
     </row>
-    <row r="17" spans="1:10" ht="26.4">
+    <row r="17" spans="1:10" ht="24.6">
       <c r="A17" s="6" t="s">
         <v>163</v>
       </c>
@@ -11386,7 +11521,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="105.6">
+    <row r="23" spans="1:10" ht="98.4">
       <c r="A23" s="14" t="s">
         <v>19</v>
       </c>
@@ -11416,7 +11551,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="79.2">
+    <row r="27" spans="1:10" ht="73.8">
       <c r="A27" s="6" t="s">
         <v>173</v>
       </c>
@@ -11446,7 +11581,7 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="52.8">
+    <row r="28" spans="1:10" ht="36.9">
       <c r="A28" s="59" t="s">
         <v>184</v>
       </c>
@@ -11478,7 +11613,7 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="92.4">
+    <row r="29" spans="1:10" ht="86.1">
       <c r="A29" s="6" t="s">
         <v>253</v>
       </c>
@@ -11508,7 +11643,7 @@
         <v>76138</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="66">
+    <row r="30" spans="1:10" ht="61.5">
       <c r="A30" s="6" t="s">
         <v>263</v>
       </c>
@@ -11534,7 +11669,7 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="232" customFormat="1" ht="92.4">
+    <row r="31" spans="1:10" s="232" customFormat="1" ht="86.1">
       <c r="A31" s="229" t="s">
         <v>282</v>
       </c>
@@ -11610,7 +11745,7 @@
       <c r="I33" s="12"/>
       <c r="J33" s="35"/>
     </row>
-    <row r="34" spans="1:10" ht="79.2">
+    <row r="34" spans="1:10" ht="73.8">
       <c r="A34" s="6" t="s">
         <v>314</v>
       </c>
@@ -11640,7 +11775,7 @@
       </c>
       <c r="J34" s="35"/>
     </row>
-    <row r="35" spans="1:10" ht="92.4">
+    <row r="35" spans="1:10" ht="86.1">
       <c r="A35" s="74" t="s">
         <v>339</v>
       </c>
@@ -11702,7 +11837,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="267" customFormat="1" ht="66">
+    <row r="37" spans="1:10" s="267" customFormat="1" ht="61.5">
       <c r="A37" s="263" t="s">
         <v>321</v>
       </c>
@@ -11732,7 +11867,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="267" customFormat="1" ht="66">
+    <row r="38" spans="1:10" s="267" customFormat="1" ht="61.5">
       <c r="A38" s="263" t="s">
         <v>321</v>
       </c>
@@ -11762,7 +11897,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="39.6">
+    <row r="39" spans="1:10" ht="36.9">
       <c r="A39" s="6" t="s">
         <v>348</v>
       </c>
@@ -11790,7 +11925,7 @@
       </c>
       <c r="J39" s="32"/>
     </row>
-    <row r="40" spans="1:10" ht="66">
+    <row r="40" spans="1:10" ht="61.5">
       <c r="A40" s="6" t="s">
         <v>355</v>
       </c>
@@ -11822,8 +11957,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="39.6">
-      <c r="A41" s="306" t="s">
+    <row r="41" spans="1:10" ht="36.9">
+      <c r="A41" s="309" t="s">
         <v>368</v>
       </c>
       <c r="B41" s="77" t="s">
@@ -11852,8 +11987,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="39.6">
-      <c r="A42" s="304"/>
+    <row r="42" spans="1:10" ht="36.9">
+      <c r="A42" s="307"/>
       <c r="B42" s="8" t="s">
         <v>21</v>
       </c>
@@ -11880,8 +12015,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="66">
-      <c r="A43" s="304"/>
+    <row r="43" spans="1:10" ht="61.5">
+      <c r="A43" s="307"/>
       <c r="B43" s="8" t="s">
         <v>21</v>
       </c>
@@ -11908,8 +12043,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="39.6">
-      <c r="A44" s="304"/>
+    <row r="44" spans="1:10" ht="36.9">
+      <c r="A44" s="307"/>
       <c r="B44" s="8" t="s">
         <v>21</v>
       </c>
@@ -11936,8 +12071,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="39.6">
-      <c r="A45" s="304"/>
+    <row r="45" spans="1:10" ht="36.9">
+      <c r="A45" s="307"/>
       <c r="B45" s="8" t="s">
         <v>21</v>
       </c>
@@ -11964,8 +12099,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="39.6">
-      <c r="A46" s="304"/>
+    <row r="46" spans="1:10" ht="36.9">
+      <c r="A46" s="307"/>
       <c r="B46" s="8" t="s">
         <v>21</v>
       </c>
@@ -11992,8 +12127,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="39.6">
-      <c r="A47" s="304"/>
+    <row r="47" spans="1:10" ht="36.9">
+      <c r="A47" s="307"/>
       <c r="B47" s="8" t="s">
         <v>21</v>
       </c>
@@ -12020,8 +12155,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="39.6">
-      <c r="A48" s="304"/>
+    <row r="48" spans="1:10" ht="36.9">
+      <c r="A48" s="307"/>
       <c r="B48" s="8" t="s">
         <v>21</v>
       </c>
@@ -12048,8 +12183,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="39.6">
-      <c r="A49" s="304"/>
+    <row r="49" spans="1:10" ht="36.9">
+      <c r="A49" s="307"/>
       <c r="B49" s="8" t="s">
         <v>21</v>
       </c>
@@ -12076,8 +12211,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="39.6">
-      <c r="A50" s="307"/>
+    <row r="50" spans="1:10" ht="36.9">
+      <c r="A50" s="310"/>
       <c r="B50" s="41" t="s">
         <v>21</v>
       </c>
@@ -12104,7 +12239,7 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="39.6">
+    <row r="51" spans="1:10" ht="36.9">
       <c r="A51" s="92" t="s">
         <v>451</v>
       </c>
@@ -12164,8 +12299,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="66">
-      <c r="A53" s="306" t="s">
+    <row r="53" spans="1:10" ht="61.5">
+      <c r="A53" s="309" t="s">
         <v>487</v>
       </c>
       <c r="B53" s="77" t="s">
@@ -12194,8 +12329,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="39.6">
-      <c r="A54" s="307"/>
+    <row r="54" spans="1:10" ht="36.9">
+      <c r="A54" s="310"/>
       <c r="B54" s="41" t="s">
         <v>21</v>
       </c>
@@ -12250,7 +12385,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="26.4">
+    <row r="56" spans="1:10" ht="24.6">
       <c r="A56" s="8" t="s">
         <v>452</v>
       </c>
@@ -12276,7 +12411,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="79.2">
+    <row r="57" spans="1:10" ht="73.8">
       <c r="A57" s="6" t="s">
         <v>539</v>
       </c>
@@ -12308,7 +12443,7 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="52.8">
+    <row r="58" spans="1:10" ht="49.2">
       <c r="A58" s="8" t="s">
         <v>539</v>
       </c>
@@ -12340,7 +12475,7 @@
         <v>43283</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="52.8">
+    <row r="59" spans="1:10" ht="49.2">
       <c r="A59" s="8" t="s">
         <v>539</v>
       </c>
@@ -12372,7 +12507,7 @@
         <v>43284</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="52.8">
+    <row r="60" spans="1:10" ht="49.2">
       <c r="A60" s="8" t="s">
         <v>539</v>
       </c>
@@ -12404,7 +12539,7 @@
         <v>43285</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="66">
+    <row r="61" spans="1:10" ht="61.5">
       <c r="A61" s="8" t="s">
         <v>539</v>
       </c>
@@ -12436,7 +12571,7 @@
         <v>43286</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="52.8">
+    <row r="62" spans="1:10" ht="49.2">
       <c r="A62" s="8" t="s">
         <v>539</v>
       </c>
@@ -12468,7 +12603,7 @@
         <v>43287</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="52.8">
+    <row r="63" spans="1:10" ht="49.2">
       <c r="A63" s="8" t="s">
         <v>539</v>
       </c>
@@ -12500,7 +12635,7 @@
         <v>43288</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="52.8">
+    <row r="64" spans="1:10" ht="49.2">
       <c r="A64" s="8" t="s">
         <v>539</v>
       </c>
@@ -12532,7 +12667,7 @@
         <v>43289</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="52.8">
+    <row r="65" spans="1:10" ht="49.2">
       <c r="A65" s="6" t="s">
         <v>580</v>
       </c>
@@ -12562,7 +12697,7 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="26.4">
+    <row r="66" spans="1:10" ht="24.6">
       <c r="A66" s="8" t="s">
         <v>580</v>
       </c>
@@ -12592,7 +12727,7 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="79.2">
+    <row r="67" spans="1:10" ht="73.8">
       <c r="A67" s="6" t="s">
         <v>594</v>
       </c>
@@ -12622,7 +12757,7 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="26.4">
+    <row r="68" spans="1:10" ht="24.6">
       <c r="A68" s="119" t="s">
         <v>602</v>
       </c>
@@ -12652,7 +12787,7 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="52.8">
+    <row r="69" spans="1:10" ht="49.2">
       <c r="A69" s="6" t="s">
         <v>627</v>
       </c>
@@ -12714,7 +12849,7 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="52.8">
+    <row r="71" spans="1:10" ht="49.2">
       <c r="A71" s="112" t="s">
         <v>642</v>
       </c>
@@ -12741,7 +12876,7 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="66">
+    <row r="72" spans="1:10" ht="61.5">
       <c r="A72" s="110" t="s">
         <v>642</v>
       </c>
@@ -12876,7 +13011,7 @@
         <v>43287</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="39.6">
+    <row r="77" spans="1:10" ht="43.2">
       <c r="A77" s="110" t="s">
         <v>642</v>
       </c>
@@ -13098,7 +13233,7 @@
         <v>43295</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="79.2">
+    <row r="85" spans="1:10" ht="61.5">
       <c r="A85" s="112" t="s">
         <v>555</v>
       </c>
@@ -13126,7 +13261,7 @@
         <v>43296</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="66">
+    <row r="86" spans="1:10" ht="57.6">
       <c r="A86" s="110" t="s">
         <v>555</v>
       </c>
@@ -13154,7 +13289,7 @@
         <v>43297</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="66">
+    <row r="87" spans="1:10" ht="61.5">
       <c r="A87" s="110" t="s">
         <v>555</v>
       </c>
@@ -13236,7 +13371,7 @@
         <v>43300</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="52.8">
+    <row r="90" spans="1:10" ht="49.2">
       <c r="A90" s="8" t="s">
         <v>744</v>
       </c>
@@ -13266,7 +13401,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="52.8">
+    <row r="91" spans="1:10" ht="49.2">
       <c r="A91" s="6" t="s">
         <v>753</v>
       </c>
@@ -13296,7 +13431,7 @@
         <v>43208</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="118.8">
+    <row r="92" spans="1:10" ht="110.7">
       <c r="A92" s="6" t="s">
         <v>758</v>
       </c>
@@ -13324,8 +13459,8 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="39.6">
-      <c r="A93" s="308" t="s">
+    <row r="93" spans="1:10" ht="36.9">
+      <c r="A93" s="311" t="s">
         <v>770</v>
       </c>
       <c r="B93" s="8" t="s">
@@ -13354,8 +13489,8 @@
         <v>43256</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="39.6">
-      <c r="A94" s="304"/>
+    <row r="94" spans="1:10" ht="36.9">
+      <c r="A94" s="307"/>
       <c r="B94" s="8" t="s">
         <v>45</v>
       </c>
@@ -13382,8 +13517,8 @@
         <v>43256</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="39.6">
-      <c r="A95" s="304"/>
+    <row r="95" spans="1:10" ht="36.9">
+      <c r="A95" s="307"/>
       <c r="B95" s="8" t="s">
         <v>45</v>
       </c>
@@ -13410,8 +13545,8 @@
         <v>43256</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="39.6">
-      <c r="A96" s="304"/>
+    <row r="96" spans="1:10" ht="36.9">
+      <c r="A96" s="307"/>
       <c r="B96" s="8" t="s">
         <v>45</v>
       </c>
@@ -13438,8 +13573,8 @@
         <v>43256</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="39.6">
-      <c r="A97" s="304"/>
+    <row r="97" spans="1:10" ht="24.6">
+      <c r="A97" s="307"/>
       <c r="B97" s="8" t="s">
         <v>45</v>
       </c>
@@ -13466,8 +13601,8 @@
         <v>43256</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="39.6">
-      <c r="A98" s="304"/>
+    <row r="98" spans="1:10" ht="24.6">
+      <c r="A98" s="307"/>
       <c r="B98" s="8" t="s">
         <v>45</v>
       </c>
@@ -13494,8 +13629,8 @@
         <v>43256</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="39.6">
-      <c r="A99" s="304"/>
+    <row r="99" spans="1:10" ht="36.9">
+      <c r="A99" s="307"/>
       <c r="B99" s="8" t="s">
         <v>45</v>
       </c>
@@ -13522,8 +13657,8 @@
         <v>43256</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="39.6">
-      <c r="A100" s="304"/>
+    <row r="100" spans="1:10" ht="36.9">
+      <c r="A100" s="307"/>
       <c r="B100" s="8" t="s">
         <v>45</v>
       </c>
@@ -13550,7 +13685,7 @@
         <v>43256</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="26.4">
+    <row r="101" spans="1:10" ht="24.6">
       <c r="A101" s="6" t="s">
         <v>803</v>
       </c>
@@ -13582,7 +13717,7 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="52.8">
+    <row r="102" spans="1:10" ht="49.2">
       <c r="A102" s="6" t="s">
         <v>824</v>
       </c>
@@ -13612,7 +13747,7 @@
         <v>43236</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="39.6">
+    <row r="103" spans="1:10" ht="36.9">
       <c r="A103" s="6" t="s">
         <v>832</v>
       </c>
@@ -13775,7 +13910,7 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="66">
+    <row r="109" spans="1:10" ht="61.5">
       <c r="A109" s="6" t="s">
         <v>882</v>
       </c>
@@ -13805,7 +13940,7 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="66">
+    <row r="110" spans="1:10" ht="61.5">
       <c r="A110" s="6" t="s">
         <v>882</v>
       </c>
@@ -14142,7 +14277,7 @@
         <v>43293</v>
       </c>
     </row>
-    <row r="122" spans="1:10" ht="118.8">
+    <row r="122" spans="1:10" ht="98.4">
       <c r="A122" s="6" t="s">
         <v>916</v>
       </c>
@@ -14174,7 +14309,7 @@
         <v>43294</v>
       </c>
     </row>
-    <row r="123" spans="1:10" ht="26.4">
+    <row r="123" spans="1:10" ht="24.6">
       <c r="A123" s="6" t="s">
         <v>916</v>
       </c>
@@ -14363,7 +14498,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -14373,7 +14508,7 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="12.3"/>
   <cols>
     <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
@@ -14387,7 +14522,7 @@
     <col min="10" max="10" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="39.6">
+    <row r="1" spans="1:10" ht="36.9">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -14412,12 +14547,12 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="310" t="s">
+      <c r="I1" s="313" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="304"/>
-    </row>
-    <row r="2" spans="1:10" ht="26.4">
+      <c r="J1" s="307"/>
+    </row>
+    <row r="2" spans="1:10" ht="24.6">
       <c r="A2" s="3"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -14433,7 +14568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="211.2">
+    <row r="3" spans="1:10" ht="196.8">
       <c r="A3" s="14" t="s">
         <v>19</v>
       </c>
@@ -14463,7 +14598,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="211.2">
+    <row r="4" spans="1:10" ht="196.8">
       <c r="A4" s="14" t="s">
         <v>19</v>
       </c>
@@ -14493,7 +14628,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="211.2">
+    <row r="5" spans="1:10" ht="196.8">
       <c r="A5" s="14" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Restored more changes to Action Items
</commit_message>
<xml_diff>
--- a/Working QA Team Folders/Pre- Release QA/Action Items (Master).xlsx
+++ b/Working QA Team Folders/Pre- Release QA/Action Items (Master).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barbj\Documents\Infoway-Health Canada CCDD\formulary\Working QA Team Folders\Pre- Release QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D0A31C1B-A009-4E14-95F9-9DC6FBBE9C11}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{55FF531F-FA46-4F04-9922-F3F9D34F80E7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="180" windowWidth="17268" windowHeight="5256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F143" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="F144" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1804" uniqueCount="1094">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1813" uniqueCount="1101">
   <si>
     <t>TM</t>
   </si>
@@ -4459,9 +4459,6 @@
     <t>U of Ps Done July 27 2018 bfj</t>
   </si>
   <si>
-    <t>Louise: DPD ingredient should be tobramycin sulfate according to monograph.</t>
-  </si>
-  <si>
     <t>Louise: change concentration to 300 mg per 16.7 mL</t>
   </si>
   <si>
@@ -4723,6 +4720,31 @@
   </si>
   <si>
     <t xml:space="preserve">Outstanding </t>
+  </si>
+  <si>
+    <t>tobramycin 40 mg per mL solution for injection</t>
+  </si>
+  <si>
+    <t>Louise: I think DPD ingredient should be tobramycin (tobramycin sulfate). Otherwise it differs from all other tobramycin injections, which I'm not inclined to believe. There is some evidence in the monograph that it contains tobramycin sodium. bfj</t>
+  </si>
+  <si>
+    <t>This outlier results in an extra (unnecessary) ntp. Bfj</t>
+  </si>
+  <si>
+    <t>valproic acid (valproate)</t>
+  </si>
+  <si>
+    <t>02238370
+02236807</t>
+  </si>
+  <si>
+    <t>valproic acid (sodium valproate) 250 mg per 5 mL syrup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Louise: both are described as oral solutions in monographs. Extra ntp results from description as syrup. </t>
+  </si>
+  <si>
+    <t>Jo and Louise looking into this one (which one is correct for all three - syrup or solution?). Bfj</t>
   </si>
 </sst>
 </file>
@@ -5388,7 +5410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="315">
+  <cellXfs count="316">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -6258,9 +6280,6 @@
     <xf numFmtId="0" fontId="61" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="62" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="17" fontId="36" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -6278,6 +6297,9 @@
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -6303,8 +6325,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="62" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6630,11 +6655,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J153"/>
+  <dimension ref="A1:J154"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J128" sqref="J128"/>
+      <pane ySplit="1" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A139" sqref="A139:XFD139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.8"/>
@@ -6919,15 +6944,15 @@
         <v>1004</v>
       </c>
       <c r="B12" s="164" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="C12" s="160"/>
       <c r="D12" s="222" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="E12" s="166"/>
       <c r="F12" s="166" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="G12" s="176"/>
       <c r="H12" s="164"/>
@@ -7050,7 +7075,7 @@
         <v>120</v>
       </c>
       <c r="H17" s="181" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="I17" s="165"/>
     </row>
@@ -7513,7 +7538,7 @@
         <v>250</v>
       </c>
       <c r="G37" s="160" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="H37" s="164"/>
       <c r="I37" s="165"/>
@@ -7536,7 +7561,7 @@
         <v>250</v>
       </c>
       <c r="G38" s="160" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="H38" s="164"/>
       <c r="I38" s="165"/>
@@ -7801,7 +7826,7 @@
         <v>319</v>
       </c>
       <c r="F48" s="185" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="G48" s="160" t="s">
         <v>320</v>
@@ -8598,7 +8623,7 @@
         <v>469</v>
       </c>
       <c r="F80" s="199" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="G80" s="164" t="s">
         <v>470</v>
@@ -8610,23 +8635,23 @@
     </row>
     <row r="81" spans="1:9" ht="41.4">
       <c r="A81" s="159" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="B81" s="160" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="C81" s="160"/>
       <c r="D81" s="161" t="s">
-        <v>1059</v>
-      </c>
-      <c r="E81" s="301" t="s">
+        <v>1058</v>
+      </c>
+      <c r="E81" s="300" t="s">
+        <v>1060</v>
+      </c>
+      <c r="F81" s="197" t="s">
         <v>1061</v>
       </c>
-      <c r="F81" s="197" t="s">
+      <c r="G81" s="164" t="s">
         <v>1062</v>
-      </c>
-      <c r="G81" s="164" t="s">
-        <v>1063</v>
       </c>
       <c r="H81" s="164"/>
       <c r="I81" s="165">
@@ -8634,24 +8659,24 @@
       </c>
     </row>
     <row r="82" spans="1:9" ht="55.2">
-      <c r="A82" s="302" t="s">
-        <v>1064</v>
+      <c r="A82" s="301" t="s">
+        <v>1063</v>
       </c>
       <c r="B82" s="160" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="C82" s="160"/>
       <c r="D82" s="161" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="E82" s="221" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="F82" s="197" t="s">
+        <v>1061</v>
+      </c>
+      <c r="G82" s="164" t="s">
         <v>1062</v>
-      </c>
-      <c r="G82" s="164" t="s">
-        <v>1063</v>
       </c>
       <c r="H82" s="164"/>
       <c r="I82" s="165">
@@ -8660,23 +8685,23 @@
     </row>
     <row r="83" spans="1:9" ht="41.4">
       <c r="A83" s="159" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="B83" s="160" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="C83" s="160"/>
       <c r="D83" s="161" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="E83" s="168" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="F83" s="197" t="s">
+        <v>1061</v>
+      </c>
+      <c r="G83" s="164" t="s">
         <v>1062</v>
-      </c>
-      <c r="G83" s="164" t="s">
-        <v>1063</v>
       </c>
       <c r="H83" s="164"/>
       <c r="I83" s="165">
@@ -8808,7 +8833,7 @@
         <v>480</v>
       </c>
       <c r="F88" s="187" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="G88" s="185" t="s">
         <v>497</v>
@@ -8918,22 +8943,22 @@
     </row>
     <row r="93" spans="1:9" ht="55.2">
       <c r="A93" s="159" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B93" s="160" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D93" s="189" t="s">
         <v>1070</v>
       </c>
-      <c r="B93" s="160" t="s">
-        <v>1060</v>
-      </c>
-      <c r="D93" s="189" t="s">
+      <c r="E93" s="221" t="s">
         <v>1071</v>
       </c>
-      <c r="E93" s="221" t="s">
-        <v>1072</v>
-      </c>
       <c r="F93" s="187" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="G93" s="164" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="H93" s="164"/>
       <c r="I93" s="165">
@@ -8954,7 +8979,7 @@
         <v>1023</v>
       </c>
       <c r="F94" s="215" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="G94" s="164"/>
       <c r="H94" s="164"/>
@@ -8964,22 +8989,22 @@
     </row>
     <row r="95" spans="1:9" ht="27.6">
       <c r="A95" s="159" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="B95" s="164" t="s">
         <v>1005</v>
       </c>
       <c r="D95" s="189" t="s">
+        <v>1081</v>
+      </c>
+      <c r="E95" s="221" t="s">
+        <v>1084</v>
+      </c>
+      <c r="F95" s="302" t="s">
         <v>1082</v>
       </c>
-      <c r="E95" s="221" t="s">
-        <v>1085</v>
-      </c>
-      <c r="F95" s="303" t="s">
+      <c r="G95" s="164" t="s">
         <v>1083</v>
-      </c>
-      <c r="G95" s="164" t="s">
-        <v>1084</v>
       </c>
       <c r="H95" s="164"/>
       <c r="I95" s="165">
@@ -9120,7 +9145,7 @@
         <v>1026</v>
       </c>
       <c r="F101" s="187" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="G101" s="160" t="s">
         <v>1027</v>
@@ -9221,7 +9246,7 @@
         <v>1030</v>
       </c>
       <c r="F105" s="187" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="G105" s="164" t="s">
         <v>1031</v>
@@ -9384,23 +9409,23 @@
     </row>
     <row r="112" spans="1:10" ht="41.4">
       <c r="A112" s="159" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="B112" s="160" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="C112" s="164"/>
       <c r="D112" s="224" t="s">
+        <v>1073</v>
+      </c>
+      <c r="E112" s="168" t="s">
         <v>1074</v>
       </c>
-      <c r="E112" s="168" t="s">
-        <v>1075</v>
-      </c>
       <c r="F112" s="187" t="s">
+        <v>1076</v>
+      </c>
+      <c r="G112" s="164" t="s">
         <v>1077</v>
-      </c>
-      <c r="G112" s="164" t="s">
-        <v>1078</v>
       </c>
       <c r="H112" s="164"/>
       <c r="I112" s="165">
@@ -9768,7 +9793,7 @@
         <v>43196</v>
       </c>
       <c r="J127" s="166" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="128" spans="1:10" ht="82.8">
@@ -9796,7 +9821,7 @@
         <v>43196</v>
       </c>
       <c r="J128" s="181" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="129" spans="1:10" ht="55.2">
@@ -9824,30 +9849,30 @@
         <v>43196</v>
       </c>
       <c r="J129" s="166" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="130" spans="1:10" ht="86.4">
       <c r="A130" s="182" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B130" s="180" t="s">
         <v>1086</v>
       </c>
-      <c r="B130" s="180" t="s">
+      <c r="C130" s="180"/>
+      <c r="D130" s="303" t="s">
         <v>1087</v>
       </c>
-      <c r="C130" s="180"/>
-      <c r="D130" s="314" t="s">
+      <c r="E130" s="168" t="s">
         <v>1088</v>
       </c>
-      <c r="E130" s="168" t="s">
+      <c r="F130" s="185" t="s">
         <v>1089</v>
-      </c>
-      <c r="F130" s="185" t="s">
-        <v>1090</v>
       </c>
       <c r="G130" s="163"/>
       <c r="H130" s="164"/>
       <c r="I130" s="165" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="131" spans="1:10" ht="41.4">
@@ -9885,14 +9910,14 @@
         <v>142</v>
       </c>
       <c r="C132" s="164"/>
-      <c r="D132" s="299" t="s">
+      <c r="D132" s="298" t="s">
         <v>876</v>
       </c>
       <c r="E132" s="160" t="s">
         <v>879</v>
       </c>
       <c r="F132" s="187" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="G132" s="164"/>
       <c r="H132" s="164"/>
@@ -10002,17 +10027,23 @@
         <v>43240</v>
       </c>
     </row>
-    <row r="137" spans="1:10" ht="41.4">
-      <c r="A137" s="170" t="s">
+    <row r="137" spans="1:10" ht="138">
+      <c r="A137" s="173" t="s">
         <v>836</v>
       </c>
-      <c r="D137" s="297">
+      <c r="D137" s="314">
         <v>2420287</v>
       </c>
-      <c r="F137" s="166" t="s">
-        <v>1040</v>
-      </c>
-      <c r="I137" s="298">
+      <c r="E137" s="221" t="s">
+        <v>1093</v>
+      </c>
+      <c r="F137" s="185" t="s">
+        <v>1094</v>
+      </c>
+      <c r="G137" s="166" t="s">
+        <v>1095</v>
+      </c>
+      <c r="I137" s="297">
         <v>372000</v>
       </c>
     </row>
@@ -10041,34 +10072,32 @@
         <v>43288</v>
       </c>
     </row>
-    <row r="139" spans="1:10" ht="138">
+    <row r="139" spans="1:10" ht="55.2">
       <c r="A139" s="159" t="s">
-        <v>857</v>
+        <v>1096</v>
       </c>
       <c r="B139" s="160" t="s">
-        <v>77</v>
-      </c>
-      <c r="C139" s="160" t="s">
-        <v>22</v>
-      </c>
-      <c r="D139" s="161" t="s">
-        <v>858</v>
-      </c>
-      <c r="E139" s="168"/>
-      <c r="F139" s="179" t="s">
-        <v>859</v>
+        <v>1086</v>
+      </c>
+      <c r="C139" s="160"/>
+      <c r="D139" s="315" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E139" s="221" t="s">
+        <v>1098</v>
+      </c>
+      <c r="F139" s="163" t="s">
+        <v>1099</v>
       </c>
       <c r="G139" s="164" t="s">
-        <v>860</v>
-      </c>
-      <c r="H139" s="209" t="s">
-        <v>962</v>
-      </c>
-      <c r="I139" s="165">
-        <v>43270</v>
-      </c>
-    </row>
-    <row r="140" spans="1:10" ht="41.4">
+        <v>1100</v>
+      </c>
+      <c r="H139" s="164"/>
+      <c r="I139" s="165" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" ht="138">
       <c r="A140" s="159" t="s">
         <v>857</v>
       </c>
@@ -10079,17 +10108,17 @@
         <v>22</v>
       </c>
       <c r="D140" s="161" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="E140" s="168"/>
       <c r="F140" s="179" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="G140" s="164" t="s">
-        <v>863</v>
-      </c>
-      <c r="H140" s="181" t="s">
-        <v>963</v>
+        <v>860</v>
+      </c>
+      <c r="H140" s="209" t="s">
+        <v>962</v>
       </c>
       <c r="I140" s="165">
         <v>43270</v>
@@ -10106,11 +10135,11 @@
         <v>22</v>
       </c>
       <c r="D141" s="161" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="E141" s="168"/>
       <c r="F141" s="179" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
       <c r="G141" s="164" t="s">
         <v>863</v>
@@ -10122,7 +10151,7 @@
         <v>43270</v>
       </c>
     </row>
-    <row r="142" spans="1:10" ht="55.2">
+    <row r="142" spans="1:10" ht="41.4">
       <c r="A142" s="159" t="s">
         <v>857</v>
       </c>
@@ -10133,85 +10162,101 @@
         <v>22</v>
       </c>
       <c r="D142" s="161" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="E142" s="168"/>
-      <c r="F142" s="197" t="s">
-        <v>867</v>
-      </c>
-      <c r="G142" s="164"/>
-      <c r="H142" s="209" t="s">
-        <v>962</v>
+      <c r="F142" s="179" t="s">
+        <v>865</v>
+      </c>
+      <c r="G142" s="164" t="s">
+        <v>863</v>
+      </c>
+      <c r="H142" s="181" t="s">
+        <v>963</v>
       </c>
       <c r="I142" s="165">
         <v>43270</v>
       </c>
     </row>
-    <row r="143" spans="1:10" ht="41.4">
+    <row r="143" spans="1:10" ht="55.2">
       <c r="A143" s="159" t="s">
+        <v>857</v>
+      </c>
+      <c r="B143" s="160" t="s">
+        <v>77</v>
+      </c>
+      <c r="C143" s="160" t="s">
+        <v>22</v>
+      </c>
+      <c r="D143" s="161" t="s">
+        <v>866</v>
+      </c>
+      <c r="E143" s="168"/>
+      <c r="F143" s="197" t="s">
+        <v>867</v>
+      </c>
+      <c r="G143" s="164"/>
+      <c r="H143" s="209" t="s">
+        <v>962</v>
+      </c>
+      <c r="I143" s="165">
+        <v>43270</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" ht="41.4">
+      <c r="A144" s="159" t="s">
         <v>868</v>
       </c>
-      <c r="B143" s="164" t="s">
+      <c r="B144" s="164" t="s">
         <v>142</v>
-      </c>
-      <c r="C143" s="164" t="s">
-        <v>22</v>
-      </c>
-      <c r="D143" s="183" t="s">
-        <v>869</v>
-      </c>
-      <c r="E143" s="210" t="s">
-        <v>870</v>
-      </c>
-      <c r="F143" s="187" t="s">
-        <v>760</v>
-      </c>
-      <c r="G143" s="164" t="s">
-        <v>877</v>
-      </c>
-      <c r="H143" s="209" t="s">
-        <v>964</v>
-      </c>
-      <c r="I143" s="165">
-        <v>43250</v>
-      </c>
-    </row>
-    <row r="144" spans="1:10" ht="27.6">
-      <c r="A144" s="159" t="s">
-        <v>878</v>
-      </c>
-      <c r="B144" s="164" t="s">
-        <v>763</v>
       </c>
       <c r="C144" s="164" t="s">
         <v>22</v>
       </c>
-      <c r="D144" s="186" t="s">
+      <c r="D144" s="183" t="s">
+        <v>869</v>
+      </c>
+      <c r="E144" s="210" t="s">
+        <v>870</v>
+      </c>
+      <c r="F144" s="187" t="s">
+        <v>760</v>
+      </c>
+      <c r="G144" s="164" t="s">
+        <v>877</v>
+      </c>
+      <c r="H144" s="209" t="s">
+        <v>964</v>
+      </c>
+      <c r="I144" s="165">
+        <v>43250</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" ht="27.6">
+      <c r="A145" s="159" t="s">
+        <v>878</v>
+      </c>
+      <c r="B145" s="164" t="s">
+        <v>763</v>
+      </c>
+      <c r="C145" s="164" t="s">
+        <v>22</v>
+      </c>
+      <c r="D145" s="186" t="s">
         <v>883</v>
       </c>
-      <c r="F144" s="187" t="s">
+      <c r="F145" s="187" t="s">
         <v>894</v>
       </c>
-      <c r="H144" s="209" t="s">
+      <c r="H145" s="209" t="s">
         <v>962</v>
       </c>
-      <c r="I144" s="211">
+      <c r="I145" s="211">
         <v>43288</v>
       </c>
     </row>
-    <row r="145" spans="1:9">
-      <c r="D145" s="164"/>
-    </row>
-    <row r="146" spans="1:9" ht="14.1">
-      <c r="A146" s="159"/>
-      <c r="B146" s="160"/>
-      <c r="C146" s="160"/>
-      <c r="D146" s="160"/>
-      <c r="E146" s="168"/>
-      <c r="F146" s="199"/>
-      <c r="G146" s="164"/>
-      <c r="H146" s="164"/>
-      <c r="I146" s="165"/>
+    <row r="146" spans="1:9">
+      <c r="D146" s="164"/>
     </row>
     <row r="147" spans="1:9" ht="14.1">
       <c r="A147" s="159"/>
@@ -10289,6 +10334,17 @@
       <c r="G153" s="164"/>
       <c r="H153" s="164"/>
       <c r="I153" s="165"/>
+    </row>
+    <row r="154" spans="1:9" ht="14.1">
+      <c r="A154" s="159"/>
+      <c r="B154" s="160"/>
+      <c r="C154" s="160"/>
+      <c r="D154" s="160"/>
+      <c r="E154" s="168"/>
+      <c r="F154" s="199"/>
+      <c r="G154" s="164"/>
+      <c r="H154" s="164"/>
+      <c r="I154" s="165"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -10926,13 +10982,13 @@
         <v>881</v>
       </c>
       <c r="H22" s="229" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="I22" s="230">
         <v>43250</v>
       </c>
-      <c r="J22" s="300" t="s">
-        <v>1042</v>
+      <c r="J22" s="299" t="s">
+        <v>1041</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="267" customFormat="1" ht="61.5">
@@ -11465,8 +11521,8 @@
       <c r="I15" s="230">
         <v>43196</v>
       </c>
-      <c r="J15" s="300" t="s">
-        <v>1052</v>
+      <c r="J15" s="299" t="s">
+        <v>1051</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="24.6">
@@ -11696,7 +11752,7 @@
         <v>43250</v>
       </c>
       <c r="J31" s="263" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="28.8">
@@ -11834,7 +11890,7 @@
         <v>43250</v>
       </c>
       <c r="J36" s="229" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="37" spans="1:10" s="267" customFormat="1" ht="61.5">
@@ -11864,7 +11920,7 @@
         <v>43278</v>
       </c>
       <c r="J37" s="229" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="38" spans="1:10" s="267" customFormat="1" ht="61.5">
@@ -11894,7 +11950,7 @@
         <v>43278</v>
       </c>
       <c r="J38" s="229" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="36.9">

</xml_diff>

<commit_message>
Updated Action Items file
</commit_message>
<xml_diff>
--- a/Working QA Team Folders/Pre- Release QA/Action Items (Master).xlsx
+++ b/Working QA Team Folders/Pre- Release QA/Action Items (Master).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barbj\Documents\Infoway-Health Canada CCDD\formulary\Working QA Team Folders\Pre- Release QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8CE121D7-BE02-4341-9643-EF065CB45640}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D3E9E178-8805-4646-ADDD-684973CCBA59}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="180" windowWidth="17268" windowHeight="5256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="1103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1817" uniqueCount="1105">
   <si>
     <t>TM</t>
   </si>
@@ -4752,6 +4752,12 @@
   <si>
     <t>(Discussed at Webex meeting in July - Barb will follow up with Julie re. 23.2 vs. 20 mcg and then add to combination product table).</t>
   </si>
+  <si>
+    <t>MP: PDP-AMANTADINE HYDROCHLORIDE SYRUP (amantadine hydrochloride 10 mg per mL syrup) PENDOPHARM DIVISION OF PHARMASCIENCE INC</t>
+  </si>
+  <si>
+    <t>Louise: decision at Webex call to change this to 50 mg per 5 mL in DPD.</t>
+  </si>
 </sst>
 </file>
 
@@ -4763,7 +4769,7 @@
     <numFmt numFmtId="166" formatCode="#0"/>
     <numFmt numFmtId="167" formatCode="mmmm\ yyyy"/>
   </numFmts>
-  <fonts count="64">
+  <fonts count="65">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -5119,6 +5125,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00008B"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -5416,7 +5428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="316">
+  <cellXfs count="318">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -6336,6 +6348,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6664,8 +6682,8 @@
   <dimension ref="A1:J155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.8"/>
@@ -7087,15 +7105,21 @@
       </c>
       <c r="I17" s="165"/>
     </row>
-    <row r="18" spans="1:9" ht="14.1">
+    <row r="18" spans="1:9" ht="72">
       <c r="A18" s="159" t="s">
         <v>1101</v>
       </c>
       <c r="B18" s="160"/>
       <c r="C18" s="160"/>
-      <c r="D18" s="183"/>
-      <c r="E18" s="168"/>
-      <c r="F18" s="179"/>
+      <c r="D18" s="316">
+        <v>2022826</v>
+      </c>
+      <c r="E18" s="317" t="s">
+        <v>1103</v>
+      </c>
+      <c r="F18" s="179" t="s">
+        <v>1104</v>
+      </c>
       <c r="G18" s="164"/>
       <c r="H18" s="181"/>
       <c r="I18" s="165"/>

</xml_diff>

<commit_message>
Updated Action Items; Issues with File
</commit_message>
<xml_diff>
--- a/Working QA Team Folders/Pre- Release QA/Action Items (Master).xlsx
+++ b/Working QA Team Folders/Pre- Release QA/Action Items (Master).xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barbj\Documents\Infoway-Health Canada CCDD\formulary\Working QA Team Folders\Pre- Release QA\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E9ACCE0D-0E95-42BD-90EA-203E0EC77EF1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="180" windowWidth="17268" windowHeight="5256"/>
+    <workbookView xWindow="0" yWindow="180" windowWidth="17268" windowHeight="5256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Action Items, Open" sheetId="1" r:id="rId1"/>
@@ -12,23 +18,24 @@
     <sheet name="Completed AIs Released" sheetId="3" r:id="rId3"/>
     <sheet name="AIs no longer relevant" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="F122" authorId="0">
+    <comment ref="F122" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Dose is a multiple of 100 mg (2.5 mL). JH</t>
         </r>
@@ -39,18 +46,19 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="F19" authorId="0">
+    <comment ref="F19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Aseptically transfer 16.7 mL (300 mg) of POSANOL®
 Solution for Injection to an IV bag
@@ -59,13 +67,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="F24" authorId="0">
+    <comment ref="F24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Dose is multiple of 100 mg; usual dose 100, 200 or 400 mg depending on weight (from PM). JH</t>
         </r>
@@ -76,42 +85,45 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="E94" authorId="0">
+    <comment ref="E94" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>or should it be "nadroparin (nadroparin calcium)"?</t>
         </r>
       </text>
     </comment>
-    <comment ref="G102" authorId="0">
+    <comment ref="G102" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>https://drive.google.com/open?id=178EHBpmulHEy36mWnxInCTkfI01T4vMG</t>
         </r>
       </text>
     </comment>
-    <comment ref="G103" authorId="0">
+    <comment ref="G103" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Link to label image
 https://drive.google.com/open?id=1_rdeWXY4haEvMsTTdbd4saBrwMLwYuf4
@@ -119,13 +131,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="H125" authorId="0">
+    <comment ref="H125" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>https://docs.google.com/document/d/14AkaFST00JclBvfARGRHooHriYgdst4Bl89TcNSfW68/edit?usp=sharing</t>
         </r>
@@ -348,6 +361,7 @@
         <sz val="10"/>
         <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Not yet generated? bfj</t>
     </r>
@@ -368,6 +382,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>DPD to be updated, LT</t>
     </r>
@@ -391,6 +406,7 @@
         <sz val="10"/>
         <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Not yet generated? bfj</t>
     </r>
@@ -414,6 +430,7 @@
         <sz val="10"/>
         <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Not yet generated? bfj</t>
     </r>
@@ -558,6 +575,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Done bfj/jh</t>
     </r>
@@ -861,6 +879,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>UoP update: 88577, 100, g, N, N</t>
     </r>
@@ -869,6 +888,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 UoP done - check with Julie. jh; using UoP the ntp will be "cefazolin (cefazolin sodium) 100 g powder for solution for injection bag"</t>
@@ -989,6 +1009,7 @@
         <sz val="10"/>
         <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Louise investigating Webex Apr18
 </t>
@@ -998,6 +1019,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>&lt;JH&gt; As far as I can tell from the labels in the Drug Submission (docubridge) both 50 mL and 100 mL bottles are present as cefixime trihydrate. JUN27</t>
     </r>
@@ -1192,6 +1214,7 @@
         <sz val="10"/>
         <color rgb="FFFF9900"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>UoP done 06Jun18 jh - check with Julie - using UoP the ntp will be "ceftriaxone (ceftriaxone sodium) 100 g  powder for solution for injection bag"</t>
     </r>
@@ -1364,6 +1387,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>inhalation</t>
     </r>
@@ -1372,6 +1396,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> solution 2 mL unit dose vial</t>
     </r>
@@ -1388,6 +1413,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Sent to DPD team
 </t>
@@ -1397,6 +1423,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>RELEASED</t>
     </r>
@@ -1993,6 +2020,7 @@
         <sz val="10"/>
         <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Discussion: TM generated as enoxaparin sodium.</t>
     </r>
@@ -2001,6 +2029,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> Should be enoxaparin. Other action items complete. bfj</t>
     </r>
@@ -2029,6 +2058,7 @@
         <sz val="10"/>
         <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Discussion: TM generated as enoxaparin sodium (June 2018).  Should be enoxaparin.</t>
     </r>
@@ -2037,6 +2067,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> Other action items complete. bfj</t>
     </r>
@@ -2056,6 +2087,7 @@
         <sz val="10"/>
         <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Discussion: TM generated as enoxaparin sodium (June 2018).  Should be enoxaparin.</t>
     </r>
@@ -2064,6 +2096,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> Other action items complete. bfj</t>
     </r>
@@ -2080,6 +2113,7 @@
         <sz val="10"/>
         <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Discussion: TM generated as enoxaparin sodium (June 2018).  Should be enoxaparin.</t>
     </r>
@@ -2088,6 +2122,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> Other action items complete. bfj</t>
     </r>
@@ -2115,6 +2150,7 @@
         <sz val="10"/>
         <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Discussion: TM generated as enoxaparin sodium (June 2018).  Should be enoxaparin.</t>
     </r>
@@ -2123,6 +2159,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> Other action items complete. bfj</t>
     </r>
@@ -2142,6 +2179,7 @@
         <sz val="10"/>
         <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Discussion: TM generated as enoxaparin sodium (June 2018).  Should be enoxaparin.</t>
     </r>
@@ -2150,6 +2188,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> Other action items complete. bfj</t>
     </r>
@@ -2178,6 +2217,7 @@
         <sz val="10"/>
         <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Discussion: TM generated as enoxaparin sodium (June 2018).  Should be enoxaparin.</t>
     </r>
@@ -2186,6 +2226,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> Other action items complete. bfj</t>
     </r>
@@ -2209,6 +2250,7 @@
         <sz val="10"/>
         <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Discussion: TM generated as enoxaparin sodium (June 2018).  Should be enoxaparin.</t>
     </r>
@@ -2217,6 +2259,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> Other action items complete. bfj</t>
     </r>
@@ -2822,6 +2865,7 @@
         <strike/>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">UoP updates were completed but not reflected in the April Generation. Hoping to see in the May gen. JH
 </t>
@@ -2831,6 +2875,7 @@
         <b/>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Julie</t>
     </r>
@@ -2839,6 +2884,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>: I don't think UoP updates were done after all? JH
 UoP done 28JUN18 jh</t>
@@ -3030,6 +3076,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> 1</t>
     </r>
@@ -3038,6 +3085,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> mL". JH</t>
     </r>
@@ -3090,6 +3138,7 @@
         <sz val="10"/>
         <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>UoP update</t>
     </r>
@@ -3098,6 +3147,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>: Should be "</t>
     </r>
@@ -3106,6 +3156,7 @@
         <sz val="10"/>
         <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>ampoule</t>
     </r>
@@ -3114,6 +3165,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>" rather than vial. JH</t>
     </r>
@@ -3137,6 +3189,7 @@
         <sz val="10"/>
         <color rgb="FFFF00FF"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>&lt;JH&gt; It can be confusing but the monograph includes a number of products with different DINs, however the ampoules and vials have different product names which is how I was able to determine this DIN belongs to the ampoules.</t>
     </r>
@@ -3159,6 +3212,7 @@
         <sz val="10"/>
         <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>UoP update</t>
     </r>
@@ -3167,6 +3221,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>: unit of presentation is "</t>
     </r>
@@ -3175,6 +3230,7 @@
         <sz val="10"/>
         <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>vial</t>
     </r>
@@ -3183,6 +3239,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>". JH</t>
     </r>
@@ -4858,7 +4915,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="mmmm\ d\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
@@ -4877,75 +4934,90 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF454545"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -4960,62 +5032,74 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF454545"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF00FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF9900"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF454545"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF434343"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <strike/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -6805,6 +6889,9 @@
     <xf numFmtId="164" fontId="49" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="52" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6830,9 +6917,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="52" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7146,22 +7230,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:J142"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A95" sqref="A95:XFD95"/>
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E121" sqref="E121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.8"/>
@@ -7179,7 +7263,7 @@
     <col min="11" max="16384" width="14.44140625" style="160"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="153" customFormat="1" ht="27.6">
+    <row r="1" spans="1:10" s="153" customFormat="1" ht="28.2">
       <c r="A1" s="149" t="s">
         <v>0</v>
       </c>
@@ -7232,7 +7316,7 @@
         <v>43281</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="105.6">
+    <row r="3" spans="1:10" ht="105">
       <c r="A3" s="154" t="s">
         <v>971</v>
       </c>
@@ -7353,7 +7437,7 @@
         <v>43255</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="317.39999999999998">
+    <row r="8" spans="1:10" ht="345">
       <c r="A8" s="164" t="s">
         <v>417</v>
       </c>
@@ -7374,7 +7458,7 @@
       <c r="H8" s="158"/>
       <c r="I8" s="159"/>
     </row>
-    <row r="9" spans="1:10" ht="331.2">
+    <row r="9" spans="1:10" ht="358.8">
       <c r="A9" s="166" t="s">
         <v>910</v>
       </c>
@@ -7395,7 +7479,7 @@
       <c r="H9" s="158"/>
       <c r="I9" s="159"/>
     </row>
-    <row r="10" spans="1:10" ht="409.6">
+    <row r="10" spans="1:10" ht="409.5">
       <c r="A10" s="164" t="s">
         <v>930</v>
       </c>
@@ -7537,7 +7621,7 @@
       </c>
       <c r="I15" s="159"/>
     </row>
-    <row r="16" spans="1:10" ht="69">
+    <row r="16" spans="1:10" ht="82.8">
       <c r="A16" s="154" t="s">
         <v>1067</v>
       </c>
@@ -7556,7 +7640,7 @@
       <c r="H16" s="173"/>
       <c r="I16" s="159"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" ht="14.1">
       <c r="A17" s="154" t="s">
         <v>121</v>
       </c>
@@ -7577,7 +7661,7 @@
         <v>43252</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="276">
+    <row r="18" spans="1:9" ht="289.8">
       <c r="A18" s="174" t="s">
         <v>121</v>
       </c>
@@ -7604,7 +7688,7 @@
         <v>43240</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="41.4">
+    <row r="19" spans="1:9" ht="42.3">
       <c r="A19" s="154" t="s">
         <v>132</v>
       </c>
@@ -7771,7 +7855,7 @@
         <v>43196</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="27.6">
+    <row r="26" spans="1:9" ht="28.2">
       <c r="A26" s="154" t="s">
         <v>206</v>
       </c>
@@ -7817,7 +7901,7 @@
       <c r="H27" s="173"/>
       <c r="I27" s="159"/>
     </row>
-    <row r="28" spans="1:9" ht="41.4">
+    <row r="28" spans="1:9" ht="55.2">
       <c r="A28" s="154" t="s">
         <v>218</v>
       </c>
@@ -7842,7 +7926,7 @@
         <v>43196</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="41.4">
+    <row r="29" spans="1:9" ht="55.2">
       <c r="A29" s="174" t="s">
         <v>218</v>
       </c>
@@ -7863,7 +7947,7 @@
         <v>43196</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="41.4">
+    <row r="30" spans="1:9" ht="55.2">
       <c r="A30" s="174" t="s">
         <v>218</v>
       </c>
@@ -7884,7 +7968,7 @@
         <v>43196</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="41.4">
+    <row r="31" spans="1:9" ht="55.2">
       <c r="A31" s="174" t="s">
         <v>218</v>
       </c>
@@ -8090,7 +8174,7 @@
       <c r="I39" s="182"/>
       <c r="J39" s="183"/>
     </row>
-    <row r="40" spans="1:10" ht="124.2">
+    <row r="40" spans="1:10" ht="151.80000000000001">
       <c r="A40" s="154" t="s">
         <v>262</v>
       </c>
@@ -8255,7 +8339,7 @@
         <v>43250</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="69.599999999999994">
+    <row r="46" spans="1:10" ht="69.3">
       <c r="A46" s="154" t="s">
         <v>332</v>
       </c>
@@ -8588,7 +8672,7 @@
         <v>43313</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="41.4">
+    <row r="60" spans="1:9" ht="55.2">
       <c r="A60" s="154" t="s">
         <v>76</v>
       </c>
@@ -8610,7 +8694,7 @@
       <c r="H60" s="158"/>
       <c r="I60" s="159"/>
     </row>
-    <row r="61" spans="1:9" ht="41.4">
+    <row r="61" spans="1:9" ht="55.2">
       <c r="A61" s="174" t="s">
         <v>76</v>
       </c>
@@ -8637,7 +8721,7 @@
         <v>43284</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="41.4">
+    <row r="62" spans="1:9" ht="55.2">
       <c r="A62" s="174" t="s">
         <v>76</v>
       </c>
@@ -8664,7 +8748,7 @@
         <v>43285</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="41.4">
+    <row r="63" spans="1:9" ht="55.2">
       <c r="A63" s="174" t="s">
         <v>76</v>
       </c>
@@ -8691,7 +8775,7 @@
         <v>43287</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="41.4">
+    <row r="64" spans="1:9" ht="55.2">
       <c r="A64" s="174" t="s">
         <v>76</v>
       </c>
@@ -8718,7 +8802,7 @@
         <v>43288</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="41.4">
+    <row r="65" spans="1:9" ht="55.2">
       <c r="A65" s="174" t="s">
         <v>76</v>
       </c>
@@ -8768,7 +8852,7 @@
       <c r="H66" s="158"/>
       <c r="I66" s="159"/>
     </row>
-    <row r="67" spans="1:9" ht="41.4">
+    <row r="67" spans="1:9" ht="55.2">
       <c r="A67" s="174" t="s">
         <v>422</v>
       </c>
@@ -8795,7 +8879,7 @@
         <v>43289</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="55.2">
+    <row r="68" spans="1:9" ht="56.4">
       <c r="A68" s="154" t="s">
         <v>425</v>
       </c>
@@ -8822,7 +8906,7 @@
         <v>43290</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="55.2">
+    <row r="69" spans="1:9" ht="56.4">
       <c r="A69" s="191" t="s">
         <v>427</v>
       </c>
@@ -8889,7 +8973,7 @@
       <c r="H71" s="158"/>
       <c r="I71" s="159"/>
     </row>
-    <row r="72" spans="1:9" ht="124.2">
+    <row r="72" spans="1:9" ht="138">
       <c r="A72" s="154" t="s">
         <v>448</v>
       </c>
@@ -8989,7 +9073,7 @@
         <v>43315</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="409.6">
+    <row r="76" spans="1:9" ht="409.5">
       <c r="A76" s="154" t="s">
         <v>454</v>
       </c>
@@ -9504,7 +9588,7 @@
       <c r="H96" s="158"/>
       <c r="I96" s="159"/>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" ht="14.1">
       <c r="A97" s="154" t="s">
         <v>583</v>
       </c>
@@ -9894,7 +9978,7 @@
       <c r="H112" s="158"/>
       <c r="I112" s="159"/>
     </row>
-    <row r="113" spans="1:10" ht="82.8">
+    <row r="113" spans="1:10" ht="96.6">
       <c r="A113" s="154" t="s">
         <v>640</v>
       </c>
@@ -10103,7 +10187,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="121" spans="1:10" ht="88.2">
+    <row r="121" spans="1:10" ht="86.4">
       <c r="A121" s="174" t="s">
         <v>1051</v>
       </c>
@@ -10126,7 +10210,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="122" spans="1:10" ht="27.6">
+    <row r="122" spans="1:10" ht="41.4">
       <c r="A122" s="154" t="s">
         <v>715</v>
       </c>
@@ -10251,7 +10335,7 @@
       <c r="H126" s="196"/>
       <c r="I126" s="159"/>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" ht="14.1">
       <c r="A127" s="154" t="s">
         <v>785</v>
       </c>
@@ -10374,7 +10458,7 @@
     <row r="134" spans="1:9">
       <c r="D134" s="276"/>
     </row>
-    <row r="135" spans="1:9">
+    <row r="135" spans="1:9" ht="14.1">
       <c r="A135" s="154"/>
       <c r="B135" s="155"/>
       <c r="C135" s="155"/>
@@ -10385,7 +10469,7 @@
       <c r="H135" s="158"/>
       <c r="I135" s="159"/>
     </row>
-    <row r="136" spans="1:9">
+    <row r="136" spans="1:9" ht="14.1">
       <c r="A136" s="154"/>
       <c r="B136" s="155"/>
       <c r="C136" s="155"/>
@@ -10396,7 +10480,7 @@
       <c r="H136" s="158"/>
       <c r="I136" s="159"/>
     </row>
-    <row r="137" spans="1:9">
+    <row r="137" spans="1:9" ht="14.1">
       <c r="A137" s="154"/>
       <c r="B137" s="155"/>
       <c r="C137" s="155"/>
@@ -10407,7 +10491,7 @@
       <c r="H137" s="158"/>
       <c r="I137" s="159"/>
     </row>
-    <row r="138" spans="1:9">
+    <row r="138" spans="1:9" ht="14.1">
       <c r="A138" s="154"/>
       <c r="B138" s="155"/>
       <c r="C138" s="155"/>
@@ -10418,7 +10502,7 @@
       <c r="H138" s="158"/>
       <c r="I138" s="159"/>
     </row>
-    <row r="139" spans="1:9">
+    <row r="139" spans="1:9" ht="14.1">
       <c r="A139" s="154"/>
       <c r="B139" s="155"/>
       <c r="C139" s="155"/>
@@ -10429,7 +10513,7 @@
       <c r="H139" s="158"/>
       <c r="I139" s="159"/>
     </row>
-    <row r="140" spans="1:9">
+    <row r="140" spans="1:9" ht="14.1">
       <c r="A140" s="154"/>
       <c r="B140" s="155"/>
       <c r="C140" s="155"/>
@@ -10440,7 +10524,7 @@
       <c r="H140" s="158"/>
       <c r="I140" s="159"/>
     </row>
-    <row r="141" spans="1:9">
+    <row r="141" spans="1:9" ht="14.1">
       <c r="A141" s="154"/>
       <c r="B141" s="155"/>
       <c r="C141" s="155"/>
@@ -10451,7 +10535,7 @@
       <c r="H141" s="158"/>
       <c r="I141" s="159"/>
     </row>
-    <row r="142" spans="1:9">
+    <row r="142" spans="1:9" ht="14.1">
       <c r="A142" s="154"/>
       <c r="B142" s="155"/>
       <c r="C142" s="155"/>
@@ -10464,7 +10548,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F113" r:id="rId1" location="gid=314589613&amp;range=309:309"/>
+    <hyperlink ref="F113" r:id="rId1" location="gid=314589613&amp;range=309:309" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -10473,7 +10557,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -10484,7 +10568,7 @@
       <selection pane="bottomLeft" activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="12.3"/>
   <cols>
     <col min="1" max="1" width="18.109375" style="207" customWidth="1"/>
     <col min="2" max="5" width="14.44140625" style="207"/>
@@ -10496,7 +10580,7 @@
     <col min="11" max="16384" width="14.44140625" style="207"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="246" customFormat="1" ht="26.4">
+    <row r="1" spans="1:10" s="246" customFormat="1" ht="24.6">
       <c r="A1" s="244" t="s">
         <v>0</v>
       </c>
@@ -10521,12 +10605,12 @@
       <c r="H1" s="244" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="389" t="s">
+      <c r="I1" s="390" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="390"/>
-    </row>
-    <row r="2" spans="1:10" s="250" customFormat="1" ht="26.4">
+      <c r="J1" s="391"/>
+    </row>
+    <row r="2" spans="1:10" s="250" customFormat="1" ht="24.6">
       <c r="A2" s="247"/>
       <c r="B2" s="248"/>
       <c r="C2" s="248"/>
@@ -10542,7 +10626,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="92.4">
+    <row r="3" spans="1:10" ht="86.1">
       <c r="A3" s="208" t="s">
         <v>19</v>
       </c>
@@ -10572,7 +10656,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="105.6">
+    <row r="4" spans="1:10" ht="98.4">
       <c r="A4" s="208" t="s">
         <v>19</v>
       </c>
@@ -10602,7 +10686,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="105.6">
+    <row r="5" spans="1:10" ht="98.4">
       <c r="A5" s="208" t="s">
         <v>19</v>
       </c>
@@ -10632,7 +10716,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="105.6">
+    <row r="6" spans="1:10" ht="98.4">
       <c r="A6" s="208" t="s">
         <v>19</v>
       </c>
@@ -10692,7 +10776,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="92.4">
+    <row r="8" spans="1:10" ht="73.8">
       <c r="A8" s="204" t="s">
         <v>44</v>
       </c>
@@ -10720,7 +10804,7 @@
       </c>
       <c r="J8" s="206"/>
     </row>
-    <row r="9" spans="1:10" ht="92.4">
+    <row r="9" spans="1:10" ht="73.8">
       <c r="A9" s="201" t="s">
         <v>44</v>
       </c>
@@ -10748,7 +10832,7 @@
       </c>
       <c r="J9" s="206"/>
     </row>
-    <row r="10" spans="1:10" ht="92.4">
+    <row r="10" spans="1:10" ht="73.8">
       <c r="A10" s="201" t="s">
         <v>44</v>
       </c>
@@ -10776,7 +10860,7 @@
       </c>
       <c r="J10" s="206"/>
     </row>
-    <row r="11" spans="1:10" ht="118.8">
+    <row r="11" spans="1:10" ht="98.4">
       <c r="A11" s="201" t="s">
         <v>190</v>
       </c>
@@ -10802,7 +10886,7 @@
       </c>
       <c r="J11" s="206"/>
     </row>
-    <row r="12" spans="1:10" ht="165.6">
+    <row r="12" spans="1:10" ht="160.19999999999999">
       <c r="A12" s="156" t="s">
         <v>278</v>
       </c>
@@ -10830,7 +10914,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="79.2">
+    <row r="13" spans="1:10" ht="73.8">
       <c r="A13" s="201" t="s">
         <v>76</v>
       </c>
@@ -10882,7 +10966,7 @@
       </c>
       <c r="J14" s="206"/>
     </row>
-    <row r="15" spans="1:10" ht="55.2">
+    <row r="15" spans="1:10" ht="51.6">
       <c r="A15" s="201" t="s">
         <v>76</v>
       </c>
@@ -10908,7 +10992,7 @@
       <c r="I15" s="205"/>
       <c r="J15" s="206"/>
     </row>
-    <row r="16" spans="1:10" ht="55.2">
+    <row r="16" spans="1:10" ht="51.6">
       <c r="A16" s="201" t="s">
         <v>76</v>
       </c>
@@ -10934,7 +11018,7 @@
       <c r="I16" s="205"/>
       <c r="J16" s="206"/>
     </row>
-    <row r="17" spans="1:10" s="241" customFormat="1" ht="39.6">
+    <row r="17" spans="1:10" s="241" customFormat="1" ht="36.9">
       <c r="A17" s="269" t="s">
         <v>570</v>
       </c>
@@ -10959,7 +11043,7 @@
         <v>43240</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="241" customFormat="1" ht="66">
+    <row r="18" spans="1:10" s="241" customFormat="1" ht="61.5">
       <c r="A18" s="237" t="s">
         <v>612</v>
       </c>
@@ -10984,7 +11068,7 @@
         <v>43240</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="79.2">
+    <row r="19" spans="1:10" ht="73.8">
       <c r="A19" s="237" t="s">
         <v>715</v>
       </c>
@@ -11016,7 +11100,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="241" customFormat="1" ht="79.2">
+    <row r="20" spans="1:10" s="241" customFormat="1" ht="61.5">
       <c r="A20" s="269" t="s">
         <v>744</v>
       </c>
@@ -11042,7 +11126,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="241" customFormat="1" ht="79.2">
+    <row r="21" spans="1:10" s="241" customFormat="1" ht="61.5">
       <c r="A21" s="269" t="s">
         <v>744</v>
       </c>
@@ -11068,7 +11152,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="241" customFormat="1" ht="79.2">
+    <row r="22" spans="1:10" s="241" customFormat="1" ht="61.5">
       <c r="A22" s="269" t="s">
         <v>744</v>
       </c>
@@ -11094,7 +11178,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="241" customFormat="1" ht="39.6">
+    <row r="23" spans="1:10" s="241" customFormat="1" ht="36.9">
       <c r="A23" s="300" t="s">
         <v>812</v>
       </c>
@@ -11115,7 +11199,7 @@
         <v>43196</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="241" customFormat="1" ht="52.8">
+    <row r="24" spans="1:10" s="241" customFormat="1" ht="36.9">
       <c r="A24" s="300" t="s">
         <v>844</v>
       </c>
@@ -11158,7 +11242,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -11171,7 +11255,7 @@
       <selection pane="bottomRight" activeCell="G91" sqref="G91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="12.3"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
@@ -11184,7 +11268,7 @@
     <col min="10" max="10" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="26.4">
+    <row r="1" spans="1:10" ht="24.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11209,12 +11293,12 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="393" t="s">
+      <c r="I1" s="394" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="392"/>
-    </row>
-    <row r="2" spans="1:10" ht="26.4">
+      <c r="J1" s="393"/>
+    </row>
+    <row r="2" spans="1:10" ht="24.6">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -11230,7 +11314,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="52.8">
+    <row r="3" spans="1:10" ht="49.2">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -11256,7 +11340,7 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="241" customFormat="1" ht="66">
+    <row r="4" spans="1:10" s="241" customFormat="1" ht="61.5">
       <c r="A4" s="348" t="s">
         <v>973</v>
       </c>
@@ -11284,7 +11368,7 @@
         <v>43313</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="26.4">
+    <row r="5" spans="1:10" ht="24.6">
       <c r="A5" s="13" t="s">
         <v>24</v>
       </c>
@@ -11311,13 +11395,13 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="86.4">
-      <c r="A6" s="396" t="s">
+      <c r="A6" s="397" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="391" t="s">
+      <c r="B6" s="392" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="391" t="s">
+      <c r="C6" s="392" t="s">
         <v>42</v>
       </c>
       <c r="D6" s="9" t="s">
@@ -11339,9 +11423,9 @@
       <c r="J6" s="28"/>
     </row>
     <row r="7" spans="1:10" ht="86.4">
-      <c r="A7" s="392"/>
-      <c r="B7" s="392"/>
-      <c r="C7" s="392"/>
+      <c r="A7" s="393"/>
+      <c r="B7" s="393"/>
+      <c r="C7" s="393"/>
       <c r="D7" s="9" t="s">
         <v>68</v>
       </c>
@@ -11358,7 +11442,7 @@
       </c>
       <c r="J7" s="31"/>
     </row>
-    <row r="8" spans="1:10" s="260" customFormat="1" ht="39.6">
+    <row r="8" spans="1:10" s="260" customFormat="1" ht="36.9">
       <c r="A8" s="251" t="s">
         <v>60</v>
       </c>
@@ -11388,8 +11472,8 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="39.6">
-      <c r="A9" s="396" t="s">
+    <row r="9" spans="1:10" ht="36.9">
+      <c r="A9" s="397" t="s">
         <v>79</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -11418,8 +11502,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="39.6">
-      <c r="A10" s="392"/>
+    <row r="10" spans="1:10" ht="36.9">
+      <c r="A10" s="393"/>
       <c r="B10" s="5" t="s">
         <v>21</v>
       </c>
@@ -11445,8 +11529,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="39.6">
-      <c r="A11" s="395"/>
+    <row r="11" spans="1:10" ht="36.9">
+      <c r="A11" s="396"/>
       <c r="B11" s="37" t="s">
         <v>21</v>
       </c>
@@ -11497,8 +11581,8 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="39.6">
-      <c r="A13" s="397" t="s">
+    <row r="13" spans="1:10" ht="36.9">
+      <c r="A13" s="398" t="s">
         <v>117</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -11526,8 +11610,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="39.6">
-      <c r="A14" s="392"/>
+    <row r="14" spans="1:10" ht="36.9">
+      <c r="A14" s="393"/>
       <c r="B14" s="5" t="s">
         <v>21</v>
       </c>
@@ -11553,8 +11637,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="39.6">
-      <c r="A15" s="392"/>
+    <row r="15" spans="1:10" ht="24.6">
+      <c r="A15" s="393"/>
       <c r="B15" s="5" t="s">
         <v>21</v>
       </c>
@@ -11580,8 +11664,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="39.6">
-      <c r="A16" s="392"/>
+    <row r="16" spans="1:10" ht="36.9">
+      <c r="A16" s="393"/>
       <c r="B16" s="37" t="s">
         <v>21</v>
       </c>
@@ -11608,7 +11692,7 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="207" customFormat="1" ht="105.6">
+    <row r="17" spans="1:10" s="207" customFormat="1" ht="98.4">
       <c r="A17" s="200" t="s">
         <v>145</v>
       </c>
@@ -11640,7 +11724,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="26.4">
+    <row r="18" spans="1:10" ht="24.6">
       <c r="A18" s="4" t="s">
         <v>152</v>
       </c>
@@ -11666,7 +11750,7 @@
       </c>
       <c r="J18" s="31"/>
     </row>
-    <row r="19" spans="1:10" ht="26.4">
+    <row r="19" spans="1:10" ht="24.6">
       <c r="A19" s="4" t="s">
         <v>160</v>
       </c>
@@ -11692,7 +11776,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="105.6">
+    <row r="20" spans="1:10" ht="98.4">
       <c r="A20" s="10" t="s">
         <v>19</v>
       </c>
@@ -11722,7 +11806,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="79.2">
+    <row r="21" spans="1:10" ht="73.8">
       <c r="A21" s="4" t="s">
         <v>170</v>
       </c>
@@ -11752,7 +11836,7 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="52.8">
+    <row r="22" spans="1:10" ht="36.9">
       <c r="A22" s="55" t="s">
         <v>181</v>
       </c>
@@ -11784,7 +11868,7 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="207" customFormat="1" ht="171.6">
+    <row r="23" spans="1:10" s="207" customFormat="1" ht="147.6">
       <c r="A23" s="204" t="s">
         <v>214</v>
       </c>
@@ -11815,7 +11899,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="92.4">
+    <row r="24" spans="1:10" ht="86.1">
       <c r="A24" s="4" t="s">
         <v>249</v>
       </c>
@@ -11845,7 +11929,7 @@
         <v>76138</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="66">
+    <row r="25" spans="1:10" ht="61.5">
       <c r="A25" s="4" t="s">
         <v>259</v>
       </c>
@@ -11871,7 +11955,7 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="207" customFormat="1" ht="92.4">
+    <row r="26" spans="1:10" s="207" customFormat="1" ht="86.1">
       <c r="A26" s="204" t="s">
         <v>278</v>
       </c>
@@ -11947,7 +12031,7 @@
       <c r="I28" s="8"/>
       <c r="J28" s="31"/>
     </row>
-    <row r="29" spans="1:10" ht="79.2">
+    <row r="29" spans="1:10" ht="73.8">
       <c r="A29" s="4" t="s">
         <v>310</v>
       </c>
@@ -11977,7 +12061,7 @@
       </c>
       <c r="J29" s="31"/>
     </row>
-    <row r="30" spans="1:10" ht="92.4">
+    <row r="30" spans="1:10" ht="86.1">
       <c r="A30" s="70" t="s">
         <v>335</v>
       </c>
@@ -12007,7 +12091,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="241" customFormat="1" ht="79.2">
+    <row r="31" spans="1:10" s="241" customFormat="1" ht="73.8">
       <c r="A31" s="300" t="s">
         <v>284</v>
       </c>
@@ -12039,7 +12123,7 @@
         <v>43313</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="241" customFormat="1" ht="52.8">
+    <row r="32" spans="1:10" s="241" customFormat="1" ht="49.2">
       <c r="A32" s="300" t="s">
         <v>284</v>
       </c>
@@ -12103,7 +12187,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="241" customFormat="1" ht="66">
+    <row r="34" spans="1:10" s="241" customFormat="1" ht="61.5">
       <c r="A34" s="237" t="s">
         <v>317</v>
       </c>
@@ -12133,7 +12217,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="241" customFormat="1" ht="66">
+    <row r="35" spans="1:10" s="241" customFormat="1" ht="61.5">
       <c r="A35" s="237" t="s">
         <v>317</v>
       </c>
@@ -12163,7 +12247,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="39.6">
+    <row r="36" spans="1:10" ht="36.9">
       <c r="A36" s="4" t="s">
         <v>344</v>
       </c>
@@ -12191,7 +12275,7 @@
       </c>
       <c r="J36" s="28"/>
     </row>
-    <row r="37" spans="1:10" ht="66">
+    <row r="37" spans="1:10" ht="61.5">
       <c r="A37" s="4" t="s">
         <v>351</v>
       </c>
@@ -12223,8 +12307,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="39.6">
-      <c r="A38" s="394" t="s">
+    <row r="38" spans="1:10" ht="36.9">
+      <c r="A38" s="395" t="s">
         <v>364</v>
       </c>
       <c r="B38" s="73" t="s">
@@ -12253,8 +12337,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="39.6">
-      <c r="A39" s="392"/>
+    <row r="39" spans="1:10" ht="36.9">
+      <c r="A39" s="393"/>
       <c r="B39" s="5" t="s">
         <v>21</v>
       </c>
@@ -12281,8 +12365,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="66">
-      <c r="A40" s="392"/>
+    <row r="40" spans="1:10" ht="61.5">
+      <c r="A40" s="393"/>
       <c r="B40" s="5" t="s">
         <v>21</v>
       </c>
@@ -12309,8 +12393,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="39.6">
-      <c r="A41" s="392"/>
+    <row r="41" spans="1:10" ht="36.9">
+      <c r="A41" s="393"/>
       <c r="B41" s="5" t="s">
         <v>21</v>
       </c>
@@ -12337,8 +12421,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="39.6">
-      <c r="A42" s="392"/>
+    <row r="42" spans="1:10" ht="36.9">
+      <c r="A42" s="393"/>
       <c r="B42" s="5" t="s">
         <v>21</v>
       </c>
@@ -12365,8 +12449,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="39.6">
-      <c r="A43" s="392"/>
+    <row r="43" spans="1:10" ht="36.9">
+      <c r="A43" s="393"/>
       <c r="B43" s="5" t="s">
         <v>21</v>
       </c>
@@ -12393,8 +12477,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="39.6">
-      <c r="A44" s="392"/>
+    <row r="44" spans="1:10" ht="36.9">
+      <c r="A44" s="393"/>
       <c r="B44" s="5" t="s">
         <v>21</v>
       </c>
@@ -12421,8 +12505,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="39.6">
-      <c r="A45" s="392"/>
+    <row r="45" spans="1:10" ht="36.9">
+      <c r="A45" s="393"/>
       <c r="B45" s="5" t="s">
         <v>21</v>
       </c>
@@ -12449,8 +12533,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="39.6">
-      <c r="A46" s="392"/>
+    <row r="46" spans="1:10" ht="36.9">
+      <c r="A46" s="393"/>
       <c r="B46" s="5" t="s">
         <v>21</v>
       </c>
@@ -12477,8 +12561,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="39.6">
-      <c r="A47" s="395"/>
+    <row r="47" spans="1:10" ht="36.9">
+      <c r="A47" s="396"/>
       <c r="B47" s="37" t="s">
         <v>21</v>
       </c>
@@ -12505,7 +12589,7 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="39.6">
+    <row r="48" spans="1:10" ht="36.9">
       <c r="A48" s="88" t="s">
         <v>433</v>
       </c>
@@ -12565,8 +12649,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="66">
-      <c r="A50" s="394" t="s">
+    <row r="50" spans="1:10" ht="61.5">
+      <c r="A50" s="395" t="s">
         <v>469</v>
       </c>
       <c r="B50" s="73" t="s">
@@ -12595,8 +12679,8 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="39.6">
-      <c r="A51" s="395"/>
+    <row r="51" spans="1:10" ht="36.9">
+      <c r="A51" s="396"/>
       <c r="B51" s="37" t="s">
         <v>21</v>
       </c>
@@ -12651,7 +12735,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:10" s="337" customFormat="1" ht="26.4">
+    <row r="53" spans="1:10" s="337" customFormat="1" ht="24.6">
       <c r="A53" s="328" t="s">
         <v>434</v>
       </c>
@@ -12677,7 +12761,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:10" s="304" customFormat="1" ht="39.6">
+    <row r="54" spans="1:10" s="304" customFormat="1" ht="36.9">
       <c r="A54" s="338" t="s">
         <v>434</v>
       </c>
@@ -12702,7 +12786,7 @@
         <v>43196</v>
       </c>
     </row>
-    <row r="55" spans="1:10" s="304" customFormat="1" ht="52.8">
+    <row r="55" spans="1:10" s="304" customFormat="1" ht="49.2">
       <c r="A55" s="339" t="s">
         <v>434</v>
       </c>
@@ -12725,7 +12809,7 @@
         <v>43196</v>
       </c>
     </row>
-    <row r="56" spans="1:10" s="347" customFormat="1" ht="145.19999999999999">
+    <row r="56" spans="1:10" s="347" customFormat="1" ht="123">
       <c r="A56" s="340" t="s">
         <v>443</v>
       </c>
@@ -12752,7 +12836,7 @@
         <v>43196</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="79.2">
+    <row r="57" spans="1:10" ht="73.8">
       <c r="A57" s="4" t="s">
         <v>521</v>
       </c>
@@ -12784,7 +12868,7 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="52.8">
+    <row r="58" spans="1:10" ht="49.2">
       <c r="A58" s="5" t="s">
         <v>521</v>
       </c>
@@ -12816,7 +12900,7 @@
         <v>43283</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="52.8">
+    <row r="59" spans="1:10" ht="49.2">
       <c r="A59" s="5" t="s">
         <v>521</v>
       </c>
@@ -12848,7 +12932,7 @@
         <v>43284</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="52.8">
+    <row r="60" spans="1:10" ht="49.2">
       <c r="A60" s="5" t="s">
         <v>521</v>
       </c>
@@ -12880,7 +12964,7 @@
         <v>43285</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="66">
+    <row r="61" spans="1:10" ht="61.5">
       <c r="A61" s="5" t="s">
         <v>521</v>
       </c>
@@ -12912,7 +12996,7 @@
         <v>43286</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="52.8">
+    <row r="62" spans="1:10" ht="49.2">
       <c r="A62" s="5" t="s">
         <v>521</v>
       </c>
@@ -12944,7 +13028,7 @@
         <v>43287</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="52.8">
+    <row r="63" spans="1:10" ht="49.2">
       <c r="A63" s="5" t="s">
         <v>521</v>
       </c>
@@ -12976,7 +13060,7 @@
         <v>43288</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="52.8">
+    <row r="64" spans="1:10" ht="49.2">
       <c r="A64" s="5" t="s">
         <v>521</v>
       </c>
@@ -13008,7 +13092,7 @@
         <v>43289</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="52.8">
+    <row r="65" spans="1:10" ht="49.2">
       <c r="A65" s="4" t="s">
         <v>562</v>
       </c>
@@ -13038,7 +13122,7 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="26.4">
+    <row r="66" spans="1:10" ht="24.6">
       <c r="A66" s="5" t="s">
         <v>562</v>
       </c>
@@ -13068,7 +13152,7 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="79.2">
+    <row r="67" spans="1:10" ht="73.8">
       <c r="A67" s="4" t="s">
         <v>575</v>
       </c>
@@ -13098,7 +13182,7 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="26.4">
+    <row r="68" spans="1:10" ht="24.6">
       <c r="A68" s="114" t="s">
         <v>582</v>
       </c>
@@ -13128,7 +13212,7 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="52.8">
+    <row r="69" spans="1:10" ht="49.2">
       <c r="A69" s="4" t="s">
         <v>607</v>
       </c>
@@ -13190,7 +13274,7 @@
         <v>43266</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="52.8">
+    <row r="71" spans="1:10" ht="49.2">
       <c r="A71" s="107" t="s">
         <v>622</v>
       </c>
@@ -13217,7 +13301,7 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="66">
+    <row r="72" spans="1:10" ht="61.5">
       <c r="A72" s="105" t="s">
         <v>622</v>
       </c>
@@ -13352,7 +13436,7 @@
         <v>43287</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="39.6">
+    <row r="77" spans="1:10" ht="43.2">
       <c r="A77" s="105" t="s">
         <v>622</v>
       </c>
@@ -13574,7 +13658,7 @@
         <v>43295</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="79.2">
+    <row r="85" spans="1:10" ht="61.5">
       <c r="A85" s="107" t="s">
         <v>537</v>
       </c>
@@ -13602,7 +13686,7 @@
         <v>43296</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="66">
+    <row r="86" spans="1:10" ht="57.6">
       <c r="A86" s="105" t="s">
         <v>537</v>
       </c>
@@ -13630,7 +13714,7 @@
         <v>43297</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="66">
+    <row r="87" spans="1:10" ht="61.5">
       <c r="A87" s="105" t="s">
         <v>537</v>
       </c>
@@ -13712,7 +13796,7 @@
         <v>43300</v>
       </c>
     </row>
-    <row r="90" spans="1:10" s="241" customFormat="1" ht="39.6">
+    <row r="90" spans="1:10" s="241" customFormat="1" ht="36.9">
       <c r="A90" s="300" t="s">
         <v>560</v>
       </c>
@@ -13720,7 +13804,7 @@
         <v>564</v>
       </c>
       <c r="C90" s="237"/>
-      <c r="D90" s="400" t="s">
+      <c r="D90" s="389" t="s">
         <v>565</v>
       </c>
       <c r="E90" s="262" t="s">
@@ -13736,7 +13820,7 @@
       <c r="I90" s="240"/>
       <c r="J90" s="237"/>
     </row>
-    <row r="91" spans="1:10" ht="52.8">
+    <row r="91" spans="1:10" ht="49.2">
       <c r="A91" s="5" t="s">
         <v>722</v>
       </c>
@@ -13766,7 +13850,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="52.8">
+    <row r="92" spans="1:10" ht="49.2">
       <c r="A92" s="4" t="s">
         <v>731</v>
       </c>
@@ -13796,7 +13880,7 @@
         <v>43208</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="118.8">
+    <row r="93" spans="1:10" ht="110.7">
       <c r="A93" s="4" t="s">
         <v>736</v>
       </c>
@@ -13824,8 +13908,8 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="39.6">
-      <c r="A94" s="396" t="s">
+    <row r="94" spans="1:10" ht="36.9">
+      <c r="A94" s="397" t="s">
         <v>748</v>
       </c>
       <c r="B94" s="5" t="s">
@@ -13854,8 +13938,8 @@
         <v>43256</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="39.6">
-      <c r="A95" s="392"/>
+    <row r="95" spans="1:10" ht="36.9">
+      <c r="A95" s="393"/>
       <c r="B95" s="5" t="s">
         <v>45</v>
       </c>
@@ -13882,8 +13966,8 @@
         <v>43256</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="39.6">
-      <c r="A96" s="392"/>
+    <row r="96" spans="1:10" ht="36.9">
+      <c r="A96" s="393"/>
       <c r="B96" s="5" t="s">
         <v>45</v>
       </c>
@@ -13910,8 +13994,8 @@
         <v>43256</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="39.6">
-      <c r="A97" s="392"/>
+    <row r="97" spans="1:10" ht="36.9">
+      <c r="A97" s="393"/>
       <c r="B97" s="5" t="s">
         <v>45</v>
       </c>
@@ -13938,8 +14022,8 @@
         <v>43256</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="39.6">
-      <c r="A98" s="392"/>
+    <row r="98" spans="1:10" ht="24.6">
+      <c r="A98" s="393"/>
       <c r="B98" s="5" t="s">
         <v>45</v>
       </c>
@@ -13966,8 +14050,8 @@
         <v>43256</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="39.6">
-      <c r="A99" s="392"/>
+    <row r="99" spans="1:10" ht="24.6">
+      <c r="A99" s="393"/>
       <c r="B99" s="5" t="s">
         <v>45</v>
       </c>
@@ -13994,8 +14078,8 @@
         <v>43256</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="39.6">
-      <c r="A100" s="392"/>
+    <row r="100" spans="1:10" ht="36.9">
+      <c r="A100" s="393"/>
       <c r="B100" s="5" t="s">
         <v>45</v>
       </c>
@@ -14022,8 +14106,8 @@
         <v>43256</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="39.6">
-      <c r="A101" s="392"/>
+    <row r="101" spans="1:10" ht="36.9">
+      <c r="A101" s="393"/>
       <c r="B101" s="5" t="s">
         <v>45</v>
       </c>
@@ -14050,7 +14134,7 @@
         <v>43256</v>
       </c>
     </row>
-    <row r="102" spans="1:10" s="207" customFormat="1" ht="39.6">
+    <row r="102" spans="1:10" s="207" customFormat="1" ht="36.9">
       <c r="A102" s="204" t="s">
         <v>792</v>
       </c>
@@ -14080,7 +14164,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="26.4">
+    <row r="103" spans="1:10" ht="24.6">
       <c r="A103" s="4" t="s">
         <v>781</v>
       </c>
@@ -14112,7 +14196,7 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="52.8">
+    <row r="104" spans="1:10" ht="49.2">
       <c r="A104" s="4" t="s">
         <v>800</v>
       </c>
@@ -14142,7 +14226,7 @@
         <v>43236</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="39.6">
+    <row r="105" spans="1:10" ht="36.9">
       <c r="A105" s="4" t="s">
         <v>808</v>
       </c>
@@ -14305,7 +14389,7 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="66">
+    <row r="111" spans="1:10" ht="61.5">
       <c r="A111" s="4" t="s">
         <v>858</v>
       </c>
@@ -14335,7 +14419,7 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="66">
+    <row r="112" spans="1:10" ht="61.5">
       <c r="A112" s="4" t="s">
         <v>858</v>
       </c>
@@ -14393,7 +14477,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="29.4" thickBot="1">
+    <row r="114" spans="1:10" ht="29.1" thickBot="1">
       <c r="A114" s="4" t="s">
         <v>866</v>
       </c>
@@ -14700,7 +14784,7 @@
         <v>43293</v>
       </c>
     </row>
-    <row r="125" spans="1:10" ht="118.8">
+    <row r="125" spans="1:10" ht="98.4">
       <c r="A125" s="4" t="s">
         <v>892</v>
       </c>
@@ -14732,7 +14816,7 @@
         <v>43294</v>
       </c>
     </row>
-    <row r="126" spans="1:10" ht="26.4">
+    <row r="126" spans="1:10" ht="24.6">
       <c r="A126" s="4" t="s">
         <v>892</v>
       </c>
@@ -14760,7 +14844,7 @@
         <v>43295</v>
       </c>
     </row>
-    <row r="127" spans="1:10" s="241" customFormat="1" ht="132">
+    <row r="127" spans="1:10" s="241" customFormat="1" ht="123">
       <c r="A127" s="300" t="s">
         <v>833</v>
       </c>
@@ -14790,7 +14874,7 @@
         <v>43313</v>
       </c>
     </row>
-    <row r="128" spans="1:10" s="241" customFormat="1" ht="26.4">
+    <row r="128" spans="1:10" s="241" customFormat="1" ht="24.6">
       <c r="A128" s="300" t="s">
         <v>833</v>
       </c>
@@ -14820,7 +14904,7 @@
         <v>43313</v>
       </c>
     </row>
-    <row r="129" spans="1:10" s="241" customFormat="1" ht="26.4">
+    <row r="129" spans="1:10" s="241" customFormat="1" ht="24.6">
       <c r="A129" s="300" t="s">
         <v>833</v>
       </c>
@@ -14850,7 +14934,7 @@
         <v>43313</v>
       </c>
     </row>
-    <row r="130" spans="1:10" s="241" customFormat="1" ht="39.6">
+    <row r="130" spans="1:10" s="241" customFormat="1" ht="36.9">
       <c r="A130" s="300" t="s">
         <v>833</v>
       </c>
@@ -14878,7 +14962,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="131" spans="1:10" s="241" customFormat="1" ht="52.8">
+    <row r="131" spans="1:10" s="241" customFormat="1" ht="36.9">
       <c r="A131" s="300" t="s">
         <v>854</v>
       </c>
@@ -15052,7 +15136,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -15078,7 +15162,7 @@
     <col min="11" max="16384" width="14.44140625" style="354"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="24">
+    <row r="1" spans="1:10" ht="22.8">
       <c r="A1" s="352" t="s">
         <v>0</v>
       </c>
@@ -15103,12 +15187,12 @@
       <c r="H1" s="352" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="398" t="s">
+      <c r="I1" s="399" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="399"/>
-    </row>
-    <row r="2" spans="1:10" ht="24">
+      <c r="J1" s="400"/>
+    </row>
+    <row r="2" spans="1:10" ht="22.8">
       <c r="A2" s="352"/>
       <c r="B2" s="353"/>
       <c r="C2" s="353"/>
@@ -15124,7 +15208,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="356" customFormat="1" ht="48">
+    <row r="3" spans="1:10" s="356" customFormat="1" ht="46.8">
       <c r="A3" s="356" t="s">
         <v>973</v>
       </c>

</xml_diff>